<commit_message>
add a bit change to the MT config
</commit_message>
<xml_diff>
--- a/invoice_gen/result.xlsx
+++ b/invoice_gen/result.xlsx
@@ -3,16 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Invoice" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Packing list" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Contract'!$A$1:$G$29</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Invoice'!$A$1:$G$31</definedName>
@@ -30,7 +27,7 @@
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="167" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="51">
+  <fonts count="47">
     <font>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -299,30 +296,6 @@
     </font>
     <font>
       <name val="Times New Roman"/>
-      <family val="1"/>
-      <sz val="16"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="14"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <b val="1"/>
-      <sz val="14"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <b val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="14"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
       <b val="1"/>
       <sz val="12"/>
     </font>
@@ -493,7 +466,7 @@
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -689,19 +662,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="43" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="46" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -720,6 +680,18 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -738,26 +710,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="43" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="25" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -778,10 +750,10 @@
     <xf numFmtId="165" fontId="26" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="49" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="165" fontId="45" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="23" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -790,22 +762,22 @@
     <xf numFmtId="165" fontId="37" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="50" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="46" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="50" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="167" fontId="46" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="167" fontId="49" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="28" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -826,67 +798,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="46" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="48" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="44" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="48" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="167" fontId="44" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="47" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="167" fontId="43" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="48" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="44" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="48" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="44" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="48" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="44" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="47" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="43" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="47" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="43" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="47" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="43" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="47" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="43" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="47" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="43" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="47" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="43" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1162,29 +1134,6 @@
 </wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
-    <sheetNames>
-      <sheetName val="Contract"/>
-      <sheetName val="Invoice"/>
-      <sheetName val="Packing list"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="7">
-          <cell r="I7" t="str">
-            <v>CLF2025-186</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1449,8 +1398,8 @@
   </sheetPr>
   <dimension ref="A1:XFD200"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A6" zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="28.7109375" defaultRowHeight="15"/>
@@ -1463,8 +1412,8 @@
     <col width="28.7109375" customWidth="1" style="54" min="16384" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="46.15" customFormat="1" customHeight="1" s="96">
-      <c r="A1" s="81" t="inlineStr">
+    <row r="1" ht="46.15" customFormat="1" customHeight="1" s="95">
+      <c r="A1" s="76" t="inlineStr">
         <is>
           <t>SALES CONTRACT</t>
         </is>
@@ -1490,13 +1439,13 @@
       <c r="C3" s="56" t="n"/>
       <c r="D3" s="56" t="n"/>
       <c r="E3" s="56" t="n"/>
-      <c r="F3" s="82" t="inlineStr">
+      <c r="F3" s="77" t="inlineStr">
         <is>
           <t>DATE:</t>
         </is>
       </c>
-      <c r="G3" s="97" t="n">
-        <v>45831</v>
+      <c r="G3" s="96" t="n">
+        <v>45906</v>
       </c>
     </row>
     <row r="4" ht="39" customFormat="1" customHeight="1" s="43">
@@ -1504,19 +1453,19 @@
       <c r="B4" s="56" t="n"/>
       <c r="C4" s="56" t="n"/>
       <c r="D4" s="56" t="n"/>
-      <c r="E4" s="82" t="inlineStr">
+      <c r="E4" s="77" t="inlineStr">
         <is>
           <t>CONTRACT NO.:</t>
         </is>
       </c>
-      <c r="G4" s="74" t="inlineStr">
-        <is>
-          <t>MT2-25003E</t>
+      <c r="G4" s="94" t="inlineStr">
+        <is>
+          <t>JFNO</t>
         </is>
       </c>
     </row>
     <row r="5" ht="31.9" customFormat="1" customHeight="1" s="44">
-      <c r="A5" s="86" t="inlineStr">
+      <c r="A5" s="85" t="inlineStr">
         <is>
           <t>The Seller:</t>
         </is>
@@ -1559,7 +1508,7 @@
       <c r="G8" s="59" t="n"/>
     </row>
     <row r="9" ht="31.9" customFormat="1" customHeight="1" s="44">
-      <c r="A9" s="86" t="inlineStr">
+      <c r="A9" s="85" t="inlineStr">
         <is>
           <t xml:space="preserve">The Buyer:  </t>
         </is>
@@ -1572,14 +1521,14 @@
     </row>
     <row r="10" ht="33" customFormat="1" customHeight="1" s="44">
       <c r="A10" s="58" t="n"/>
-      <c r="B10" s="83" t="inlineStr">
+      <c r="B10" s="78" t="inlineStr">
         <is>
           <t>Factory C-1B-B1-B and C-1B-B2, Lot C-1B-CN, DE4 Street, My Phuoc 3 Industrial Park, Thoi Hoa Ward, Ben Cat City, Binh Duong Province, Vietnam</t>
         </is>
       </c>
     </row>
     <row r="11" ht="30" customFormat="1" customHeight="1" s="44">
-      <c r="B11" s="86" t="inlineStr">
+      <c r="B11" s="85" t="inlineStr">
         <is>
           <t>Contact Person : ZHENGYANYUN  Tel:  0274 3803833</t>
         </is>
@@ -1590,438 +1539,468 @@
       <c r="F11" s="58" t="n"/>
       <c r="G11" s="58" t="n"/>
     </row>
-    <row r="12" ht="24" customFormat="1" customHeight="1" s="98">
-      <c r="A12" s="99" t="inlineStr">
+    <row r="12" ht="24" customFormat="1" customHeight="1" s="97">
+      <c r="A12" s="98" t="inlineStr">
         <is>
           <t>After discussion, the both parties agree to sell and purchase the commodities on the following terms and conditions:</t>
         </is>
       </c>
-      <c r="B12" s="99" t="n"/>
-      <c r="E12" s="100" t="n"/>
-      <c r="F12" s="100" t="n"/>
-      <c r="G12" s="100" t="n"/>
-      <c r="H12" s="100" t="n"/>
-      <c r="K12" s="100" t="n"/>
-      <c r="L12" s="100" t="n"/>
-      <c r="M12" s="101" t="n"/>
-      <c r="N12" s="101" t="n"/>
-    </row>
-    <row r="13" ht="26.1" customFormat="1" customHeight="1" s="98">
-      <c r="A13" s="102" t="inlineStr">
+      <c r="B12" s="98" t="n"/>
+      <c r="E12" s="99" t="n"/>
+      <c r="F12" s="99" t="n"/>
+      <c r="G12" s="99" t="n"/>
+      <c r="H12" s="99" t="n"/>
+      <c r="K12" s="99" t="n"/>
+      <c r="L12" s="99" t="n"/>
+      <c r="M12" s="100" t="n"/>
+      <c r="N12" s="100" t="n"/>
+    </row>
+    <row r="13" ht="26.1" customFormat="1" customHeight="1" s="97">
+      <c r="A13" s="101" t="inlineStr">
         <is>
           <t>1.NAME OF COMMODITY AND SPECIFICATION:</t>
         </is>
       </c>
-      <c r="B13" s="102" t="n"/>
-      <c r="E13" s="100" t="n"/>
-      <c r="F13" s="100" t="n"/>
-      <c r="G13" s="100" t="n"/>
-      <c r="H13" s="100" t="n"/>
-      <c r="I13" s="100" t="n"/>
-      <c r="J13" s="100" t="n"/>
-      <c r="K13" s="100" t="n"/>
-      <c r="L13" s="100" t="n"/>
-      <c r="M13" s="101" t="n"/>
-      <c r="N13" s="101" t="n"/>
-    </row>
-    <row r="14" ht="24.95" customFormat="1" customHeight="1" s="98">
-      <c r="A14" s="99" t="inlineStr">
+      <c r="B13" s="101" t="n"/>
+      <c r="E13" s="99" t="n"/>
+      <c r="F13" s="99" t="n"/>
+      <c r="G13" s="99" t="n"/>
+      <c r="H13" s="99" t="n"/>
+      <c r="I13" s="99" t="n"/>
+      <c r="J13" s="99" t="n"/>
+      <c r="K13" s="99" t="n"/>
+      <c r="L13" s="99" t="n"/>
+      <c r="M13" s="100" t="n"/>
+      <c r="N13" s="100" t="n"/>
+    </row>
+    <row r="14" ht="24.95" customFormat="1" customHeight="1" s="97">
+      <c r="A14" s="98" t="inlineStr">
         <is>
           <t>The seller guaranteed the correct color delivery, Commodity, Dimension and quantity as follow:</t>
         </is>
       </c>
-      <c r="B14" s="99" t="n"/>
-      <c r="E14" s="100" t="n"/>
-      <c r="F14" s="100" t="n"/>
-      <c r="G14" s="100" t="n"/>
-      <c r="H14" s="100" t="n"/>
-      <c r="I14" s="100" t="n"/>
-      <c r="J14" s="100" t="n"/>
-      <c r="K14" s="100" t="n"/>
-      <c r="L14" s="100" t="n"/>
-      <c r="M14" s="101" t="n"/>
-      <c r="N14" s="101" t="n"/>
-    </row>
-    <row r="15" ht="36" customFormat="1" customHeight="1" s="103">
-      <c r="A15" s="104" t="inlineStr">
+      <c r="B14" s="98" t="n"/>
+      <c r="E14" s="99" t="n"/>
+      <c r="F14" s="99" t="n"/>
+      <c r="G14" s="99" t="n"/>
+      <c r="H14" s="99" t="n"/>
+      <c r="I14" s="99" t="n"/>
+      <c r="J14" s="99" t="n"/>
+      <c r="K14" s="99" t="n"/>
+      <c r="L14" s="99" t="n"/>
+      <c r="M14" s="100" t="n"/>
+      <c r="N14" s="100" t="n"/>
+    </row>
+    <row r="15" ht="36" customFormat="1" customHeight="1" s="102">
+      <c r="A15" s="103" t="inlineStr">
         <is>
           <t>No.</t>
         </is>
       </c>
-      <c r="B15" s="104" t="inlineStr">
+      <c r="B15" s="103" t="inlineStr">
         <is>
           <t>P.O. Nº</t>
         </is>
       </c>
-      <c r="C15" s="105" t="inlineStr">
+      <c r="C15" s="104" t="inlineStr">
         <is>
           <t>Name of
 Cormodity</t>
         </is>
       </c>
-      <c r="D15" s="105" t="inlineStr">
+      <c r="D15" s="104" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="E15" s="104" t="inlineStr">
+      <c r="E15" s="103" t="inlineStr">
         <is>
           <t>Quantity
 (SF)</t>
         </is>
       </c>
-      <c r="F15" s="104" t="inlineStr">
+      <c r="F15" s="103" t="inlineStr">
         <is>
           <t>Unit Price
 (USD)</t>
         </is>
       </c>
-      <c r="G15" s="104" t="inlineStr">
+      <c r="G15" s="103" t="inlineStr">
         <is>
           <t>Total value
 (USD)</t>
         </is>
       </c>
-      <c r="H15" s="106" t="n"/>
-      <c r="I15" s="106" t="n"/>
-      <c r="J15" s="106" t="n"/>
-      <c r="K15" s="106" t="n"/>
-      <c r="L15" s="106" t="n"/>
-      <c r="M15" s="107" t="n"/>
-      <c r="N15" s="107" t="n"/>
+      <c r="H15" s="105" t="n"/>
+      <c r="I15" s="105" t="n"/>
+      <c r="J15" s="105" t="n"/>
+      <c r="K15" s="105" t="n"/>
+      <c r="L15" s="105" t="n"/>
+      <c r="M15" s="106" t="n"/>
+      <c r="N15" s="106" t="n"/>
     </row>
     <row r="16" ht="30" customFormat="1" customHeight="1" s="48">
-      <c r="A16" s="108" t="n">
+      <c r="A16" s="107" t="n">
         <v>1</v>
       </c>
-      <c r="B16" s="108" t="inlineStr">
+      <c r="B16" s="107" t="inlineStr">
         <is>
           <t>YNGY25022</t>
         </is>
       </c>
-      <c r="C16" s="108" t="inlineStr">
+      <c r="C16" s="107" t="inlineStr">
         <is>
           <t>M1243</t>
         </is>
       </c>
-      <c r="D16" s="109" t="inlineStr">
+      <c r="D16" s="108" t="inlineStr">
         <is>
           <t>LEATHER</t>
         </is>
       </c>
-      <c r="E16" s="110" t="n">
+      <c r="E16" s="109" t="n">
         <v>10045.4</v>
       </c>
-      <c r="F16" s="110">
-        <f>G16/E16</f>
+      <c r="F16" s="109" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="G16" s="109">
+        <f>F16*E16</f>
         <v/>
       </c>
-      <c r="G16" s="110" t="n">
-        <v>11451.756</v>
-      </c>
     </row>
     <row r="17" ht="30" customFormat="1" customHeight="1" s="48">
-      <c r="A17" s="108" t="n">
+      <c r="A17" s="107" t="n">
         <v>2</v>
       </c>
-      <c r="B17" s="108" t="inlineStr">
+      <c r="B17" s="107" t="inlineStr">
         <is>
           <t>YNGY25028</t>
         </is>
       </c>
-      <c r="C17" s="108" t="inlineStr">
+      <c r="C17" s="107" t="inlineStr">
         <is>
           <t>M1243</t>
         </is>
       </c>
-      <c r="D17" s="111" t="n"/>
-      <c r="E17" s="110" t="n">
-        <v>40549.3</v>
-      </c>
-      <c r="F17" s="110">
-        <f>G17/E17</f>
+      <c r="D17" s="110" t="n"/>
+      <c r="E17" s="109" t="n">
+        <v>40074.3</v>
+      </c>
+      <c r="F17" s="109" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="G17" s="109">
+        <f>F17*E17</f>
         <v/>
       </c>
-      <c r="G17" s="110" t="n">
-        <v>46116.952</v>
-      </c>
     </row>
     <row r="18" ht="30" customFormat="1" customHeight="1" s="48">
-      <c r="A18" s="108" t="n">
+      <c r="A18" s="107" t="n">
         <v>3</v>
       </c>
-      <c r="B18" s="108" t="inlineStr">
+      <c r="B18" s="107" t="inlineStr">
+        <is>
+          <t>YNGY25028</t>
+        </is>
+      </c>
+      <c r="C18" s="107" t="inlineStr">
+        <is>
+          <t>M1243</t>
+        </is>
+      </c>
+      <c r="D18" s="110" t="n"/>
+      <c r="E18" s="109" t="n">
+        <v>475</v>
+      </c>
+      <c r="F18" s="109" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="G18" s="109">
+        <f>F18*E18</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" ht="30" customFormat="1" customHeight="1" s="48">
+      <c r="A19" s="107" t="n">
+        <v>4</v>
+      </c>
+      <c r="B19" s="107" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="C18" s="108" t="inlineStr">
+      <c r="C19" s="107" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="D18" s="111" t="n"/>
-      <c r="E18" s="110" t="n">
-        <v>136491.8</v>
-      </c>
-      <c r="F18" s="110">
-        <f>G18/E18</f>
+      <c r="D19" s="110" t="n"/>
+      <c r="E19" s="109" t="n">
+        <v>136378.1</v>
+      </c>
+      <c r="F19" s="109" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="G19" s="109">
+        <f>F19*E19</f>
         <v/>
       </c>
-      <c r="G18" s="110" t="n">
-        <v>156939.419</v>
-      </c>
-    </row>
-    <row r="19" ht="30" customFormat="1" customHeight="1" s="48">
-      <c r="A19" s="108" t="n">
-        <v>4</v>
-      </c>
-      <c r="B19" s="108" t="inlineStr">
+    </row>
+    <row r="20" ht="30" customFormat="1" customHeight="1" s="48">
+      <c r="A20" s="107" t="n">
+        <v>5</v>
+      </c>
+      <c r="B20" s="107" t="inlineStr">
+        <is>
+          <t>GYOJY_M25371</t>
+        </is>
+      </c>
+      <c r="C20" s="107" t="inlineStr">
+        <is>
+          <t>Nick Dove</t>
+        </is>
+      </c>
+      <c r="D20" s="110" t="n"/>
+      <c r="E20" s="109" t="n">
+        <v>113.7</v>
+      </c>
+      <c r="F20" s="109" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="G20" s="109">
+        <f>F20*E20</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" ht="30" customFormat="1" customHeight="1" s="48">
+      <c r="A21" s="107" t="n">
+        <v>6</v>
+      </c>
+      <c r="B21" s="107" t="inlineStr">
         <is>
           <t>GYOJY_M25374</t>
         </is>
       </c>
-      <c r="C19" s="108" t="inlineStr">
+      <c r="C21" s="107" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="D19" s="112" t="n"/>
-      <c r="E19" s="110" t="n">
-        <v>38841.3</v>
-      </c>
-      <c r="F19" s="110">
-        <f>G19/E19</f>
+      <c r="D21" s="110" t="n"/>
+      <c r="E21" s="109" t="n">
+        <v>38430</v>
+      </c>
+      <c r="F21" s="109" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="G21" s="109">
+        <f>F21*E21</f>
         <v/>
       </c>
-      <c r="G19" s="110" t="n">
-        <v>44572.89599999999</v>
-      </c>
-    </row>
-    <row r="20" ht="36" customFormat="1" customHeight="1" s="48">
-      <c r="A20" s="113" t="inlineStr">
+    </row>
+    <row r="22" ht="30" customFormat="1" customHeight="1" s="48">
+      <c r="A22" s="107" t="n">
+        <v>7</v>
+      </c>
+      <c r="B22" s="107" t="inlineStr">
+        <is>
+          <t>GYOJY_M25374</t>
+        </is>
+      </c>
+      <c r="C22" s="107" t="inlineStr">
+        <is>
+          <t>Nick Dove</t>
+        </is>
+      </c>
+      <c r="D22" s="111" t="n"/>
+      <c r="E22" s="109" t="n">
+        <v>411.3</v>
+      </c>
+      <c r="F22" s="109" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="G22" s="109">
+        <f>F22*E22</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" ht="36" customFormat="1" customHeight="1" s="48">
+      <c r="A23" s="112" t="inlineStr">
         <is>
           <t>TOTAL:</t>
         </is>
       </c>
-      <c r="B20" s="114" t="n"/>
-      <c r="C20" s="113" t="n"/>
-      <c r="D20" s="113" t="n"/>
-      <c r="E20" s="115">
-        <f>SUM(E16:E19)</f>
+      <c r="B23" s="113" t="n"/>
+      <c r="C23" s="112" t="n"/>
+      <c r="D23" s="112" t="n"/>
+      <c r="E23" s="114">
+        <f>SUM(E16:E22)</f>
         <v/>
       </c>
-      <c r="F20" s="113" t="n"/>
-      <c r="G20" s="115">
-        <f>SUM(G16:G19)</f>
+      <c r="F23" s="112" t="n"/>
+      <c r="G23" s="114">
+        <f>SUM(G16:G22)</f>
         <v/>
       </c>
     </row>
-    <row r="21" ht="44.1" customFormat="1" customHeight="1" s="48">
-      <c r="A21" s="65" t="inlineStr">
+    <row r="24" ht="28.9" customFormat="1" customHeight="1" s="48">
+      <c r="A24" s="65" t="inlineStr">
         <is>
           <t>DAP:</t>
         </is>
       </c>
-      <c r="B21" s="66" t="inlineStr">
+      <c r="B24" s="66" t="inlineStr">
         <is>
           <t>BINH DUONG</t>
         </is>
       </c>
-      <c r="D21" s="66" t="n"/>
-      <c r="E21" s="67" t="n"/>
-      <c r="F21" s="67" t="n"/>
-      <c r="G21" s="67" t="n"/>
-    </row>
-    <row r="22" ht="28.9" customFormat="1" customHeight="1" s="48">
-      <c r="A22" s="67" t="inlineStr">
-        <is>
-          <t>Term of Payment: 100% TT after shipment</t>
-        </is>
-      </c>
-      <c r="B22" s="67" t="n"/>
-      <c r="C22" s="67" t="n"/>
-      <c r="D22" s="67" t="n"/>
-      <c r="E22" s="67" t="n"/>
-      <c r="F22" s="67" t="n"/>
-      <c r="G22" s="67" t="n"/>
-    </row>
-    <row r="23" ht="28.9" customFormat="1" customHeight="1" s="48">
-      <c r="A23" s="67" t="inlineStr">
-        <is>
-          <t>Transaction method: DAP(USD)</t>
-        </is>
-      </c>
-      <c r="B23" s="67" t="n"/>
-      <c r="C23" s="67" t="n"/>
-      <c r="D23" s="67" t="n"/>
-      <c r="E23" s="67" t="n"/>
-      <c r="F23" s="67" t="n"/>
-      <c r="G23" s="67" t="n"/>
-    </row>
-    <row r="24" ht="28.9" customFormat="1" customHeight="1" s="48">
-      <c r="A24" s="67" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Beneficiary bank information: </t>
-        </is>
-      </c>
-      <c r="B24" s="67" t="n"/>
-      <c r="C24" s="67" t="n"/>
-      <c r="D24" s="67" t="n"/>
-      <c r="E24" s="67" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
-        </is>
-      </c>
+      <c r="D24" s="66" t="n"/>
+      <c r="E24" s="67" t="n"/>
       <c r="F24" s="67" t="n"/>
       <c r="G24" s="67" t="n"/>
     </row>
-    <row r="25" ht="62.1" customFormat="1" customHeight="1" s="43">
+    <row r="25" ht="28.9" customFormat="1" customHeight="1" s="43">
       <c r="A25" s="67" t="inlineStr">
         <is>
-          <t xml:space="preserve">Beneficiary Bank' s Name: </t>
+          <t>Term of Payment: 100% TT after shipment</t>
         </is>
       </c>
       <c r="B25" s="67" t="n"/>
       <c r="C25" s="67" t="n"/>
       <c r="D25" s="67" t="n"/>
-      <c r="E25" s="78" t="inlineStr">
-        <is>
-          <t>BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH /BANK OF CHINA PHNOM PENH BRANCH</t>
-        </is>
-      </c>
-    </row>
-    <row r="26" ht="44.1" customFormat="1" customHeight="1" s="43">
+      <c r="E25" s="67" t="n"/>
+      <c r="F25" s="67" t="n"/>
+      <c r="G25" s="67" t="n"/>
+    </row>
+    <row r="26" ht="57" customFormat="1" customHeight="1" s="43">
       <c r="A26" s="67" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bank Address:  </t>
+          <t>Transaction method: DAP(USD)</t>
         </is>
       </c>
       <c r="B26" s="67" t="n"/>
       <c r="C26" s="67" t="n"/>
       <c r="D26" s="67" t="n"/>
-      <c r="E26" s="78" t="inlineStr">
-        <is>
-          <t>1st AND 2nd FLOOR,CANADIA TOWER,No.315 ANDDUONG ST.,PHNOM PEMH,CAMBODIA.</t>
-        </is>
-      </c>
-    </row>
-    <row r="27" ht="28.9" customFormat="1" customHeight="1" s="116">
+      <c r="E26" s="67" t="n"/>
+      <c r="F26" s="67" t="n"/>
+      <c r="G26" s="67" t="n"/>
+    </row>
+    <row r="27" ht="39" customFormat="1" customHeight="1" s="115">
       <c r="A27" s="67" t="inlineStr">
         <is>
-          <t>Bank account :</t>
+          <t xml:space="preserve">Beneficiary bank information: </t>
         </is>
       </c>
       <c r="B27" s="67" t="n"/>
       <c r="C27" s="67" t="n"/>
       <c r="D27" s="67" t="n"/>
-      <c r="E27" s="79" t="inlineStr">
-        <is>
-          <t>100001100764430</t>
-        </is>
-      </c>
-    </row>
-    <row r="28" ht="39" customFormat="1" customHeight="1" s="116">
+      <c r="E27" s="67" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
+        </is>
+      </c>
+      <c r="F27" s="67" t="n"/>
+      <c r="G27" s="67" t="n"/>
+    </row>
+    <row r="28" ht="62.1" customFormat="1" customHeight="1" s="115">
       <c r="A28" s="67" t="inlineStr">
         <is>
-          <t>SWIFT CODE  ：</t>
+          <t xml:space="preserve">Beneficiary Bank' s Name: </t>
         </is>
       </c>
       <c r="B28" s="67" t="n"/>
       <c r="C28" s="67" t="n"/>
       <c r="D28" s="67" t="n"/>
-      <c r="E28" s="67" t="inlineStr">
-        <is>
-          <t>BKCHKHPPXXX</t>
-        </is>
-      </c>
-      <c r="F28" s="67" t="n"/>
-      <c r="G28" s="67" t="n"/>
-    </row>
-    <row r="29" ht="39" customFormat="1" customHeight="1" s="116">
-      <c r="A29" s="67" t="n"/>
+      <c r="E28" s="73" t="inlineStr">
+        <is>
+          <t>BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH /BANK OF CHINA PHNOM PENH BRANCH</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" ht="44.1" customFormat="1" customHeight="1" s="115">
+      <c r="A29" s="67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bank Address:  </t>
+        </is>
+      </c>
       <c r="B29" s="67" t="n"/>
       <c r="C29" s="67" t="n"/>
       <c r="D29" s="67" t="n"/>
-      <c r="E29" s="67" t="n"/>
-      <c r="F29" s="67" t="n"/>
-      <c r="G29" s="67" t="n"/>
-      <c r="H29" s="67" t="n"/>
-    </row>
-    <row r="30" ht="39" customFormat="1" customHeight="1" s="116">
-      <c r="B30" s="68" t="inlineStr">
+      <c r="E29" s="73" t="inlineStr">
+        <is>
+          <t>1st AND 2nd FLOOR,CANADIA TOWER,No.315 ANDDUONG ST.,PHNOM PEMH,CAMBODIA.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" ht="28.9" customFormat="1" customHeight="1" s="115">
+      <c r="A30" s="67" t="inlineStr">
+        <is>
+          <t>Bank account :</t>
+        </is>
+      </c>
+      <c r="B30" s="67" t="n"/>
+      <c r="C30" s="67" t="n"/>
+      <c r="D30" s="67" t="n"/>
+      <c r="E30" s="74" t="inlineStr">
+        <is>
+          <t>100001100764430</t>
+        </is>
+      </c>
+    </row>
+    <row r="31" ht="39" customFormat="1" customHeight="1" s="115">
+      <c r="A31" s="67" t="inlineStr">
+        <is>
+          <t>SWIFT CODE  ：</t>
+        </is>
+      </c>
+      <c r="B31" s="67" t="n"/>
+      <c r="C31" s="67" t="n"/>
+      <c r="D31" s="67" t="n"/>
+      <c r="E31" s="67" t="inlineStr">
+        <is>
+          <t>BKCHKHPPXXX</t>
+        </is>
+      </c>
+      <c r="F31" s="67" t="n"/>
+      <c r="G31" s="67" t="n"/>
+    </row>
+    <row r="32" ht="39" customFormat="1" customHeight="1" s="116">
+      <c r="A32" s="67" t="n"/>
+      <c r="B32" s="67" t="n"/>
+      <c r="C32" s="67" t="n"/>
+      <c r="D32" s="67" t="n"/>
+      <c r="E32" s="67" t="n"/>
+      <c r="F32" s="67" t="n"/>
+      <c r="G32" s="67" t="n"/>
+      <c r="H32" s="67" t="n"/>
+    </row>
+    <row r="33" ht="39" customFormat="1" customHeight="1" s="116">
+      <c r="B33" s="68" t="inlineStr">
         <is>
           <t>The Buyer:</t>
         </is>
       </c>
-      <c r="F30" s="68" t="inlineStr">
+      <c r="F33" s="68" t="inlineStr">
         <is>
           <t>The Seller:</t>
         </is>
       </c>
     </row>
-    <row r="31" ht="57" customFormat="1" customHeight="1" s="116">
-      <c r="A31" s="80" t="inlineStr">
+    <row r="34" ht="57" customFormat="1" customHeight="1" s="116">
+      <c r="A34" s="75" t="inlineStr">
         <is>
           <t>MOTO INNOVATION VIETNAM LIMITED COMPANY</t>
         </is>
       </c>
-      <c r="D31" s="80" t="n"/>
-      <c r="E31" s="80" t="inlineStr">
+      <c r="D34" s="75" t="n"/>
+      <c r="E34" s="75" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
         </is>
       </c>
     </row>
-    <row r="32" ht="39" customFormat="1" customHeight="1" s="117">
-      <c r="A32" s="54" t="n"/>
-      <c r="B32" s="54" t="n"/>
-      <c r="C32" s="54" t="n"/>
-      <c r="D32" s="54" t="n"/>
-      <c r="E32" s="54" t="n"/>
-      <c r="F32" s="54" t="n"/>
-      <c r="G32" s="54" t="n"/>
-      <c r="H32" s="54" t="n"/>
-      <c r="I32" s="54" t="n"/>
-      <c r="J32" s="54" t="n"/>
-      <c r="K32" s="54" t="n"/>
-      <c r="L32" s="54" t="n"/>
-      <c r="M32" s="54" t="n"/>
-      <c r="XFD32" s="54" t="n"/>
-    </row>
-    <row r="33" ht="39" customFormat="1" customHeight="1" s="117">
-      <c r="A33" s="54" t="n"/>
-      <c r="B33" s="54" t="n"/>
-      <c r="C33" s="54" t="n"/>
-      <c r="D33" s="54" t="n"/>
-      <c r="E33" s="54" t="n"/>
-      <c r="F33" s="54" t="n"/>
-      <c r="G33" s="54" t="n"/>
-      <c r="H33" s="54" t="n"/>
-      <c r="I33" s="54" t="n"/>
-      <c r="J33" s="54" t="n"/>
-      <c r="K33" s="54" t="n"/>
-      <c r="L33" s="54" t="n"/>
-      <c r="M33" s="54" t="n"/>
-      <c r="XFD33" s="54" t="n"/>
-    </row>
-    <row r="34" ht="39" customFormat="1" customHeight="1" s="117">
-      <c r="A34" s="54" t="n"/>
-      <c r="B34" s="54" t="n"/>
-      <c r="C34" s="54" t="n"/>
-      <c r="D34" s="54" t="n"/>
-      <c r="E34" s="54" t="n"/>
-      <c r="F34" s="54" t="n"/>
-      <c r="G34" s="54" t="n"/>
-      <c r="H34" s="54" t="n"/>
-      <c r="I34" s="54" t="n"/>
-      <c r="J34" s="54" t="n"/>
-      <c r="K34" s="54" t="n"/>
-      <c r="L34" s="54" t="n"/>
-      <c r="M34" s="54" t="n"/>
-      <c r="XFD34" s="54" t="n"/>
-    </row>
-    <row r="35" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="35" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A35" s="54" t="n"/>
       <c r="B35" s="54" t="n"/>
       <c r="C35" s="54" t="n"/>
@@ -2037,7 +2016,7 @@
       <c r="M35" s="54" t="n"/>
       <c r="XFD35" s="54" t="n"/>
     </row>
-    <row r="36" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="36" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A36" s="54" t="n"/>
       <c r="B36" s="54" t="n"/>
       <c r="C36" s="54" t="n"/>
@@ -2053,7 +2032,7 @@
       <c r="M36" s="54" t="n"/>
       <c r="XFD36" s="54" t="n"/>
     </row>
-    <row r="37" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="37" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A37" s="54" t="n"/>
       <c r="B37" s="54" t="n"/>
       <c r="C37" s="54" t="n"/>
@@ -2069,7 +2048,7 @@
       <c r="M37" s="54" t="n"/>
       <c r="XFD37" s="54" t="n"/>
     </row>
-    <row r="38" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="38" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A38" s="54" t="n"/>
       <c r="B38" s="54" t="n"/>
       <c r="C38" s="54" t="n"/>
@@ -2085,7 +2064,7 @@
       <c r="M38" s="54" t="n"/>
       <c r="XFD38" s="54" t="n"/>
     </row>
-    <row r="39" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="39" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A39" s="54" t="n"/>
       <c r="B39" s="54" t="n"/>
       <c r="C39" s="54" t="n"/>
@@ -2101,7 +2080,7 @@
       <c r="M39" s="54" t="n"/>
       <c r="XFD39" s="54" t="n"/>
     </row>
-    <row r="40" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="40" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A40" s="54" t="n"/>
       <c r="B40" s="54" t="n"/>
       <c r="C40" s="54" t="n"/>
@@ -2117,7 +2096,7 @@
       <c r="M40" s="54" t="n"/>
       <c r="XFD40" s="54" t="n"/>
     </row>
-    <row r="41" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="41" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A41" s="54" t="n"/>
       <c r="B41" s="54" t="n"/>
       <c r="C41" s="54" t="n"/>
@@ -2133,7 +2112,7 @@
       <c r="M41" s="54" t="n"/>
       <c r="XFD41" s="54" t="n"/>
     </row>
-    <row r="42" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="42" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A42" s="54" t="n"/>
       <c r="B42" s="54" t="n"/>
       <c r="C42" s="54" t="n"/>
@@ -2149,7 +2128,7 @@
       <c r="M42" s="54" t="n"/>
       <c r="XFD42" s="54" t="n"/>
     </row>
-    <row r="43" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="43" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A43" s="54" t="n"/>
       <c r="B43" s="54" t="n"/>
       <c r="C43" s="54" t="n"/>
@@ -2165,7 +2144,7 @@
       <c r="M43" s="54" t="n"/>
       <c r="XFD43" s="54" t="n"/>
     </row>
-    <row r="44" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="44" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A44" s="54" t="n"/>
       <c r="B44" s="54" t="n"/>
       <c r="C44" s="54" t="n"/>
@@ -2181,7 +2160,7 @@
       <c r="M44" s="54" t="n"/>
       <c r="XFD44" s="54" t="n"/>
     </row>
-    <row r="45" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="45" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A45" s="54" t="n"/>
       <c r="B45" s="54" t="n"/>
       <c r="C45" s="54" t="n"/>
@@ -2197,7 +2176,7 @@
       <c r="M45" s="54" t="n"/>
       <c r="XFD45" s="54" t="n"/>
     </row>
-    <row r="46" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="46" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A46" s="54" t="n"/>
       <c r="B46" s="54" t="n"/>
       <c r="C46" s="54" t="n"/>
@@ -2213,7 +2192,7 @@
       <c r="M46" s="54" t="n"/>
       <c r="XFD46" s="54" t="n"/>
     </row>
-    <row r="47" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="47" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A47" s="54" t="n"/>
       <c r="B47" s="54" t="n"/>
       <c r="C47" s="54" t="n"/>
@@ -2229,7 +2208,7 @@
       <c r="M47" s="54" t="n"/>
       <c r="XFD47" s="54" t="n"/>
     </row>
-    <row r="48" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="48" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A48" s="54" t="n"/>
       <c r="B48" s="54" t="n"/>
       <c r="C48" s="54" t="n"/>
@@ -2245,7 +2224,7 @@
       <c r="M48" s="54" t="n"/>
       <c r="XFD48" s="54" t="n"/>
     </row>
-    <row r="49" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="49" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A49" s="54" t="n"/>
       <c r="B49" s="54" t="n"/>
       <c r="C49" s="54" t="n"/>
@@ -2261,7 +2240,7 @@
       <c r="M49" s="54" t="n"/>
       <c r="XFD49" s="54" t="n"/>
     </row>
-    <row r="50" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="50" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A50" s="54" t="n"/>
       <c r="B50" s="54" t="n"/>
       <c r="C50" s="54" t="n"/>
@@ -2277,7 +2256,7 @@
       <c r="M50" s="54" t="n"/>
       <c r="XFD50" s="54" t="n"/>
     </row>
-    <row r="51" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="51" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A51" s="54" t="n"/>
       <c r="B51" s="54" t="n"/>
       <c r="C51" s="54" t="n"/>
@@ -2293,7 +2272,7 @@
       <c r="M51" s="54" t="n"/>
       <c r="XFD51" s="54" t="n"/>
     </row>
-    <row r="52" ht="39" customFormat="1" customHeight="1" s="118">
+    <row r="52" ht="39" customFormat="1" customHeight="1" s="117">
       <c r="A52" s="54" t="n"/>
       <c r="B52" s="54" t="n"/>
       <c r="C52" s="54" t="n"/>
@@ -2309,7 +2288,7 @@
       <c r="M52" s="54" t="n"/>
       <c r="XFD52" s="54" t="n"/>
     </row>
-    <row r="53" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="53" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A53" s="54" t="n"/>
       <c r="B53" s="54" t="n"/>
       <c r="C53" s="54" t="n"/>
@@ -2325,7 +2304,7 @@
       <c r="M53" s="54" t="n"/>
       <c r="XFD53" s="54" t="n"/>
     </row>
-    <row r="54" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="54" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A54" s="54" t="n"/>
       <c r="B54" s="54" t="n"/>
       <c r="C54" s="54" t="n"/>
@@ -2341,7 +2320,7 @@
       <c r="M54" s="54" t="n"/>
       <c r="XFD54" s="54" t="n"/>
     </row>
-    <row r="55" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="55" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A55" s="54" t="n"/>
       <c r="B55" s="54" t="n"/>
       <c r="C55" s="54" t="n"/>
@@ -2357,7 +2336,7 @@
       <c r="M55" s="54" t="n"/>
       <c r="XFD55" s="54" t="n"/>
     </row>
-    <row r="56" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="56" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A56" s="54" t="n"/>
       <c r="B56" s="54" t="n"/>
       <c r="C56" s="54" t="n"/>
@@ -2373,7 +2352,7 @@
       <c r="M56" s="54" t="n"/>
       <c r="XFD56" s="54" t="n"/>
     </row>
-    <row r="57" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="57" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A57" s="54" t="n"/>
       <c r="B57" s="54" t="n"/>
       <c r="C57" s="54" t="n"/>
@@ -2385,9 +2364,11 @@
       <c r="I57" s="54" t="n"/>
       <c r="J57" s="54" t="n"/>
       <c r="K57" s="54" t="n"/>
+      <c r="L57" s="54" t="n"/>
+      <c r="M57" s="54" t="n"/>
       <c r="XFD57" s="54" t="n"/>
     </row>
-    <row r="58" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="58" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A58" s="54" t="n"/>
       <c r="B58" s="54" t="n"/>
       <c r="C58" s="54" t="n"/>
@@ -2403,7 +2384,7 @@
       <c r="M58" s="54" t="n"/>
       <c r="XFD58" s="54" t="n"/>
     </row>
-    <row r="59" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="59" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A59" s="54" t="n"/>
       <c r="B59" s="54" t="n"/>
       <c r="C59" s="54" t="n"/>
@@ -2419,7 +2400,7 @@
       <c r="M59" s="54" t="n"/>
       <c r="XFD59" s="54" t="n"/>
     </row>
-    <row r="60" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="60" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A60" s="54" t="n"/>
       <c r="B60" s="54" t="n"/>
       <c r="C60" s="54" t="n"/>
@@ -2431,11 +2412,9 @@
       <c r="I60" s="54" t="n"/>
       <c r="J60" s="54" t="n"/>
       <c r="K60" s="54" t="n"/>
-      <c r="L60" s="54" t="n"/>
-      <c r="M60" s="54" t="n"/>
       <c r="XFD60" s="54" t="n"/>
     </row>
-    <row r="61" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="61" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A61" s="54" t="n"/>
       <c r="B61" s="54" t="n"/>
       <c r="C61" s="54" t="n"/>
@@ -2451,7 +2430,7 @@
       <c r="M61" s="54" t="n"/>
       <c r="XFD61" s="54" t="n"/>
     </row>
-    <row r="62" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="62" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A62" s="54" t="n"/>
       <c r="B62" s="54" t="n"/>
       <c r="C62" s="54" t="n"/>
@@ -2467,7 +2446,7 @@
       <c r="M62" s="54" t="n"/>
       <c r="XFD62" s="54" t="n"/>
     </row>
-    <row r="63" customFormat="1" s="119">
+    <row r="63" customFormat="1" s="118">
       <c r="A63" s="54" t="n"/>
       <c r="B63" s="54" t="n"/>
       <c r="C63" s="54" t="n"/>
@@ -2483,7 +2462,7 @@
       <c r="M63" s="54" t="n"/>
       <c r="XFD63" s="54" t="n"/>
     </row>
-    <row r="64" customFormat="1" s="119">
+    <row r="64" customFormat="1" s="118">
       <c r="A64" s="54" t="n"/>
       <c r="B64" s="54" t="n"/>
       <c r="C64" s="54" t="n"/>
@@ -2499,7 +2478,7 @@
       <c r="M64" s="54" t="n"/>
       <c r="XFD64" s="54" t="n"/>
     </row>
-    <row r="65" customFormat="1" s="119">
+    <row r="65" customFormat="1" s="118">
       <c r="A65" s="54" t="n"/>
       <c r="B65" s="54" t="n"/>
       <c r="C65" s="54" t="n"/>
@@ -2507,12 +2486,15 @@
       <c r="E65" s="54" t="n"/>
       <c r="F65" s="54" t="n"/>
       <c r="G65" s="54" t="n"/>
+      <c r="H65" s="54" t="n"/>
+      <c r="I65" s="54" t="n"/>
       <c r="J65" s="54" t="n"/>
       <c r="K65" s="54" t="n"/>
       <c r="L65" s="54" t="n"/>
+      <c r="M65" s="54" t="n"/>
       <c r="XFD65" s="54" t="n"/>
     </row>
-    <row r="66" customFormat="1" s="119">
+    <row r="66" customFormat="1" s="118">
       <c r="A66" s="54" t="n"/>
       <c r="B66" s="54" t="n"/>
       <c r="C66" s="54" t="n"/>
@@ -2520,12 +2502,15 @@
       <c r="E66" s="54" t="n"/>
       <c r="F66" s="54" t="n"/>
       <c r="G66" s="54" t="n"/>
+      <c r="H66" s="54" t="n"/>
+      <c r="I66" s="54" t="n"/>
       <c r="J66" s="54" t="n"/>
       <c r="K66" s="54" t="n"/>
       <c r="L66" s="54" t="n"/>
+      <c r="M66" s="54" t="n"/>
       <c r="XFD66" s="54" t="n"/>
     </row>
-    <row r="67" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="67" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A67" s="54" t="n"/>
       <c r="B67" s="54" t="n"/>
       <c r="C67" s="54" t="n"/>
@@ -2533,12 +2518,15 @@
       <c r="E67" s="54" t="n"/>
       <c r="F67" s="54" t="n"/>
       <c r="G67" s="54" t="n"/>
+      <c r="H67" s="54" t="n"/>
+      <c r="I67" s="54" t="n"/>
       <c r="J67" s="54" t="n"/>
       <c r="K67" s="54" t="n"/>
       <c r="L67" s="54" t="n"/>
+      <c r="M67" s="54" t="n"/>
       <c r="XFD67" s="54" t="n"/>
     </row>
-    <row r="68" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="68" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A68" s="54" t="n"/>
       <c r="B68" s="54" t="n"/>
       <c r="C68" s="54" t="n"/>
@@ -2546,15 +2534,12 @@
       <c r="E68" s="54" t="n"/>
       <c r="F68" s="54" t="n"/>
       <c r="G68" s="54" t="n"/>
-      <c r="H68" s="54" t="n"/>
-      <c r="I68" s="54" t="n"/>
       <c r="J68" s="54" t="n"/>
       <c r="K68" s="54" t="n"/>
       <c r="L68" s="54" t="n"/>
-      <c r="M68" s="54" t="n"/>
       <c r="XFD68" s="54" t="n"/>
     </row>
-    <row r="69" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="69" ht="39" customFormat="1" customHeight="1" s="116">
       <c r="A69" s="54" t="n"/>
       <c r="B69" s="54" t="n"/>
       <c r="C69" s="54" t="n"/>
@@ -2562,15 +2547,12 @@
       <c r="E69" s="54" t="n"/>
       <c r="F69" s="54" t="n"/>
       <c r="G69" s="54" t="n"/>
-      <c r="H69" s="54" t="n"/>
-      <c r="I69" s="54" t="n"/>
       <c r="J69" s="54" t="n"/>
       <c r="K69" s="54" t="n"/>
       <c r="L69" s="54" t="n"/>
-      <c r="M69" s="54" t="n"/>
       <c r="XFD69" s="54" t="n"/>
     </row>
-    <row r="70" customFormat="1" s="119">
+    <row r="70" customFormat="1" s="118">
       <c r="A70" s="54" t="n"/>
       <c r="B70" s="54" t="n"/>
       <c r="C70" s="54" t="n"/>
@@ -2578,15 +2560,12 @@
       <c r="E70" s="54" t="n"/>
       <c r="F70" s="54" t="n"/>
       <c r="G70" s="54" t="n"/>
-      <c r="H70" s="54" t="n"/>
-      <c r="I70" s="54" t="n"/>
       <c r="J70" s="54" t="n"/>
       <c r="K70" s="54" t="n"/>
       <c r="L70" s="54" t="n"/>
-      <c r="M70" s="54" t="n"/>
       <c r="XFD70" s="54" t="n"/>
     </row>
-    <row r="71" customFormat="1" s="119">
+    <row r="71" customFormat="1" s="118">
       <c r="A71" s="54" t="n"/>
       <c r="B71" s="54" t="n"/>
       <c r="C71" s="54" t="n"/>
@@ -2602,7 +2581,7 @@
       <c r="M71" s="54" t="n"/>
       <c r="XFD71" s="54" t="n"/>
     </row>
-    <row r="72" customFormat="1" s="119">
+    <row r="72" customFormat="1" s="118">
       <c r="A72" s="54" t="n"/>
       <c r="B72" s="54" t="n"/>
       <c r="C72" s="54" t="n"/>
@@ -2610,12 +2589,15 @@
       <c r="E72" s="54" t="n"/>
       <c r="F72" s="54" t="n"/>
       <c r="G72" s="54" t="n"/>
+      <c r="H72" s="54" t="n"/>
+      <c r="I72" s="54" t="n"/>
       <c r="J72" s="54" t="n"/>
       <c r="K72" s="54" t="n"/>
       <c r="L72" s="54" t="n"/>
+      <c r="M72" s="54" t="n"/>
       <c r="XFD72" s="54" t="n"/>
     </row>
-    <row r="73" customFormat="1" s="119">
+    <row r="73" customFormat="1" s="118">
       <c r="A73" s="54" t="n"/>
       <c r="B73" s="54" t="n"/>
       <c r="C73" s="54" t="n"/>
@@ -2623,12 +2605,15 @@
       <c r="E73" s="54" t="n"/>
       <c r="F73" s="54" t="n"/>
       <c r="G73" s="54" t="n"/>
+      <c r="H73" s="54" t="n"/>
+      <c r="I73" s="54" t="n"/>
       <c r="J73" s="54" t="n"/>
       <c r="K73" s="54" t="n"/>
       <c r="L73" s="54" t="n"/>
+      <c r="M73" s="54" t="n"/>
       <c r="XFD73" s="54" t="n"/>
     </row>
-    <row r="74" customFormat="1" s="119">
+    <row r="74" customFormat="1" s="118">
       <c r="A74" s="54" t="n"/>
       <c r="B74" s="54" t="n"/>
       <c r="C74" s="54" t="n"/>
@@ -2636,12 +2621,15 @@
       <c r="E74" s="54" t="n"/>
       <c r="F74" s="54" t="n"/>
       <c r="G74" s="54" t="n"/>
+      <c r="H74" s="54" t="n"/>
+      <c r="I74" s="54" t="n"/>
       <c r="J74" s="54" t="n"/>
       <c r="K74" s="54" t="n"/>
       <c r="L74" s="54" t="n"/>
+      <c r="M74" s="54" t="n"/>
       <c r="XFD74" s="54" t="n"/>
     </row>
-    <row r="75" ht="31.5" customFormat="1" customHeight="1" s="120">
+    <row r="75" ht="31.5" customFormat="1" customHeight="1" s="119">
       <c r="A75" s="54" t="n"/>
       <c r="B75" s="54" t="n"/>
       <c r="C75" s="54" t="n"/>
@@ -2649,15 +2637,12 @@
       <c r="E75" s="54" t="n"/>
       <c r="F75" s="54" t="n"/>
       <c r="G75" s="54" t="n"/>
-      <c r="H75" s="54" t="n"/>
-      <c r="I75" s="54" t="n"/>
       <c r="J75" s="54" t="n"/>
       <c r="K75" s="54" t="n"/>
       <c r="L75" s="54" t="n"/>
-      <c r="M75" s="54" t="n"/>
       <c r="XFD75" s="54" t="n"/>
     </row>
-    <row r="76" customFormat="1" s="119">
+    <row r="76" customFormat="1" s="118">
       <c r="A76" s="54" t="n"/>
       <c r="B76" s="54" t="n"/>
       <c r="C76" s="54" t="n"/>
@@ -2665,12 +2650,9 @@
       <c r="E76" s="54" t="n"/>
       <c r="F76" s="54" t="n"/>
       <c r="G76" s="54" t="n"/>
-      <c r="H76" s="54" t="n"/>
-      <c r="I76" s="54" t="n"/>
       <c r="J76" s="54" t="n"/>
       <c r="K76" s="54" t="n"/>
       <c r="L76" s="54" t="n"/>
-      <c r="M76" s="54" t="n"/>
       <c r="XFD76" s="54" t="n"/>
     </row>
     <row r="77">
@@ -2681,12 +2663,9 @@
       <c r="E77" s="54" t="n"/>
       <c r="F77" s="54" t="n"/>
       <c r="G77" s="54" t="n"/>
-      <c r="H77" s="54" t="n"/>
-      <c r="I77" s="54" t="n"/>
       <c r="J77" s="54" t="n"/>
       <c r="K77" s="54" t="n"/>
       <c r="L77" s="54" t="n"/>
-      <c r="M77" s="54" t="n"/>
       <c r="XFD77" s="54" t="n"/>
     </row>
     <row r="78">
@@ -2731,6 +2710,10 @@
       <c r="G80" s="54" t="n"/>
       <c r="H80" s="54" t="n"/>
       <c r="I80" s="54" t="n"/>
+      <c r="J80" s="54" t="n"/>
+      <c r="K80" s="54" t="n"/>
+      <c r="L80" s="54" t="n"/>
+      <c r="M80" s="54" t="n"/>
       <c r="XFD80" s="54" t="n"/>
     </row>
     <row r="81" customFormat="1" s="54">
@@ -2749,9 +2732,50 @@
       <c r="M81" s="54" t="n"/>
       <c r="XFD81" s="54" t="n"/>
     </row>
-    <row r="82" customFormat="1" s="54"/>
-    <row r="83" customFormat="1" s="54"/>
-    <row r="84" customFormat="1" s="54"/>
+    <row r="82" customFormat="1" s="54">
+      <c r="A82" s="54" t="n"/>
+      <c r="B82" s="54" t="n"/>
+      <c r="C82" s="54" t="n"/>
+      <c r="D82" s="54" t="n"/>
+      <c r="E82" s="54" t="n"/>
+      <c r="F82" s="54" t="n"/>
+      <c r="G82" s="54" t="n"/>
+      <c r="H82" s="54" t="n"/>
+      <c r="I82" s="54" t="n"/>
+      <c r="J82" s="54" t="n"/>
+      <c r="K82" s="54" t="n"/>
+      <c r="L82" s="54" t="n"/>
+      <c r="M82" s="54" t="n"/>
+      <c r="XFD82" s="54" t="n"/>
+    </row>
+    <row r="83" customFormat="1" s="54">
+      <c r="A83" s="54" t="n"/>
+      <c r="B83" s="54" t="n"/>
+      <c r="C83" s="54" t="n"/>
+      <c r="D83" s="54" t="n"/>
+      <c r="E83" s="54" t="n"/>
+      <c r="F83" s="54" t="n"/>
+      <c r="G83" s="54" t="n"/>
+      <c r="H83" s="54" t="n"/>
+      <c r="I83" s="54" t="n"/>
+      <c r="XFD83" s="54" t="n"/>
+    </row>
+    <row r="84" customFormat="1" s="54">
+      <c r="A84" s="54" t="n"/>
+      <c r="B84" s="54" t="n"/>
+      <c r="C84" s="54" t="n"/>
+      <c r="D84" s="54" t="n"/>
+      <c r="E84" s="54" t="n"/>
+      <c r="F84" s="54" t="n"/>
+      <c r="G84" s="54" t="n"/>
+      <c r="H84" s="54" t="n"/>
+      <c r="I84" s="54" t="n"/>
+      <c r="J84" s="54" t="n"/>
+      <c r="K84" s="54" t="n"/>
+      <c r="L84" s="54" t="n"/>
+      <c r="M84" s="54" t="n"/>
+      <c r="XFD84" s="54" t="n"/>
+    </row>
     <row r="85" customFormat="1" s="54"/>
     <row r="86"/>
     <row r="87"/>
@@ -2869,20 +2893,19 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="12">
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="E28:G28"/>
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E30:G30"/>
     <mergeCell ref="E26:G26"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D16:D22"/>
     <mergeCell ref="A26:C26"/>
-    <mergeCell ref="E25:G25"/>
   </mergeCells>
   <pageMargins left="1.0625" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" scale="36"/>
@@ -2898,81 +2921,81 @@
   </sheetPr>
   <dimension ref="A1:N200"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:C24"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="7.140625" defaultRowHeight="15"/>
   <cols>
-    <col width="28.28515625" customWidth="1" style="94" min="1" max="1"/>
-    <col width="27.28515625" customWidth="1" style="94" min="2" max="2"/>
-    <col width="30.5703125" customWidth="1" style="94" min="3" max="3"/>
-    <col width="22.140625" customWidth="1" style="94" min="4" max="4"/>
-    <col width="18.28515625" customWidth="1" style="94" min="5" max="5"/>
-    <col width="18.7109375" customWidth="1" style="94" min="6" max="6"/>
+    <col width="28.28515625" customWidth="1" style="90" min="1" max="1"/>
+    <col width="27.28515625" customWidth="1" style="90" min="2" max="2"/>
+    <col width="30.5703125" customWidth="1" style="90" min="3" max="3"/>
+    <col width="22.140625" customWidth="1" style="90" min="4" max="4"/>
+    <col width="18.28515625" customWidth="1" style="90" min="5" max="5"/>
+    <col width="18.7109375" customWidth="1" style="90" min="6" max="6"/>
     <col width="21.5703125" customWidth="1" style="4" min="7" max="7"/>
-    <col width="5" customWidth="1" style="94" min="8" max="8"/>
-    <col width="15.5703125" customWidth="1" style="94" min="9" max="9"/>
-    <col width="15.85546875" customWidth="1" style="94" min="10" max="11"/>
-    <col width="17.140625" customWidth="1" style="94" min="12" max="12"/>
-    <col width="7.140625" customWidth="1" style="94" min="13" max="16384"/>
+    <col width="5" customWidth="1" style="90" min="8" max="8"/>
+    <col width="15.5703125" customWidth="1" style="90" min="9" max="9"/>
+    <col width="15.85546875" customWidth="1" style="90" min="10" max="11"/>
+    <col width="17.140625" customWidth="1" style="90" min="12" max="12"/>
+    <col width="7.140625" customWidth="1" style="90" min="13" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="38.25" customHeight="1" s="121">
-      <c r="A1" s="90" t="inlineStr">
+    <row r="1" ht="38.25" customHeight="1" s="120">
+      <c r="A1" s="79" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="24" customHeight="1" s="121">
-      <c r="A2" s="91" t="inlineStr">
+    <row r="2" ht="24" customHeight="1" s="120">
+      <c r="A2" s="80" t="inlineStr">
         <is>
           <t xml:space="preserve"> XIN BAVET SEZ, Road No. 316A, Trapeang Bon and  Prey Kokir  Villages, Prey Kokir  Commune, Chantrea District, </t>
         </is>
       </c>
     </row>
-    <row r="3" ht="17.25" customHeight="1" s="121">
-      <c r="A3" s="92" t="inlineStr">
+    <row r="3" ht="17.25" customHeight="1" s="120">
+      <c r="A3" s="81" t="inlineStr">
         <is>
           <t>Svay Rieng Province, Kingdom of Cambodia.</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="17.25" customHeight="1" s="121">
-      <c r="A4" s="92" t="inlineStr">
+    <row r="4" ht="17.25" customHeight="1" s="120">
+      <c r="A4" s="81" t="inlineStr">
         <is>
           <t>VAT:L001-901903209</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="25.5" customHeight="1" s="121">
-      <c r="A5" s="93" t="inlineStr">
+    <row r="5" ht="25.5" customHeight="1" s="120">
+      <c r="A5" s="82" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="B5" s="122" t="n"/>
-      <c r="C5" s="122" t="n"/>
-      <c r="D5" s="122" t="n"/>
-      <c r="E5" s="122" t="n"/>
-      <c r="F5" s="122" t="n"/>
-      <c r="G5" s="122" t="n"/>
-    </row>
-    <row r="6" ht="69" customHeight="1" s="121">
-      <c r="A6" s="85" t="inlineStr">
+      <c r="B5" s="121" t="n"/>
+      <c r="C5" s="121" t="n"/>
+      <c r="D5" s="121" t="n"/>
+      <c r="E5" s="121" t="n"/>
+      <c r="F5" s="121" t="n"/>
+      <c r="G5" s="121" t="n"/>
+    </row>
+    <row r="6" ht="69" customHeight="1" s="120">
+      <c r="A6" s="84" t="inlineStr">
         <is>
           <t>INVOICE</t>
         </is>
       </c>
-      <c r="B6" s="123" t="n"/>
-      <c r="C6" s="123" t="n"/>
-      <c r="D6" s="123" t="n"/>
-      <c r="E6" s="123" t="n"/>
-      <c r="F6" s="123" t="n"/>
-      <c r="G6" s="123" t="n"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1" s="121">
+      <c r="B6" s="122" t="n"/>
+      <c r="C6" s="122" t="n"/>
+      <c r="D6" s="122" t="n"/>
+      <c r="E6" s="122" t="n"/>
+      <c r="F6" s="122" t="n"/>
+      <c r="G6" s="122" t="n"/>
+    </row>
+    <row r="7" ht="14.25" customHeight="1" s="120">
       <c r="A7" s="6" t="n"/>
       <c r="B7" s="6" t="n"/>
       <c r="C7" s="6" t="n"/>
@@ -2983,12 +3006,13 @@
           <t>Ref No.:</t>
         </is>
       </c>
-      <c r="G7" s="75">
-        <f>'[1]Packing list'!I7</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" ht="30" customHeight="1" s="121">
+      <c r="G7" s="10" t="inlineStr">
+        <is>
+          <t>CLF2025-116</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="30" customHeight="1" s="120">
       <c r="A8" s="36" t="inlineStr">
         <is>
           <t>EXPORTER:</t>
@@ -3007,13 +3031,13 @@
           <t>INVOICE NO :</t>
         </is>
       </c>
-      <c r="G8" s="76" t="inlineStr">
-        <is>
-          <t>MT2-25003E</t>
-        </is>
-      </c>
-    </row>
-    <row r="9" ht="21" customHeight="1" s="121">
+      <c r="G8" s="92" t="inlineStr">
+        <is>
+          <t>JFNO</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="21" customHeight="1" s="120">
       <c r="A9" s="31" t="n"/>
       <c r="B9" s="31" t="inlineStr">
         <is>
@@ -3028,11 +3052,11 @@
           <t>Date:</t>
         </is>
       </c>
-      <c r="G9" s="124" t="n">
-        <v>45831</v>
-      </c>
-    </row>
-    <row r="10" ht="22.5" customHeight="1" s="121">
+      <c r="G9" s="123" t="n">
+        <v>45906</v>
+      </c>
+    </row>
+    <row r="10" ht="22.5" customHeight="1" s="120">
       <c r="A10" s="31" t="n"/>
       <c r="B10" s="31" t="inlineStr">
         <is>
@@ -3053,7 +3077,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="20.25" customHeight="1" s="121">
+    <row r="11" ht="20.25" customHeight="1" s="120">
       <c r="A11" s="31" t="n"/>
       <c r="B11" s="31" t="inlineStr">
         <is>
@@ -3064,24 +3088,24 @@
       <c r="D11" s="37" t="n"/>
       <c r="E11" s="31" t="n"/>
       <c r="F11" s="6" t="n"/>
-      <c r="G11" s="91" t="n"/>
-    </row>
-    <row r="12" ht="15.75" customHeight="1" s="121">
+      <c r="G11" s="80" t="n"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1" s="120">
       <c r="A12" s="6" t="n"/>
       <c r="B12" s="6" t="n"/>
       <c r="C12" s="6" t="n"/>
       <c r="D12" s="6" t="n"/>
       <c r="E12" s="6" t="n"/>
       <c r="F12" s="6" t="n"/>
-      <c r="G12" s="91" t="n"/>
-    </row>
-    <row r="13" ht="25.5" customHeight="1" s="121">
+      <c r="G12" s="80" t="n"/>
+    </row>
+    <row r="13" ht="25.5" customHeight="1" s="120">
       <c r="B13" s="38" t="n"/>
       <c r="E13" s="39" t="n"/>
       <c r="F13" s="39" t="n"/>
       <c r="G13" s="32" t="n"/>
     </row>
-    <row r="14" ht="25.5" customHeight="1" s="121">
+    <row r="14" ht="25.5" customHeight="1" s="120">
       <c r="A14" s="11" t="inlineStr">
         <is>
           <t>CONSIGNEE :</t>
@@ -3097,16 +3121,16 @@
       <c r="E14" s="12" t="n"/>
       <c r="F14" s="12" t="n"/>
     </row>
-    <row r="15" ht="25.5" customHeight="1" s="121">
+    <row r="15" ht="25.5" customHeight="1" s="120">
       <c r="A15" s="10" t="n"/>
-      <c r="B15" s="86" t="inlineStr">
+      <c r="B15" s="85" t="inlineStr">
         <is>
           <t>Factory C-1B-B1-B and C-1B-B2, Lot C-1B-CN, DE4 Street,</t>
         </is>
       </c>
       <c r="F15" s="14" t="n"/>
     </row>
-    <row r="16" ht="25.5" customHeight="1" s="121">
+    <row r="16" ht="25.5" customHeight="1" s="120">
       <c r="A16" s="10" t="n"/>
       <c r="B16" s="15" t="inlineStr">
         <is>
@@ -3118,7 +3142,7 @@
       <c r="E16" s="12" t="n"/>
       <c r="F16" s="12" t="n"/>
     </row>
-    <row r="17" ht="24" customHeight="1" s="121">
+    <row r="17" ht="24" customHeight="1" s="120">
       <c r="A17" s="16" t="n"/>
       <c r="B17" s="15" t="inlineStr">
         <is>
@@ -3130,7 +3154,7 @@
       <c r="E17" s="1" t="n"/>
       <c r="F17" s="17" t="n"/>
     </row>
-    <row r="18" ht="26.1" customHeight="1" s="121">
+    <row r="18" ht="26.1" customHeight="1" s="120">
       <c r="A18" s="16" t="n"/>
       <c r="B18" s="15" t="inlineStr">
         <is>
@@ -3142,7 +3166,7 @@
       <c r="E18" s="1" t="n"/>
       <c r="F18" s="17" t="n"/>
     </row>
-    <row r="19" ht="27.75" customHeight="1" s="121">
+    <row r="19" ht="27.75" customHeight="1" s="120">
       <c r="A19" s="16" t="inlineStr">
         <is>
           <t xml:space="preserve">SHIP: </t>
@@ -3158,302 +3182,371 @@
       <c r="E19" s="1" t="n"/>
       <c r="F19" s="17" t="n"/>
     </row>
-    <row r="20" ht="27.75" customHeight="1" s="121">
+    <row r="20" ht="27.75" customHeight="1" s="120">
       <c r="A20" s="18" t="n"/>
       <c r="B20" s="18" t="n"/>
     </row>
-    <row r="21" ht="35" customHeight="1" s="121">
-      <c r="A21" s="125" t="inlineStr">
+    <row r="21" ht="35" customHeight="1" s="120">
+      <c r="A21" s="124" t="inlineStr">
         <is>
           <t>Mark &amp; Nº</t>
         </is>
       </c>
-      <c r="B21" s="125" t="inlineStr">
+      <c r="B21" s="124" t="inlineStr">
         <is>
           <t>P.O. Nº</t>
         </is>
       </c>
-      <c r="C21" s="125" t="inlineStr">
+      <c r="C21" s="124" t="inlineStr">
         <is>
           <t>ITEM Nº</t>
         </is>
       </c>
-      <c r="D21" s="125" t="inlineStr">
+      <c r="D21" s="124" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="E21" s="125" t="inlineStr">
+      <c r="E21" s="124" t="inlineStr">
         <is>
           <t>Quantity
 (SF)</t>
         </is>
       </c>
-      <c r="F21" s="125" t="inlineStr">
+      <c r="F21" s="124" t="inlineStr">
         <is>
           <t>Unit Price
 (USD)</t>
         </is>
       </c>
-      <c r="G21" s="125" t="inlineStr">
+      <c r="G21" s="124" t="inlineStr">
         <is>
           <t>Amount(USD)</t>
         </is>
       </c>
     </row>
-    <row r="22" ht="35" customHeight="1" s="121">
-      <c r="A22" s="126" t="inlineStr">
+    <row r="22" ht="35" customHeight="1" s="120">
+      <c r="A22" s="125" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B22" s="127" t="inlineStr">
+      <c r="B22" s="126" t="inlineStr">
         <is>
           <t>YNGY25022</t>
         </is>
       </c>
-      <c r="C22" s="127" t="inlineStr">
+      <c r="C22" s="126" t="inlineStr">
         <is>
           <t>M1243</t>
         </is>
       </c>
-      <c r="D22" s="128" t="inlineStr">
+      <c r="D22" s="127" t="inlineStr">
         <is>
           <t>LEATHER</t>
         </is>
       </c>
-      <c r="E22" s="129" t="n">
+      <c r="E22" s="128" t="n">
         <v>10045.4</v>
       </c>
-      <c r="F22" s="129">
-        <f>G22/E22</f>
+      <c r="F22" s="128" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="G22" s="128">
+        <f>F22*E22</f>
         <v/>
       </c>
-      <c r="G22" s="129" t="n">
-        <v>11451.756</v>
-      </c>
-    </row>
-    <row r="23" ht="35" customHeight="1" s="121">
-      <c r="A23" s="130" t="inlineStr">
+    </row>
+    <row r="23" ht="35" customHeight="1" s="120">
+      <c r="A23" s="129" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B23" s="127" t="inlineStr">
+      <c r="B23" s="126" t="inlineStr">
         <is>
           <t>YNGY25028</t>
         </is>
       </c>
-      <c r="C23" s="127" t="inlineStr">
+      <c r="C23" s="126" t="inlineStr">
         <is>
           <t>M1243</t>
         </is>
       </c>
-      <c r="D23" s="111" t="n"/>
-      <c r="E23" s="129" t="n">
-        <v>40549.3</v>
-      </c>
-      <c r="F23" s="129">
-        <f>G23/E23</f>
+      <c r="D23" s="110" t="n"/>
+      <c r="E23" s="128" t="n">
+        <v>40074.3</v>
+      </c>
+      <c r="F23" s="128" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="G23" s="128">
+        <f>F23*E23</f>
         <v/>
       </c>
-      <c r="G23" s="129" t="n">
-        <v>46116.952</v>
-      </c>
-    </row>
-    <row r="24" ht="35" customHeight="1" s="121">
-      <c r="A24" s="130" t="inlineStr">
+    </row>
+    <row r="24" ht="35" customHeight="1" s="120">
+      <c r="A24" s="129" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B24" s="127" t="inlineStr">
+      <c r="B24" s="126" t="inlineStr">
+        <is>
+          <t>YNGY25028</t>
+        </is>
+      </c>
+      <c r="C24" s="126" t="inlineStr">
+        <is>
+          <t>M1243</t>
+        </is>
+      </c>
+      <c r="D24" s="110" t="n"/>
+      <c r="E24" s="128" t="n">
+        <v>475</v>
+      </c>
+      <c r="F24" s="128" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="G24" s="128">
+        <f>F24*E24</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" ht="35" customHeight="1" s="120">
+      <c r="A25" s="129" t="inlineStr">
+        <is>
+          <t>MADE IN CAMBODIA</t>
+        </is>
+      </c>
+      <c r="B25" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="C24" s="127" t="inlineStr">
+      <c r="C25" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="D24" s="111" t="n"/>
-      <c r="E24" s="129" t="n">
-        <v>136491.8</v>
-      </c>
-      <c r="F24" s="129">
-        <f>G24/E24</f>
+      <c r="D25" s="110" t="n"/>
+      <c r="E25" s="128" t="n">
+        <v>136378.1</v>
+      </c>
+      <c r="F25" s="128" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="G25" s="128">
+        <f>F25*E25</f>
         <v/>
       </c>
-      <c r="G24" s="129" t="n">
-        <v>156939.419</v>
-      </c>
-    </row>
-    <row r="25" ht="35" customHeight="1" s="121">
-      <c r="A25" s="130" t="inlineStr">
-        <is>
-          <t>MADE IN CAMBODIA</t>
-        </is>
-      </c>
-      <c r="B25" s="127" t="inlineStr">
+    </row>
+    <row r="26" ht="35" customFormat="1" customHeight="1" s="2">
+      <c r="A26" s="129" t="n"/>
+      <c r="B26" s="126" t="inlineStr">
+        <is>
+          <t>GYOJY_M25371</t>
+        </is>
+      </c>
+      <c r="C26" s="126" t="inlineStr">
+        <is>
+          <t>Nick Dove</t>
+        </is>
+      </c>
+      <c r="D26" s="110" t="n"/>
+      <c r="E26" s="128" t="n">
+        <v>113.7</v>
+      </c>
+      <c r="F26" s="128" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="G26" s="128">
+        <f>F26*E26</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" ht="35" customHeight="1" s="120">
+      <c r="A27" s="129" t="n"/>
+      <c r="B27" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25374</t>
         </is>
       </c>
-      <c r="C25" s="127" t="inlineStr">
+      <c r="C27" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="D25" s="112" t="n"/>
-      <c r="E25" s="129" t="n">
-        <v>38841.3</v>
-      </c>
-      <c r="F25" s="129">
-        <f>G25/E25</f>
+      <c r="D27" s="110" t="n"/>
+      <c r="E27" s="128" t="n">
+        <v>38430</v>
+      </c>
+      <c r="F27" s="128" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="G27" s="128">
+        <f>F27*E27</f>
         <v/>
       </c>
-      <c r="G25" s="129" t="n">
-        <v>44572.89599999999</v>
-      </c>
-    </row>
-    <row r="26" ht="35" customFormat="1" customHeight="1" s="2">
-      <c r="A26" s="128" t="n"/>
-      <c r="B26" s="127" t="inlineStr">
+    </row>
+    <row r="28" ht="35" customHeight="1" s="120">
+      <c r="A28" s="129" t="n"/>
+      <c r="B28" s="126" t="inlineStr">
+        <is>
+          <t>GYOJY_M25374</t>
+        </is>
+      </c>
+      <c r="C28" s="126" t="inlineStr">
+        <is>
+          <t>Nick Dove</t>
+        </is>
+      </c>
+      <c r="D28" s="111" t="n"/>
+      <c r="E28" s="128" t="n">
+        <v>411.3</v>
+      </c>
+      <c r="F28" s="128" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="G28" s="128">
+        <f>F28*E28</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" ht="35" customHeight="1" s="120">
+      <c r="A29" s="127" t="n"/>
+      <c r="B29" s="126" t="inlineStr">
         <is>
           <t>HS.CODE: 4107.12.00</t>
         </is>
       </c>
-      <c r="C26" s="128" t="n"/>
-      <c r="D26" s="128" t="n"/>
-      <c r="E26" s="129" t="n"/>
-      <c r="F26" s="129" t="n"/>
-      <c r="G26" s="129" t="n"/>
-    </row>
-    <row r="27" ht="35" customHeight="1" s="121">
-      <c r="A27" s="131" t="n"/>
-      <c r="B27" s="131" t="inlineStr">
+      <c r="C29" s="127" t="n"/>
+      <c r="D29" s="127" t="n"/>
+      <c r="E29" s="128" t="n"/>
+      <c r="F29" s="128" t="n"/>
+      <c r="G29" s="128" t="n"/>
+    </row>
+    <row r="30" ht="35" customHeight="1" s="120">
+      <c r="A30" s="130" t="n"/>
+      <c r="B30" s="130" t="inlineStr">
         <is>
           <t>TOTAL OF:</t>
         </is>
       </c>
-      <c r="C27" s="131" t="inlineStr">
+      <c r="C30" s="130" t="inlineStr">
         <is>
           <t>22 PALLETS</t>
         </is>
       </c>
-      <c r="D27" s="131" t="n"/>
-      <c r="E27" s="132">
-        <f>SUM(E22:E25)</f>
+      <c r="D30" s="130" t="n"/>
+      <c r="E30" s="131">
+        <f>SUM(E22:E28)</f>
         <v/>
       </c>
-      <c r="F27" s="131" t="n"/>
-      <c r="G27" s="132">
-        <f>SUM(G22:G25)</f>
+      <c r="F30" s="130" t="n"/>
+      <c r="G30" s="131">
+        <f>SUM(G22:G28)</f>
         <v/>
       </c>
     </row>
-    <row r="28" ht="42" customHeight="1" s="121">
-      <c r="A28" s="87" t="inlineStr">
+    <row r="31" ht="42" customHeight="1" s="120">
+      <c r="A31" s="86" t="inlineStr">
         <is>
           <t xml:space="preserve">Country of Original Cambodia </t>
         </is>
       </c>
-      <c r="D28" s="87" t="n"/>
-      <c r="E28" s="6" t="n"/>
-      <c r="F28" s="6" t="n"/>
-      <c r="G28" s="91" t="n"/>
-    </row>
-    <row r="29" ht="61.5" customHeight="1" s="121">
-      <c r="A29" s="22" t="inlineStr">
+      <c r="D31" s="86" t="n"/>
+      <c r="E31" s="6" t="n"/>
+      <c r="F31" s="6" t="n"/>
+      <c r="G31" s="80" t="n"/>
+    </row>
+    <row r="32" ht="61.5" customHeight="1" s="120">
+      <c r="A32" s="22" t="inlineStr">
         <is>
           <t>Manufacture:</t>
         </is>
       </c>
-      <c r="B29" s="88" t="inlineStr">
+      <c r="B32" s="87" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="D29" s="88" t="n"/>
-      <c r="E29" s="88" t="n"/>
-      <c r="F29" s="6" t="n"/>
-      <c r="G29" s="91" t="n"/>
-    </row>
-    <row r="30" ht="44.1" customHeight="1" s="121">
-      <c r="A30" s="89" t="inlineStr">
+      <c r="D32" s="87" t="n"/>
+      <c r="E32" s="87" t="n"/>
+      <c r="F32" s="6" t="n"/>
+      <c r="G32" s="80" t="n"/>
+    </row>
+    <row r="33" ht="44.1" customHeight="1" s="120">
+      <c r="A33" s="88" t="inlineStr">
         <is>
           <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
                                                   /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
-      <c r="D30" s="89" t="n"/>
-      <c r="E30" s="89" t="n"/>
-      <c r="F30" s="89" t="n"/>
-      <c r="G30" s="91" t="n"/>
-    </row>
-    <row r="31" ht="24.75" customHeight="1" s="121">
-      <c r="A31" s="84" t="inlineStr">
+      <c r="D33" s="88" t="n"/>
+      <c r="E33" s="88" t="n"/>
+      <c r="F33" s="88" t="n"/>
+      <c r="G33" s="80" t="n"/>
+    </row>
+    <row r="34" ht="24.75" customHeight="1" s="120">
+      <c r="A34" s="83" t="inlineStr">
         <is>
           <t>A/C NO:100001100764430</t>
         </is>
       </c>
     </row>
-    <row r="32" ht="27" customHeight="1" s="121">
-      <c r="A32" s="84" t="inlineStr">
+    <row r="35" ht="27" customHeight="1" s="120">
+      <c r="A35" s="83" t="inlineStr">
         <is>
           <t>SWIFT CODE  ：BKCHKHPPXXX</t>
         </is>
       </c>
     </row>
-    <row r="33" ht="27.75" customHeight="1" s="121">
-      <c r="E33" s="31" t="n"/>
-      <c r="F33" s="33" t="inlineStr">
+    <row r="36" ht="21" customHeight="1" s="120">
+      <c r="E36" s="31" t="n"/>
+      <c r="F36" s="33" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
-      <c r="G33" s="91" t="n"/>
-    </row>
-    <row r="34" ht="27.75" customHeight="1" s="121">
-      <c r="E34" s="6" t="n"/>
-      <c r="F34" s="34" t="inlineStr">
+      <c r="G36" s="80" t="n"/>
+    </row>
+    <row r="37" ht="21" customHeight="1" s="120">
+      <c r="E37" s="6" t="n"/>
+      <c r="F37" s="34" t="inlineStr">
         <is>
           <t>Sign &amp; Stamp</t>
         </is>
       </c>
     </row>
-    <row r="35" ht="24.75" customHeight="1" s="121">
-      <c r="E35" s="6" t="n"/>
-      <c r="F35" s="6" t="n"/>
-    </row>
-    <row r="36" ht="21" customHeight="1" s="121">
-      <c r="E36" s="6" t="n"/>
-      <c r="F36" s="6" t="n"/>
-    </row>
-    <row r="37" ht="21" customHeight="1" s="121">
-      <c r="E37" s="6" t="n"/>
-      <c r="F37" s="40" t="inlineStr">
+    <row r="38" ht="21" customHeight="1" s="120">
+      <c r="E38" s="6" t="n"/>
+      <c r="F38" s="6" t="n"/>
+    </row>
+    <row r="39" ht="21" customHeight="1" s="120">
+      <c r="E39" s="6" t="n"/>
+      <c r="F39" s="6" t="n"/>
+    </row>
+    <row r="40" ht="21" customHeight="1" s="120">
+      <c r="E40" s="6" t="n"/>
+      <c r="F40" s="40" t="inlineStr">
         <is>
           <t>ZENG XUELI</t>
         </is>
       </c>
-      <c r="G37" s="35" t="n"/>
-    </row>
-    <row r="38" ht="21" customHeight="1" s="121"/>
-    <row r="39" ht="21" customHeight="1" s="121"/>
-    <row r="40" ht="21" customHeight="1" s="121"/>
-    <row r="41" ht="21" customHeight="1" s="121"/>
-    <row r="42" ht="21" customHeight="1" s="121"/>
-    <row r="43" ht="21" customHeight="1" s="121"/>
-    <row r="44" ht="25.5" customHeight="1" s="121"/>
-    <row r="45" ht="21" customHeight="1" s="121"/>
-    <row r="46" ht="21" customHeight="1" s="121"/>
-    <row r="47" ht="21" customHeight="1" s="121"/>
-    <row r="48" ht="21" customHeight="1" s="121"/>
-    <row r="49" ht="21" customHeight="1" s="121"/>
-    <row r="50" ht="17.25" customHeight="1" s="121"/>
+      <c r="G40" s="35" t="n"/>
+    </row>
+    <row r="41" ht="21" customHeight="1" s="120"/>
+    <row r="42" ht="21" customHeight="1" s="120"/>
+    <row r="43" ht="21" customHeight="1" s="120"/>
+    <row r="44" ht="25.5" customHeight="1" s="120"/>
+    <row r="45" ht="21" customHeight="1" s="120"/>
+    <row r="46" ht="21" customHeight="1" s="120"/>
+    <row r="47" ht="21" customHeight="1" s="120"/>
+    <row r="48" ht="21" customHeight="1" s="120"/>
+    <row r="49" ht="21" customHeight="1" s="120"/>
+    <row r="50" ht="17.25" customHeight="1" s="120"/>
     <row r="51"/>
     <row r="52"/>
     <row r="53"/>
@@ -3465,7 +3558,7 @@
     <row r="59"/>
     <row r="60"/>
     <row r="61"/>
-    <row r="62" ht="15" customHeight="1" s="121"/>
+    <row r="62" ht="15" customHeight="1" s="120"/>
     <row r="63"/>
     <row r="64"/>
     <row r="65"/>
@@ -3606,20 +3699,20 @@
     <row r="200"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="A33:C33"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="A3:G3"/>
     <mergeCell ref="A6:G6"/>
+    <mergeCell ref="D22:D28"/>
+    <mergeCell ref="B30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="A2:G2"/>
     <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="B32:C32"/>
     <mergeCell ref="A5:G5"/>
-    <mergeCell ref="B27"/>
   </mergeCells>
   <conditionalFormatting sqref="J22:J34">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>
@@ -3640,34 +3733,34 @@
   </sheetPr>
   <dimension ref="A1:N200"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A11" zoomScale="85" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A8" zoomScale="85" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="7.140625" defaultRowHeight="15"/>
   <cols>
-    <col width="29.140625" customWidth="1" style="94" min="1" max="1"/>
-    <col width="12.140625" customWidth="1" style="94" min="2" max="2"/>
-    <col width="25.85546875" customWidth="1" style="94" min="3" max="3"/>
-    <col width="23.140625" customWidth="1" style="94" min="4" max="4"/>
-    <col width="32.42578125" customWidth="1" style="94" min="5" max="5"/>
-    <col width="21.5703125" customWidth="1" style="94" min="6" max="6"/>
-    <col width="17.7109375" customWidth="1" style="94" min="7" max="7"/>
-    <col width="13.7109375" customWidth="1" style="94" min="8" max="8"/>
-    <col width="16.28515625" customWidth="1" style="94" min="9" max="9"/>
+    <col width="29.140625" customWidth="1" style="90" min="1" max="1"/>
+    <col width="12.140625" customWidth="1" style="90" min="2" max="2"/>
+    <col width="25.85546875" customWidth="1" style="90" min="3" max="3"/>
+    <col width="23.140625" customWidth="1" style="90" min="4" max="4"/>
+    <col width="32.42578125" customWidth="1" style="90" min="5" max="5"/>
+    <col width="21.5703125" customWidth="1" style="90" min="6" max="6"/>
+    <col width="17.7109375" customWidth="1" style="90" min="7" max="7"/>
+    <col width="13.7109375" customWidth="1" style="90" min="8" max="8"/>
+    <col width="16.28515625" customWidth="1" style="90" min="9" max="9"/>
     <col width="24.140625" customWidth="1" style="4" min="10" max="10"/>
-    <col width="15" customWidth="1" style="94" min="11" max="11"/>
-    <col width="10" customWidth="1" style="94" min="12" max="12"/>
-    <col width="25.140625" customWidth="1" style="94" min="13" max="13"/>
-    <col width="15.5703125" customWidth="1" style="94" min="14" max="14"/>
-    <col width="10.28515625" customWidth="1" style="94" min="15" max="15"/>
-    <col width="7.140625" customWidth="1" style="94" min="16" max="16"/>
-    <col width="12.42578125" customWidth="1" style="94" min="17" max="17"/>
-    <col width="7.140625" customWidth="1" style="94" min="18" max="16384"/>
+    <col width="15" customWidth="1" style="90" min="11" max="11"/>
+    <col width="10" customWidth="1" style="90" min="12" max="12"/>
+    <col width="25.140625" customWidth="1" style="90" min="13" max="13"/>
+    <col width="15.5703125" customWidth="1" style="90" min="14" max="14"/>
+    <col width="10.28515625" customWidth="1" style="90" min="15" max="15"/>
+    <col width="7.140625" customWidth="1" style="90" min="16" max="16"/>
+    <col width="12.42578125" customWidth="1" style="90" min="17" max="17"/>
+    <col width="7.140625" customWidth="1" style="90" min="18" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="38.25" customHeight="1" s="121">
-      <c r="A1" s="90" t="inlineStr">
+    <row r="1" ht="38.25" customHeight="1" s="120">
+      <c r="A1" s="79" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
@@ -3675,8 +3768,8 @@
       <c r="K1" s="26" t="n"/>
       <c r="L1" s="26" t="n"/>
     </row>
-    <row r="2" ht="24" customHeight="1" s="121">
-      <c r="A2" s="91" t="inlineStr">
+    <row r="2" ht="24" customHeight="1" s="120">
+      <c r="A2" s="80" t="inlineStr">
         <is>
           <t xml:space="preserve"> XIN BAVET SEZ, Road No. 316A, Trapeang Bon and  Prey Kokir  Villages, Prey Kokir  Commune, Chantrea District, </t>
         </is>
@@ -3684,61 +3777,61 @@
       <c r="K2" s="6" t="n"/>
       <c r="L2" s="6" t="n"/>
     </row>
-    <row r="3" ht="25.5" customHeight="1" s="121">
-      <c r="A3" s="92" t="inlineStr">
+    <row r="3" ht="25.5" customHeight="1" s="120">
+      <c r="A3" s="81" t="inlineStr">
         <is>
           <t>Svay Rieng Province, Kingdom of Cambodia.</t>
         </is>
       </c>
-      <c r="K3" s="84" t="n"/>
-      <c r="L3" s="84" t="n"/>
-    </row>
-    <row r="4" ht="25.5" customHeight="1" s="121">
-      <c r="A4" s="95" t="inlineStr">
+      <c r="K3" s="83" t="n"/>
+      <c r="L3" s="83" t="n"/>
+    </row>
+    <row r="4" ht="25.5" customHeight="1" s="120">
+      <c r="A4" s="89" t="inlineStr">
         <is>
           <t>VAT:L001-901903209</t>
         </is>
       </c>
-      <c r="K4" s="84" t="n"/>
-      <c r="L4" s="84" t="n"/>
-    </row>
-    <row r="5" ht="21.95" customHeight="1" s="121">
-      <c r="A5" s="93" t="inlineStr">
+      <c r="K4" s="83" t="n"/>
+      <c r="L4" s="83" t="n"/>
+    </row>
+    <row r="5" ht="21.95" customHeight="1" s="120">
+      <c r="A5" s="82" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="B5" s="122" t="n"/>
-      <c r="C5" s="122" t="n"/>
-      <c r="D5" s="122" t="n"/>
-      <c r="E5" s="122" t="n"/>
-      <c r="F5" s="122" t="n"/>
-      <c r="G5" s="122" t="n"/>
-      <c r="H5" s="122" t="n"/>
-      <c r="I5" s="122" t="n"/>
-      <c r="J5" s="122" t="n"/>
-      <c r="K5" s="84" t="n"/>
-      <c r="L5" s="84" t="n"/>
-    </row>
-    <row r="6" ht="54" customHeight="1" s="121">
-      <c r="A6" s="85" t="inlineStr">
+      <c r="B5" s="121" t="n"/>
+      <c r="C5" s="121" t="n"/>
+      <c r="D5" s="121" t="n"/>
+      <c r="E5" s="121" t="n"/>
+      <c r="F5" s="121" t="n"/>
+      <c r="G5" s="121" t="n"/>
+      <c r="H5" s="121" t="n"/>
+      <c r="I5" s="121" t="n"/>
+      <c r="J5" s="121" t="n"/>
+      <c r="K5" s="83" t="n"/>
+      <c r="L5" s="83" t="n"/>
+    </row>
+    <row r="6" ht="54" customHeight="1" s="120">
+      <c r="A6" s="84" t="inlineStr">
         <is>
           <t>PACKING LIST</t>
         </is>
       </c>
-      <c r="B6" s="123" t="n"/>
-      <c r="C6" s="123" t="n"/>
-      <c r="D6" s="123" t="n"/>
-      <c r="E6" s="123" t="n"/>
-      <c r="F6" s="123" t="n"/>
-      <c r="G6" s="123" t="n"/>
-      <c r="H6" s="123" t="n"/>
-      <c r="I6" s="123" t="n"/>
-      <c r="J6" s="123" t="n"/>
+      <c r="B6" s="122" t="n"/>
+      <c r="C6" s="122" t="n"/>
+      <c r="D6" s="122" t="n"/>
+      <c r="E6" s="122" t="n"/>
+      <c r="F6" s="122" t="n"/>
+      <c r="G6" s="122" t="n"/>
+      <c r="H6" s="122" t="n"/>
+      <c r="I6" s="122" t="n"/>
+      <c r="J6" s="122" t="n"/>
       <c r="K6" s="27" t="n"/>
       <c r="L6" s="27" t="n"/>
     </row>
-    <row r="7" ht="18.95" customHeight="1" s="121">
+    <row r="7" ht="18.95" customHeight="1" s="120">
       <c r="A7" s="6" t="n"/>
       <c r="B7" s="6" t="n"/>
       <c r="C7" s="6" t="n"/>
@@ -3752,13 +3845,13 @@
           <t>Ref No.:</t>
         </is>
       </c>
-      <c r="J7" s="75" t="inlineStr">
-        <is>
-          <t>CLF2025-186</t>
-        </is>
-      </c>
-    </row>
-    <row r="8" ht="30" customHeight="1" s="121">
+      <c r="J7" s="10" t="inlineStr">
+        <is>
+          <t>CLF2025-116</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="30" customHeight="1" s="120">
       <c r="A8" s="7" t="inlineStr">
         <is>
           <t>EXPORTER:</t>
@@ -3779,13 +3872,13 @@
           <t>INVOICE NO :</t>
         </is>
       </c>
-      <c r="J8" s="76" t="inlineStr">
-        <is>
-          <t>MT2-25003E</t>
-        </is>
-      </c>
-    </row>
-    <row r="9" ht="21" customHeight="1" s="121">
+      <c r="J8" s="92" t="inlineStr">
+        <is>
+          <t>JFNO</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="21" customHeight="1" s="120">
       <c r="A9" s="10" t="n"/>
       <c r="B9" s="10" t="inlineStr">
         <is>
@@ -3802,11 +3895,11 @@
           <t>Date:</t>
         </is>
       </c>
-      <c r="J9" s="124" t="n">
-        <v>45831</v>
-      </c>
-    </row>
-    <row r="10" ht="22.5" customHeight="1" s="121">
+      <c r="J9" s="123" t="n">
+        <v>45906</v>
+      </c>
+    </row>
+    <row r="10" ht="22.5" customHeight="1" s="120">
       <c r="A10" s="10" t="n"/>
       <c r="B10" s="10" t="inlineStr">
         <is>
@@ -3830,7 +3923,7 @@
       </c>
       <c r="K10" s="31" t="n"/>
     </row>
-    <row r="11" ht="20.25" customHeight="1" s="121">
+    <row r="11" ht="20.25" customHeight="1" s="120">
       <c r="A11" s="10" t="n"/>
       <c r="B11" s="10" t="inlineStr">
         <is>
@@ -3843,11 +3936,11 @@
       <c r="G11" s="10" t="n"/>
       <c r="H11" s="6" t="n"/>
       <c r="I11" s="6" t="n"/>
-      <c r="J11" s="91" t="n"/>
+      <c r="J11" s="80" t="n"/>
       <c r="K11" s="6" t="n"/>
       <c r="L11" s="6" t="n"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1" s="121">
+    <row r="12" ht="15.75" customHeight="1" s="120">
       <c r="A12" s="10" t="n"/>
       <c r="B12" s="10" t="n"/>
       <c r="C12" s="10" t="n"/>
@@ -3857,11 +3950,11 @@
       <c r="G12" s="10" t="n"/>
       <c r="H12" s="6" t="n"/>
       <c r="I12" s="6" t="n"/>
-      <c r="J12" s="91" t="n"/>
+      <c r="J12" s="80" t="n"/>
       <c r="K12" s="6" t="n"/>
       <c r="L12" s="6" t="n"/>
     </row>
-    <row r="13" ht="25.5" customHeight="1" s="121">
+    <row r="13" ht="25.5" customHeight="1" s="120">
       <c r="A13" s="11" t="inlineStr">
         <is>
           <t>CONSIGNEE :</t>
@@ -3877,20 +3970,20 @@
       <c r="F13" s="12" t="n"/>
       <c r="G13" s="12" t="n"/>
       <c r="H13" s="4" t="n"/>
-      <c r="J13" s="94" t="n"/>
-    </row>
-    <row r="14" ht="25.5" customHeight="1" s="121">
+      <c r="J13" s="90" t="n"/>
+    </row>
+    <row r="14" ht="25.5" customHeight="1" s="120">
       <c r="A14" s="10" t="n"/>
-      <c r="B14" s="86" t="inlineStr">
+      <c r="B14" s="85" t="inlineStr">
         <is>
           <t>Factory C-1B-B1-B and C-1B-B2, Lot C-1B-CN, DE4 Street,</t>
         </is>
       </c>
       <c r="G14" s="14" t="n"/>
       <c r="H14" s="4" t="n"/>
-      <c r="J14" s="94" t="n"/>
-    </row>
-    <row r="15" ht="25.5" customHeight="1" s="121">
+      <c r="J14" s="90" t="n"/>
+    </row>
+    <row r="15" ht="25.5" customHeight="1" s="120">
       <c r="A15" s="10" t="n"/>
       <c r="B15" s="15" t="inlineStr">
         <is>
@@ -3902,9 +3995,9 @@
       <c r="E15" s="12" t="n"/>
       <c r="G15" s="12" t="n"/>
       <c r="H15" s="4" t="n"/>
-      <c r="J15" s="94" t="n"/>
-    </row>
-    <row r="16" ht="24" customHeight="1" s="121">
+      <c r="J15" s="90" t="n"/>
+    </row>
+    <row r="16" ht="24" customHeight="1" s="120">
       <c r="A16" s="16" t="n"/>
       <c r="B16" s="15" t="inlineStr">
         <is>
@@ -3916,9 +4009,9 @@
       <c r="F16" s="1" t="n"/>
       <c r="G16" s="17" t="n"/>
       <c r="H16" s="4" t="n"/>
-      <c r="J16" s="94" t="n"/>
-    </row>
-    <row r="17" ht="26.1" customHeight="1" s="121">
+      <c r="J16" s="90" t="n"/>
+    </row>
+    <row r="17" ht="26.1" customHeight="1" s="120">
       <c r="A17" s="16" t="n"/>
       <c r="B17" s="15" t="inlineStr">
         <is>
@@ -3930,9 +4023,9 @@
       <c r="F17" s="1" t="n"/>
       <c r="G17" s="17" t="n"/>
       <c r="H17" s="4" t="n"/>
-      <c r="J17" s="94" t="n"/>
-    </row>
-    <row r="18" ht="27.75" customHeight="1" s="121">
+      <c r="J17" s="90" t="n"/>
+    </row>
+    <row r="18" ht="27.75" customHeight="1" s="120">
       <c r="A18" s="16" t="inlineStr">
         <is>
           <t xml:space="preserve">SHIP: </t>
@@ -3948,1253 +4041,1253 @@
       <c r="E18" s="1" t="n"/>
       <c r="F18" s="17" t="n"/>
       <c r="H18" s="4" t="n"/>
-      <c r="J18" s="94" t="n"/>
-    </row>
-    <row r="19" ht="27.75" customHeight="1" s="121">
+      <c r="J18" s="90" t="n"/>
+    </row>
+    <row r="19" ht="27.75" customHeight="1" s="120">
       <c r="A19" s="18" t="n"/>
       <c r="B19" s="18" t="n"/>
       <c r="C19" s="18" t="n"/>
     </row>
-    <row r="20" ht="27" customHeight="1" s="121">
-      <c r="A20" s="125" t="inlineStr">
+    <row r="20" ht="27" customHeight="1" s="120">
+      <c r="A20" s="124" t="inlineStr">
         <is>
           <t>Mark &amp; Nº</t>
         </is>
       </c>
-      <c r="B20" s="125" t="inlineStr">
+      <c r="B20" s="124" t="inlineStr">
         <is>
           <t>PALLET
 N.</t>
         </is>
       </c>
-      <c r="C20" s="125" t="inlineStr">
+      <c r="C20" s="124" t="inlineStr">
         <is>
           <t>P.O Nº</t>
         </is>
       </c>
-      <c r="D20" s="125" t="inlineStr">
+      <c r="D20" s="124" t="inlineStr">
         <is>
           <t>ITEM Nº</t>
         </is>
       </c>
-      <c r="E20" s="125" t="inlineStr">
+      <c r="E20" s="124" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="F20" s="125" t="inlineStr">
+      <c r="F20" s="124" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="G20" s="114" t="n"/>
-      <c r="H20" s="125" t="inlineStr">
+      <c r="G20" s="113" t="n"/>
+      <c r="H20" s="124" t="inlineStr">
         <is>
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="I20" s="125" t="inlineStr">
+      <c r="I20" s="124" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
         </is>
       </c>
-      <c r="J20" s="125" t="inlineStr">
+      <c r="J20" s="124" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
       </c>
     </row>
-    <row r="21" ht="27" customHeight="1" s="121">
-      <c r="A21" s="112" t="n"/>
-      <c r="B21" s="112" t="n"/>
-      <c r="C21" s="112" t="n"/>
-      <c r="D21" s="112" t="n"/>
-      <c r="E21" s="112" t="n"/>
-      <c r="F21" s="125" t="inlineStr">
+    <row r="21" ht="27" customHeight="1" s="120">
+      <c r="A21" s="111" t="n"/>
+      <c r="B21" s="111" t="n"/>
+      <c r="C21" s="111" t="n"/>
+      <c r="D21" s="111" t="n"/>
+      <c r="E21" s="111" t="n"/>
+      <c r="F21" s="124" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
       </c>
-      <c r="G21" s="125" t="inlineStr">
+      <c r="G21" s="124" t="inlineStr">
         <is>
           <t>SF</t>
         </is>
       </c>
-      <c r="H21" s="112" t="n"/>
-      <c r="I21" s="112" t="n"/>
-      <c r="J21" s="112" t="n"/>
-    </row>
-    <row r="22" ht="27" customHeight="1" s="121">
-      <c r="A22" s="133" t="inlineStr">
+      <c r="H21" s="111" t="n"/>
+      <c r="I21" s="111" t="n"/>
+      <c r="J21" s="111" t="n"/>
+    </row>
+    <row r="22" ht="27" customHeight="1" s="120">
+      <c r="A22" s="132" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B22" s="128" t="inlineStr">
+      <c r="B22" s="127" t="inlineStr">
         <is>
           <t>1-7</t>
         </is>
       </c>
-      <c r="C22" s="127" t="inlineStr">
+      <c r="C22" s="126" t="inlineStr">
         <is>
           <t>YNGY25022</t>
         </is>
       </c>
-      <c r="D22" s="127" t="inlineStr">
+      <c r="D22" s="126" t="inlineStr">
         <is>
           <t>M1243</t>
         </is>
       </c>
-      <c r="E22" s="127" t="inlineStr">
+      <c r="E22" s="126" t="inlineStr">
         <is>
           <t>LEATHER</t>
         </is>
       </c>
-      <c r="F22" s="134" t="n">
+      <c r="F22" s="133" t="n">
         <v>195</v>
       </c>
-      <c r="G22" s="135" t="n">
+      <c r="G22" s="134" t="n">
         <v>10045.4</v>
       </c>
-      <c r="H22" s="135" t="n">
+      <c r="H22" s="134" t="n">
         <v>804</v>
       </c>
-      <c r="I22" s="135" t="n">
+      <c r="I22" s="134" t="n">
         <v>759</v>
       </c>
-      <c r="J22" s="136" t="n">
+      <c r="J22" s="135" t="n">
         <v>2.4948</v>
       </c>
     </row>
-    <row r="23" ht="27" customHeight="1" s="121">
-      <c r="A23" s="137" t="inlineStr">
+    <row r="23" ht="27" customHeight="1" s="120">
+      <c r="A23" s="136" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B23" s="128" t="inlineStr">
+      <c r="B23" s="127" t="inlineStr">
         <is>
           <t>2-7</t>
         </is>
       </c>
-      <c r="C23" s="127" t="inlineStr">
+      <c r="C23" s="126" t="inlineStr">
         <is>
           <t>YNGY25028</t>
         </is>
       </c>
-      <c r="D23" s="127" t="inlineStr">
+      <c r="D23" s="126" t="inlineStr">
         <is>
           <t>M1243</t>
         </is>
       </c>
-      <c r="E23" s="111" t="n"/>
-      <c r="F23" s="134" t="n">
+      <c r="E23" s="110" t="n"/>
+      <c r="F23" s="133" t="n">
         <v>215</v>
       </c>
-      <c r="G23" s="135" t="n">
+      <c r="G23" s="134" t="n">
         <v>11181.6</v>
       </c>
-      <c r="H23" s="135" t="n">
+      <c r="H23" s="134" t="n">
         <v>887</v>
       </c>
-      <c r="I23" s="135" t="n">
+      <c r="I23" s="134" t="n">
         <v>842</v>
       </c>
-      <c r="J23" s="136" t="n">
+      <c r="J23" s="135" t="n">
         <v>2.772</v>
       </c>
     </row>
-    <row r="24" ht="27" customHeight="1" s="121">
-      <c r="A24" s="137" t="inlineStr">
+    <row r="24" ht="27" customHeight="1" s="120">
+      <c r="A24" s="136" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B24" s="128" t="inlineStr">
+      <c r="B24" s="127" t="inlineStr">
         <is>
           <t>3-7</t>
         </is>
       </c>
-      <c r="C24" s="127" t="inlineStr">
+      <c r="C24" s="126" t="inlineStr">
         <is>
           <t>YNGY25028</t>
         </is>
       </c>
-      <c r="D24" s="127" t="inlineStr">
+      <c r="D24" s="126" t="inlineStr">
         <is>
           <t>M1243</t>
         </is>
       </c>
-      <c r="E24" s="111" t="n"/>
-      <c r="F24" s="134" t="n">
+      <c r="E24" s="110" t="n"/>
+      <c r="F24" s="133" t="n">
         <v>210</v>
       </c>
-      <c r="G24" s="135" t="n">
+      <c r="G24" s="134" t="n">
         <v>10982.8</v>
       </c>
-      <c r="H24" s="135" t="n">
+      <c r="H24" s="134" t="n">
         <v>866.5</v>
       </c>
-      <c r="I24" s="135" t="n">
+      <c r="I24" s="134" t="n">
         <v>821.5</v>
       </c>
-      <c r="J24" s="136" t="n">
+      <c r="J24" s="135" t="n">
         <v>2.6532</v>
       </c>
     </row>
     <row r="25" ht="27" customFormat="1" customHeight="1" s="2">
-      <c r="A25" s="137" t="inlineStr">
+      <c r="A25" s="136" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B25" s="128" t="inlineStr">
+      <c r="B25" s="127" t="inlineStr">
         <is>
           <t>4-7</t>
         </is>
       </c>
-      <c r="C25" s="127" t="inlineStr">
+      <c r="C25" s="126" t="inlineStr">
         <is>
           <t>YNGY25028</t>
         </is>
       </c>
-      <c r="D25" s="127" t="inlineStr">
+      <c r="D25" s="126" t="inlineStr">
         <is>
           <t>M1243</t>
         </is>
       </c>
-      <c r="E25" s="111" t="n"/>
-      <c r="F25" s="134" t="n">
+      <c r="E25" s="110" t="n"/>
+      <c r="F25" s="133" t="n">
         <v>210</v>
       </c>
-      <c r="G25" s="135" t="n">
+      <c r="G25" s="134" t="n">
         <v>11087.8</v>
       </c>
-      <c r="H25" s="135" t="n">
+      <c r="H25" s="134" t="n">
         <v>878.5</v>
       </c>
-      <c r="I25" s="135" t="n">
+      <c r="I25" s="134" t="n">
         <v>833.5</v>
       </c>
-      <c r="J25" s="136" t="n">
+      <c r="J25" s="135" t="n">
         <v>2.8512</v>
       </c>
     </row>
-    <row r="26" ht="27" customHeight="1" s="121">
-      <c r="A26" s="137" t="n"/>
-      <c r="B26" s="128" t="inlineStr">
+    <row r="26" ht="27" customHeight="1" s="120">
+      <c r="A26" s="136" t="n"/>
+      <c r="B26" s="127" t="inlineStr">
         <is>
           <t>5-7</t>
         </is>
       </c>
-      <c r="C26" s="127" t="inlineStr">
+      <c r="C26" s="126" t="inlineStr">
         <is>
           <t>YNGY25028</t>
         </is>
       </c>
-      <c r="D26" s="127" t="inlineStr">
+      <c r="D26" s="126" t="inlineStr">
         <is>
           <t>M1243</t>
         </is>
       </c>
-      <c r="E26" s="111" t="n"/>
-      <c r="F26" s="134" t="n">
+      <c r="E26" s="110" t="n"/>
+      <c r="F26" s="133" t="n">
         <v>130</v>
       </c>
-      <c r="G26" s="135" t="n">
+      <c r="G26" s="134" t="n">
         <v>6822.1</v>
       </c>
-      <c r="H26" s="135" t="n">
+      <c r="H26" s="134" t="n">
         <v>555.7971</v>
       </c>
-      <c r="I26" s="135" t="n">
+      <c r="I26" s="134" t="n">
         <v>513.4058</v>
       </c>
-      <c r="J26" s="136" t="n">
+      <c r="J26" s="135" t="n">
         <v>2.1637</v>
       </c>
     </row>
-    <row r="27" ht="27" customHeight="1" s="121">
-      <c r="A27" s="137" t="n"/>
-      <c r="B27" s="112" t="n"/>
-      <c r="C27" s="127" t="inlineStr">
+    <row r="27" ht="27" customHeight="1" s="120">
+      <c r="A27" s="136" t="n"/>
+      <c r="B27" s="111" t="n"/>
+      <c r="C27" s="126" t="inlineStr">
         <is>
           <t>YNGY25028</t>
         </is>
       </c>
-      <c r="D27" s="127" t="inlineStr">
+      <c r="D27" s="126" t="inlineStr">
         <is>
           <t>M1243</t>
         </is>
       </c>
-      <c r="E27" s="111" t="n"/>
-      <c r="F27" s="134" t="n">
+      <c r="E27" s="110" t="n"/>
+      <c r="F27" s="133" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="135" t="n">
+      <c r="G27" s="134" t="n">
         <v>475</v>
       </c>
-      <c r="H27" s="135" t="n">
+      <c r="H27" s="134" t="n">
         <v>34.2029</v>
       </c>
-      <c r="I27" s="135" t="n">
+      <c r="I27" s="134" t="n">
         <v>31.5942</v>
       </c>
-      <c r="J27" s="136" t="n">
+      <c r="J27" s="135" t="n">
         <v>0.1331</v>
       </c>
     </row>
-    <row r="28" ht="27" customHeight="1" s="121">
-      <c r="A28" s="137" t="n"/>
-      <c r="B28" s="128" t="inlineStr">
+    <row r="28" ht="27" customHeight="1" s="120">
+      <c r="A28" s="136" t="n"/>
+      <c r="B28" s="127" t="inlineStr">
         <is>
           <t>6-7</t>
         </is>
       </c>
-      <c r="C28" s="127" t="inlineStr">
+      <c r="C28" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D28" s="127" t="inlineStr">
+      <c r="D28" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E28" s="111" t="n"/>
-      <c r="F28" s="134" t="n">
+      <c r="E28" s="110" t="n"/>
+      <c r="F28" s="133" t="n">
         <v>220</v>
       </c>
-      <c r="G28" s="135" t="n">
+      <c r="G28" s="134" t="n">
         <v>10205.7</v>
       </c>
-      <c r="H28" s="135" t="n">
+      <c r="H28" s="134" t="n">
         <v>820</v>
       </c>
-      <c r="I28" s="135" t="n">
+      <c r="I28" s="134" t="n">
         <v>775</v>
       </c>
-      <c r="J28" s="136" t="n">
+      <c r="J28" s="135" t="n">
         <v>2.4948</v>
       </c>
     </row>
-    <row r="29" ht="27" customHeight="1" s="121">
-      <c r="A29" s="137" t="n"/>
-      <c r="B29" s="128" t="inlineStr">
+    <row r="29" ht="27" customHeight="1" s="120">
+      <c r="A29" s="136" t="n"/>
+      <c r="B29" s="127" t="inlineStr">
         <is>
           <t>7-7</t>
         </is>
       </c>
-      <c r="C29" s="127" t="inlineStr">
+      <c r="C29" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D29" s="127" t="inlineStr">
+      <c r="D29" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E29" s="112" t="n"/>
-      <c r="F29" s="134" t="n">
+      <c r="E29" s="111" t="n"/>
+      <c r="F29" s="133" t="n">
         <v>215</v>
       </c>
-      <c r="G29" s="135" t="n">
+      <c r="G29" s="134" t="n">
         <v>10012.8</v>
       </c>
-      <c r="H29" s="135" t="n">
+      <c r="H29" s="134" t="n">
         <v>797.5</v>
       </c>
-      <c r="I29" s="135" t="n">
+      <c r="I29" s="134" t="n">
         <v>752.5</v>
       </c>
-      <c r="J29" s="136" t="n">
+      <c r="J29" s="135" t="n">
         <v>2.772</v>
       </c>
     </row>
-    <row r="30" ht="27" customHeight="1" s="121">
-      <c r="A30" s="131" t="n"/>
-      <c r="B30" s="131" t="n"/>
-      <c r="C30" s="131" t="inlineStr">
+    <row r="30" ht="27" customHeight="1" s="120">
+      <c r="A30" s="130" t="n"/>
+      <c r="B30" s="130" t="inlineStr">
         <is>
           <t>TOTAL:</t>
         </is>
       </c>
-      <c r="D30" s="131" t="inlineStr">
+      <c r="C30" s="130" t="inlineStr">
         <is>
           <t>7 PALLETS</t>
         </is>
       </c>
-      <c r="E30" s="131" t="n"/>
-      <c r="F30" s="138">
+      <c r="D30" s="130" t="n"/>
+      <c r="E30" s="130" t="n"/>
+      <c r="F30" s="137">
         <f>SUM(F22:F29)</f>
         <v/>
       </c>
-      <c r="G30" s="139">
+      <c r="G30" s="138">
         <f>SUM(G22:G29)</f>
         <v/>
       </c>
-      <c r="H30" s="139">
+      <c r="H30" s="138">
         <f>SUM(H22:H29)</f>
         <v/>
       </c>
-      <c r="I30" s="139">
+      <c r="I30" s="138">
         <f>SUM(I22:I29)</f>
         <v/>
       </c>
-      <c r="J30" s="140">
+      <c r="J30" s="139">
         <f>SUM(J22:J29)</f>
         <v/>
       </c>
     </row>
-    <row r="31" ht="27" customHeight="1" s="121"/>
-    <row r="32" ht="27" customHeight="1" s="121">
-      <c r="A32" s="125" t="inlineStr">
+    <row r="31" ht="27" customHeight="1" s="120"/>
+    <row r="32" ht="27" customHeight="1" s="120">
+      <c r="A32" s="124" t="inlineStr">
         <is>
           <t>Mark &amp; Nº</t>
         </is>
       </c>
-      <c r="B32" s="125" t="inlineStr">
+      <c r="B32" s="124" t="inlineStr">
         <is>
           <t>PALLET
 N.</t>
         </is>
       </c>
-      <c r="C32" s="125" t="inlineStr">
+      <c r="C32" s="124" t="inlineStr">
         <is>
           <t>P.O Nº</t>
         </is>
       </c>
-      <c r="D32" s="125" t="inlineStr">
+      <c r="D32" s="124" t="inlineStr">
         <is>
           <t>ITEM Nº</t>
         </is>
       </c>
-      <c r="E32" s="125" t="inlineStr">
+      <c r="E32" s="124" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="F32" s="125" t="inlineStr">
+      <c r="F32" s="124" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="G32" s="114" t="n"/>
-      <c r="H32" s="125" t="inlineStr">
+      <c r="G32" s="113" t="n"/>
+      <c r="H32" s="124" t="inlineStr">
         <is>
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="I32" s="125" t="inlineStr">
+      <c r="I32" s="124" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
         </is>
       </c>
-      <c r="J32" s="125" t="inlineStr">
+      <c r="J32" s="124" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
       </c>
     </row>
-    <row r="33" ht="27" customHeight="1" s="121">
-      <c r="A33" s="112" t="n"/>
-      <c r="B33" s="112" t="n"/>
-      <c r="C33" s="112" t="n"/>
-      <c r="D33" s="112" t="n"/>
-      <c r="E33" s="112" t="n"/>
-      <c r="F33" s="125" t="inlineStr">
+    <row r="33" ht="27" customHeight="1" s="120">
+      <c r="A33" s="111" t="n"/>
+      <c r="B33" s="111" t="n"/>
+      <c r="C33" s="111" t="n"/>
+      <c r="D33" s="111" t="n"/>
+      <c r="E33" s="111" t="n"/>
+      <c r="F33" s="124" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
       </c>
-      <c r="G33" s="125" t="inlineStr">
+      <c r="G33" s="124" t="inlineStr">
         <is>
           <t>SF</t>
         </is>
       </c>
-      <c r="H33" s="112" t="n"/>
-      <c r="I33" s="112" t="n"/>
-      <c r="J33" s="112" t="n"/>
-    </row>
-    <row r="34" ht="27" customHeight="1" s="121">
-      <c r="A34" s="133" t="inlineStr">
+      <c r="H33" s="111" t="n"/>
+      <c r="I33" s="111" t="n"/>
+      <c r="J33" s="111" t="n"/>
+    </row>
+    <row r="34" ht="27" customHeight="1" s="120">
+      <c r="A34" s="132" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B34" s="128" t="inlineStr">
+      <c r="B34" s="127" t="inlineStr">
         <is>
           <t>1-11</t>
         </is>
       </c>
-      <c r="C34" s="127" t="inlineStr">
+      <c r="C34" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D34" s="127" t="inlineStr">
+      <c r="D34" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E34" s="127" t="inlineStr">
+      <c r="E34" s="126" t="inlineStr">
         <is>
           <t>LEATHER</t>
         </is>
       </c>
-      <c r="F34" s="134" t="n">
+      <c r="F34" s="133" t="n">
         <v>225</v>
       </c>
-      <c r="G34" s="135" t="n">
+      <c r="G34" s="134" t="n">
         <v>10166.7</v>
       </c>
-      <c r="H34" s="135" t="n">
+      <c r="H34" s="134" t="n">
         <v>805.5</v>
       </c>
-      <c r="I34" s="135" t="n">
+      <c r="I34" s="134" t="n">
         <v>760.5</v>
       </c>
-      <c r="J34" s="136" t="n">
+      <c r="J34" s="135" t="n">
         <v>2.4948</v>
       </c>
     </row>
-    <row r="35" ht="27" customHeight="1" s="121">
-      <c r="A35" s="137" t="inlineStr">
+    <row r="35" ht="27" customHeight="1" s="120">
+      <c r="A35" s="136" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B35" s="128" t="inlineStr">
+      <c r="B35" s="127" t="inlineStr">
         <is>
           <t>2-11</t>
         </is>
       </c>
-      <c r="C35" s="127" t="inlineStr">
+      <c r="C35" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D35" s="127" t="inlineStr">
+      <c r="D35" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E35" s="111" t="n"/>
-      <c r="F35" s="134" t="n">
+      <c r="E35" s="110" t="n"/>
+      <c r="F35" s="133" t="n">
         <v>225</v>
       </c>
-      <c r="G35" s="135" t="n">
+      <c r="G35" s="134" t="n">
         <v>10363.9</v>
       </c>
-      <c r="H35" s="135" t="n">
+      <c r="H35" s="134" t="n">
         <v>818.5</v>
       </c>
-      <c r="I35" s="135" t="n">
+      <c r="I35" s="134" t="n">
         <v>773.5</v>
       </c>
-      <c r="J35" s="136" t="n">
+      <c r="J35" s="135" t="n">
         <v>2.5344</v>
       </c>
     </row>
-    <row r="36" ht="27" customHeight="1" s="121">
-      <c r="A36" s="137" t="inlineStr">
+    <row r="36" ht="27" customHeight="1" s="120">
+      <c r="A36" s="136" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B36" s="128" t="inlineStr">
+      <c r="B36" s="127" t="inlineStr">
         <is>
           <t>3-11</t>
         </is>
       </c>
-      <c r="C36" s="127" t="inlineStr">
+      <c r="C36" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D36" s="127" t="inlineStr">
+      <c r="D36" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E36" s="111" t="n"/>
-      <c r="F36" s="134" t="n">
+      <c r="E36" s="110" t="n"/>
+      <c r="F36" s="133" t="n">
         <v>220</v>
       </c>
-      <c r="G36" s="135" t="n">
+      <c r="G36" s="134" t="n">
         <v>10090.5</v>
       </c>
-      <c r="H36" s="135" t="n">
+      <c r="H36" s="134" t="n">
         <v>809</v>
       </c>
-      <c r="I36" s="135" t="n">
+      <c r="I36" s="134" t="n">
         <v>764</v>
       </c>
-      <c r="J36" s="136" t="n">
+      <c r="J36" s="135" t="n">
         <v>2.6136</v>
       </c>
     </row>
-    <row r="37" ht="27" customHeight="1" s="121">
-      <c r="A37" s="137" t="inlineStr">
+    <row r="37" ht="27" customHeight="1" s="120">
+      <c r="A37" s="136" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B37" s="128" t="inlineStr">
+      <c r="B37" s="127" t="inlineStr">
         <is>
           <t>4-11</t>
         </is>
       </c>
-      <c r="C37" s="127" t="inlineStr">
+      <c r="C37" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D37" s="127" t="inlineStr">
+      <c r="D37" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E37" s="111" t="n"/>
-      <c r="F37" s="134" t="n">
+      <c r="E37" s="110" t="n"/>
+      <c r="F37" s="133" t="n">
         <v>194</v>
       </c>
-      <c r="G37" s="135" t="n">
+      <c r="G37" s="134" t="n">
         <v>8956.4</v>
       </c>
-      <c r="H37" s="135" t="n">
+      <c r="H37" s="134" t="n">
         <v>711.5</v>
       </c>
-      <c r="I37" s="135" t="n">
+      <c r="I37" s="134" t="n">
         <v>666.5</v>
       </c>
-      <c r="J37" s="136" t="n">
+      <c r="J37" s="135" t="n">
         <v>2.3364</v>
       </c>
     </row>
-    <row r="38" ht="27" customHeight="1" s="121">
-      <c r="A38" s="137" t="n"/>
-      <c r="B38" s="128" t="inlineStr">
+    <row r="38" ht="27" customHeight="1" s="120">
+      <c r="A38" s="136" t="n"/>
+      <c r="B38" s="127" t="inlineStr">
         <is>
           <t>5-11</t>
         </is>
       </c>
-      <c r="C38" s="127" t="inlineStr">
+      <c r="C38" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D38" s="127" t="inlineStr">
+      <c r="D38" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E38" s="111" t="n"/>
-      <c r="F38" s="134" t="n">
+      <c r="E38" s="110" t="n"/>
+      <c r="F38" s="133" t="n">
         <v>220</v>
       </c>
-      <c r="G38" s="135" t="n">
+      <c r="G38" s="134" t="n">
         <v>10072.8</v>
       </c>
-      <c r="H38" s="135" t="n">
+      <c r="H38" s="134" t="n">
         <v>789.5</v>
       </c>
-      <c r="I38" s="135" t="n">
+      <c r="I38" s="134" t="n">
         <v>744.5</v>
       </c>
-      <c r="J38" s="136" t="n">
+      <c r="J38" s="135" t="n">
         <v>2.2968</v>
       </c>
     </row>
-    <row r="39" ht="27" customHeight="1" s="121">
-      <c r="A39" s="137" t="n"/>
-      <c r="B39" s="128" t="inlineStr">
+    <row r="39" ht="27" customHeight="1" s="120">
+      <c r="A39" s="136" t="n"/>
+      <c r="B39" s="127" t="inlineStr">
         <is>
           <t>6-11</t>
         </is>
       </c>
-      <c r="C39" s="127" t="inlineStr">
+      <c r="C39" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D39" s="127" t="inlineStr">
+      <c r="D39" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E39" s="111" t="n"/>
-      <c r="F39" s="134" t="n">
+      <c r="E39" s="110" t="n"/>
+      <c r="F39" s="133" t="n">
         <v>255</v>
       </c>
-      <c r="G39" s="135" t="n">
+      <c r="G39" s="134" t="n">
         <v>11907.9</v>
       </c>
-      <c r="H39" s="135" t="n">
+      <c r="H39" s="134" t="n">
         <v>939</v>
       </c>
-      <c r="I39" s="135" t="n">
+      <c r="I39" s="134" t="n">
         <v>894</v>
       </c>
-      <c r="J39" s="136" t="n">
+      <c r="J39" s="135" t="n">
         <v>2.772</v>
       </c>
     </row>
-    <row r="40" ht="27" customHeight="1" s="121">
-      <c r="A40" s="137" t="n"/>
-      <c r="B40" s="128" t="inlineStr">
+    <row r="40" ht="27" customHeight="1" s="120">
+      <c r="A40" s="136" t="n"/>
+      <c r="B40" s="127" t="inlineStr">
         <is>
           <t>7-11</t>
         </is>
       </c>
-      <c r="C40" s="127" t="inlineStr">
+      <c r="C40" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D40" s="127" t="inlineStr">
+      <c r="D40" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E40" s="111" t="n"/>
-      <c r="F40" s="134" t="n">
+      <c r="E40" s="110" t="n"/>
+      <c r="F40" s="133" t="n">
         <v>245</v>
       </c>
-      <c r="G40" s="135" t="n">
+      <c r="G40" s="134" t="n">
         <v>11152.3</v>
       </c>
-      <c r="H40" s="135" t="n">
+      <c r="H40" s="134" t="n">
         <v>879.7278</v>
       </c>
-      <c r="I40" s="135" t="n">
+      <c r="I40" s="134" t="n">
         <v>835.2722</v>
       </c>
-      <c r="J40" s="136" t="n">
+      <c r="J40" s="135" t="n">
         <v>2.5037</v>
       </c>
     </row>
-    <row r="41" ht="27" customHeight="1" s="121">
-      <c r="A41" s="137" t="n"/>
-      <c r="B41" s="112" t="n"/>
-      <c r="C41" s="127" t="inlineStr">
+    <row r="41" ht="27" customHeight="1" s="120">
+      <c r="A41" s="136" t="n"/>
+      <c r="B41" s="111" t="n"/>
+      <c r="C41" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D41" s="127" t="inlineStr">
+      <c r="D41" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E41" s="111" t="n"/>
-      <c r="F41" s="134" t="n">
+      <c r="E41" s="110" t="n"/>
+      <c r="F41" s="133" t="n">
         <v>3</v>
       </c>
-      <c r="G41" s="135" t="n">
+      <c r="G41" s="134" t="n">
         <v>113.7</v>
       </c>
-      <c r="H41" s="135" t="n">
+      <c r="H41" s="134" t="n">
         <v>10.7722</v>
       </c>
-      <c r="I41" s="135" t="n">
+      <c r="I41" s="134" t="n">
         <v>10.2278</v>
       </c>
-      <c r="J41" s="136" t="n">
+      <c r="J41" s="135" t="n">
         <v>0.0307</v>
       </c>
     </row>
-    <row r="42" ht="27" customHeight="1" s="121">
-      <c r="A42" s="137" t="n"/>
-      <c r="B42" s="128" t="inlineStr">
+    <row r="42" ht="27" customHeight="1" s="120">
+      <c r="A42" s="136" t="n"/>
+      <c r="B42" s="127" t="inlineStr">
         <is>
           <t>8-11</t>
         </is>
       </c>
-      <c r="C42" s="127" t="inlineStr">
+      <c r="C42" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D42" s="127" t="inlineStr">
+      <c r="D42" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E42" s="111" t="n"/>
-      <c r="F42" s="134" t="n">
+      <c r="E42" s="110" t="n"/>
+      <c r="F42" s="133" t="n">
         <v>232</v>
       </c>
-      <c r="G42" s="135" t="n">
+      <c r="G42" s="134" t="n">
         <v>11138.3</v>
       </c>
-      <c r="H42" s="135" t="n">
+      <c r="H42" s="134" t="n">
         <v>872.5</v>
       </c>
-      <c r="I42" s="135" t="n">
+      <c r="I42" s="134" t="n">
         <v>827.5</v>
       </c>
-      <c r="J42" s="136" t="n">
+      <c r="J42" s="135" t="n">
         <v>2.5344</v>
       </c>
     </row>
-    <row r="43" ht="27" customHeight="1" s="121">
-      <c r="A43" s="137" t="n"/>
-      <c r="B43" s="128" t="inlineStr">
+    <row r="43" ht="27" customHeight="1" s="120">
+      <c r="A43" s="136" t="n"/>
+      <c r="B43" s="127" t="inlineStr">
         <is>
           <t>9-11</t>
         </is>
       </c>
-      <c r="C43" s="127" t="inlineStr">
+      <c r="C43" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D43" s="127" t="inlineStr">
+      <c r="D43" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E43" s="111" t="n"/>
-      <c r="F43" s="134" t="n">
+      <c r="E43" s="110" t="n"/>
+      <c r="F43" s="133" t="n">
         <v>210</v>
       </c>
-      <c r="G43" s="135" t="n">
+      <c r="G43" s="134" t="n">
         <v>9969.5</v>
       </c>
-      <c r="H43" s="135" t="n">
+      <c r="H43" s="134" t="n">
         <v>786.5</v>
       </c>
-      <c r="I43" s="135" t="n">
+      <c r="I43" s="134" t="n">
         <v>741.5</v>
       </c>
-      <c r="J43" s="136" t="n">
+      <c r="J43" s="135" t="n">
         <v>2.376</v>
       </c>
     </row>
-    <row r="44" ht="27" customHeight="1" s="121">
-      <c r="A44" s="137" t="n"/>
-      <c r="B44" s="128" t="inlineStr">
+    <row r="44" ht="27" customHeight="1" s="120">
+      <c r="A44" s="136" t="n"/>
+      <c r="B44" s="127" t="inlineStr">
         <is>
           <t>10-11</t>
         </is>
       </c>
-      <c r="C44" s="127" t="inlineStr">
+      <c r="C44" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D44" s="127" t="inlineStr">
+      <c r="D44" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E44" s="111" t="n"/>
-      <c r="F44" s="134" t="n">
+      <c r="E44" s="110" t="n"/>
+      <c r="F44" s="133" t="n">
         <v>235</v>
       </c>
-      <c r="G44" s="135" t="n">
+      <c r="G44" s="134" t="n">
         <v>11202.6</v>
       </c>
-      <c r="H44" s="135" t="n">
+      <c r="H44" s="134" t="n">
         <v>884</v>
       </c>
-      <c r="I44" s="135" t="n">
+      <c r="I44" s="134" t="n">
         <v>839</v>
       </c>
-      <c r="J44" s="136" t="n">
+      <c r="J44" s="135" t="n">
         <v>2.376</v>
       </c>
     </row>
-    <row r="45" ht="27" customHeight="1" s="121">
-      <c r="A45" s="137" t="n"/>
-      <c r="B45" s="128" t="inlineStr">
+    <row r="45" ht="27" customHeight="1" s="120">
+      <c r="A45" s="136" t="n"/>
+      <c r="B45" s="127" t="inlineStr">
         <is>
           <t>11-11</t>
         </is>
       </c>
-      <c r="C45" s="127" t="inlineStr">
+      <c r="C45" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D45" s="127" t="inlineStr">
+      <c r="D45" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E45" s="112" t="n"/>
-      <c r="F45" s="134" t="n">
+      <c r="E45" s="111" t="n"/>
+      <c r="F45" s="133" t="n">
         <v>235</v>
       </c>
-      <c r="G45" s="135" t="n">
+      <c r="G45" s="134" t="n">
         <v>11138.7</v>
       </c>
-      <c r="H45" s="135" t="n">
+      <c r="H45" s="134" t="n">
         <v>878</v>
       </c>
-      <c r="I45" s="135" t="n">
+      <c r="I45" s="134" t="n">
         <v>833</v>
       </c>
-      <c r="J45" s="136" t="n">
+      <c r="J45" s="135" t="n">
         <v>2.376</v>
       </c>
     </row>
-    <row r="46" ht="27" customHeight="1" s="121">
-      <c r="A46" s="131" t="n"/>
-      <c r="B46" s="131" t="n"/>
-      <c r="C46" s="131" t="inlineStr">
+    <row r="46" ht="27" customHeight="1" s="120">
+      <c r="A46" s="130" t="n"/>
+      <c r="B46" s="130" t="inlineStr">
         <is>
           <t>TOTAL:</t>
         </is>
       </c>
-      <c r="D46" s="131" t="inlineStr">
+      <c r="C46" s="130" t="inlineStr">
         <is>
           <t>11 PALLETS</t>
         </is>
       </c>
-      <c r="E46" s="131" t="n"/>
-      <c r="F46" s="138">
+      <c r="D46" s="130" t="n"/>
+      <c r="E46" s="130" t="n"/>
+      <c r="F46" s="137">
         <f>SUM(F34:F45)</f>
         <v/>
       </c>
-      <c r="G46" s="139">
+      <c r="G46" s="138">
         <f>SUM(G34:G45)</f>
         <v/>
       </c>
-      <c r="H46" s="139">
+      <c r="H46" s="138">
         <f>SUM(H34:H45)</f>
         <v/>
       </c>
-      <c r="I46" s="139">
+      <c r="I46" s="138">
         <f>SUM(I34:I45)</f>
         <v/>
       </c>
-      <c r="J46" s="140">
+      <c r="J46" s="139">
         <f>SUM(J34:J45)</f>
         <v/>
       </c>
     </row>
-    <row r="47" ht="27" customHeight="1" s="121"/>
-    <row r="48" ht="27" customHeight="1" s="121">
-      <c r="A48" s="125" t="inlineStr">
+    <row r="47" ht="27" customHeight="1" s="120"/>
+    <row r="48" ht="27" customHeight="1" s="120">
+      <c r="A48" s="124" t="inlineStr">
         <is>
           <t>Mark &amp; Nº</t>
         </is>
       </c>
-      <c r="B48" s="125" t="inlineStr">
+      <c r="B48" s="124" t="inlineStr">
         <is>
           <t>PALLET
 N.</t>
         </is>
       </c>
-      <c r="C48" s="125" t="inlineStr">
+      <c r="C48" s="124" t="inlineStr">
         <is>
           <t>P.O Nº</t>
         </is>
       </c>
-      <c r="D48" s="125" t="inlineStr">
+      <c r="D48" s="124" t="inlineStr">
         <is>
           <t>ITEM Nº</t>
         </is>
       </c>
-      <c r="E48" s="125" t="inlineStr">
+      <c r="E48" s="124" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="F48" s="125" t="inlineStr">
+      <c r="F48" s="124" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="G48" s="114" t="n"/>
-      <c r="H48" s="125" t="inlineStr">
+      <c r="G48" s="113" t="n"/>
+      <c r="H48" s="124" t="inlineStr">
         <is>
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="I48" s="125" t="inlineStr">
+      <c r="I48" s="124" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
         </is>
       </c>
-      <c r="J48" s="125" t="inlineStr">
+      <c r="J48" s="124" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
       </c>
     </row>
-    <row r="49" ht="27" customHeight="1" s="121">
-      <c r="A49" s="112" t="n"/>
-      <c r="B49" s="112" t="n"/>
-      <c r="C49" s="112" t="n"/>
-      <c r="D49" s="112" t="n"/>
-      <c r="E49" s="112" t="n"/>
-      <c r="F49" s="125" t="inlineStr">
+    <row r="49" ht="27" customHeight="1" s="120">
+      <c r="A49" s="111" t="n"/>
+      <c r="B49" s="111" t="n"/>
+      <c r="C49" s="111" t="n"/>
+      <c r="D49" s="111" t="n"/>
+      <c r="E49" s="111" t="n"/>
+      <c r="F49" s="124" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
       </c>
-      <c r="G49" s="125" t="inlineStr">
+      <c r="G49" s="124" t="inlineStr">
         <is>
           <t>SF</t>
         </is>
       </c>
-      <c r="H49" s="112" t="n"/>
-      <c r="I49" s="112" t="n"/>
-      <c r="J49" s="112" t="n"/>
-    </row>
-    <row r="50" ht="27" customHeight="1" s="121">
-      <c r="A50" s="133" t="inlineStr">
+      <c r="H49" s="111" t="n"/>
+      <c r="I49" s="111" t="n"/>
+      <c r="J49" s="111" t="n"/>
+    </row>
+    <row r="50" ht="27" customHeight="1" s="120">
+      <c r="A50" s="132" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B50" s="128" t="inlineStr">
+      <c r="B50" s="127" t="inlineStr">
         <is>
           <t>1-4</t>
         </is>
       </c>
-      <c r="C50" s="127" t="inlineStr">
+      <c r="C50" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25374</t>
         </is>
       </c>
-      <c r="D50" s="127" t="inlineStr">
+      <c r="D50" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E50" s="127" t="inlineStr">
+      <c r="E50" s="126" t="inlineStr">
         <is>
           <t>LEATHER</t>
         </is>
       </c>
-      <c r="F50" s="134" t="n">
+      <c r="F50" s="133" t="n">
         <v>240</v>
       </c>
-      <c r="G50" s="135" t="n">
+      <c r="G50" s="134" t="n">
         <v>11235.9</v>
       </c>
-      <c r="H50" s="135" t="n">
+      <c r="H50" s="134" t="n">
         <v>874.5</v>
       </c>
-      <c r="I50" s="135" t="n">
+      <c r="I50" s="134" t="n">
         <v>829.5</v>
       </c>
-      <c r="J50" s="136" t="n">
+      <c r="J50" s="135" t="n">
         <v>2.772</v>
       </c>
     </row>
-    <row r="51" ht="27" customHeight="1" s="121">
-      <c r="A51" s="137" t="inlineStr">
+    <row r="51" ht="27" customHeight="1" s="120">
+      <c r="A51" s="136" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B51" s="128" t="inlineStr">
+      <c r="B51" s="127" t="inlineStr">
         <is>
           <t>2-4</t>
         </is>
       </c>
-      <c r="C51" s="127" t="inlineStr">
+      <c r="C51" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25374</t>
         </is>
       </c>
-      <c r="D51" s="127" t="inlineStr">
+      <c r="D51" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E51" s="111" t="n"/>
-      <c r="F51" s="134" t="n">
+      <c r="E51" s="110" t="n"/>
+      <c r="F51" s="133" t="n">
         <v>230</v>
       </c>
-      <c r="G51" s="135" t="n">
+      <c r="G51" s="134" t="n">
         <v>11142</v>
       </c>
-      <c r="H51" s="135" t="n">
+      <c r="H51" s="134" t="n">
         <v>865.5</v>
       </c>
-      <c r="I51" s="135" t="n">
+      <c r="I51" s="134" t="n">
         <v>820.5</v>
       </c>
-      <c r="J51" s="136" t="n">
+      <c r="J51" s="135" t="n">
         <v>2.6136</v>
       </c>
     </row>
-    <row r="52" ht="27" customHeight="1" s="121">
-      <c r="A52" s="137" t="inlineStr">
+    <row r="52" ht="27" customHeight="1" s="120">
+      <c r="A52" s="136" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B52" s="128" t="inlineStr">
+      <c r="B52" s="127" t="inlineStr">
         <is>
           <t>3-4</t>
         </is>
       </c>
-      <c r="C52" s="127" t="inlineStr">
+      <c r="C52" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25374</t>
         </is>
       </c>
-      <c r="D52" s="127" t="inlineStr">
+      <c r="D52" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E52" s="111" t="n"/>
-      <c r="F52" s="134" t="n">
+      <c r="E52" s="110" t="n"/>
+      <c r="F52" s="133" t="n">
         <v>235</v>
       </c>
-      <c r="G52" s="135" t="n">
+      <c r="G52" s="134" t="n">
         <v>11237.6</v>
       </c>
-      <c r="H52" s="135" t="n">
+      <c r="H52" s="134" t="n">
         <v>868.5</v>
       </c>
-      <c r="I52" s="135" t="n">
+      <c r="I52" s="134" t="n">
         <v>823.5</v>
       </c>
-      <c r="J52" s="136" t="n">
+      <c r="J52" s="135" t="n">
         <v>2.574</v>
       </c>
     </row>
-    <row r="53" ht="27" customHeight="1" s="121">
-      <c r="A53" s="137" t="inlineStr">
+    <row r="53" ht="27" customHeight="1" s="120">
+      <c r="A53" s="136" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B53" s="128" t="inlineStr">
+      <c r="B53" s="127" t="inlineStr">
         <is>
           <t>4-4</t>
         </is>
       </c>
-      <c r="C53" s="127" t="inlineStr">
+      <c r="C53" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25374</t>
         </is>
       </c>
-      <c r="D53" s="127" t="inlineStr">
+      <c r="D53" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E53" s="111" t="n"/>
-      <c r="F53" s="134" t="n">
+      <c r="E53" s="110" t="n"/>
+      <c r="F53" s="133" t="n">
         <v>99</v>
       </c>
-      <c r="G53" s="135" t="n">
+      <c r="G53" s="134" t="n">
         <v>4814.5</v>
       </c>
-      <c r="H53" s="135" t="n">
+      <c r="H53" s="134" t="n">
         <v>401.5</v>
       </c>
-      <c r="I53" s="135" t="n">
+      <c r="I53" s="134" t="n">
         <v>360.25</v>
       </c>
-      <c r="J53" s="136" t="n">
+      <c r="J53" s="135" t="n">
         <v>2.178</v>
       </c>
     </row>
-    <row r="54" ht="27" customHeight="1" s="121">
-      <c r="A54" s="137" t="n"/>
-      <c r="B54" s="112" t="n"/>
-      <c r="C54" s="127" t="inlineStr">
+    <row r="54" ht="27" customHeight="1" s="120">
+      <c r="A54" s="136" t="n"/>
+      <c r="B54" s="111" t="n"/>
+      <c r="C54" s="126" t="inlineStr">
         <is>
           <t>GYOJY_M25374</t>
         </is>
       </c>
-      <c r="D54" s="127" t="inlineStr">
+      <c r="D54" s="126" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E54" s="112" t="n"/>
-      <c r="F54" s="134" t="n">
+      <c r="E54" s="111" t="n"/>
+      <c r="F54" s="133" t="n">
         <v>9</v>
       </c>
-      <c r="G54" s="135" t="n">
+      <c r="G54" s="134" t="n">
         <v>411.3</v>
       </c>
-      <c r="H54" s="135" t="n">
+      <c r="H54" s="134" t="n">
         <v>36.5</v>
       </c>
-      <c r="I54" s="135" t="n">
+      <c r="I54" s="134" t="n">
         <v>32.75</v>
       </c>
-      <c r="J54" s="136" t="n">
+      <c r="J54" s="135" t="n">
         <v>0.198</v>
       </c>
     </row>
-    <row r="55" ht="27" customHeight="1" s="121">
-      <c r="A55" s="131" t="n"/>
-      <c r="B55" s="131" t="n"/>
-      <c r="C55" s="131" t="inlineStr">
+    <row r="55" ht="27" customHeight="1" s="120">
+      <c r="A55" s="130" t="n"/>
+      <c r="B55" s="130" t="inlineStr">
         <is>
           <t>TOTAL:</t>
         </is>
       </c>
-      <c r="D55" s="131" t="inlineStr">
+      <c r="C55" s="130" t="inlineStr">
         <is>
           <t>4 PALLETS</t>
         </is>
       </c>
-      <c r="E55" s="131" t="n"/>
-      <c r="F55" s="138">
+      <c r="D55" s="130" t="n"/>
+      <c r="E55" s="130" t="n"/>
+      <c r="F55" s="137">
         <f>SUM(F50:F54)</f>
         <v/>
       </c>
-      <c r="G55" s="139">
+      <c r="G55" s="138">
         <f>SUM(G50:G54)</f>
         <v/>
       </c>
-      <c r="H55" s="139">
+      <c r="H55" s="138">
         <f>SUM(H50:H54)</f>
         <v/>
       </c>
-      <c r="I55" s="139">
+      <c r="I55" s="138">
         <f>SUM(I50:I54)</f>
         <v/>
       </c>
-      <c r="J55" s="140">
+      <c r="J55" s="139">
         <f>SUM(J50:J54)</f>
         <v/>
       </c>
     </row>
-    <row r="56" ht="27" customHeight="1" s="121">
-      <c r="C56" s="141" t="inlineStr">
+    <row r="56" ht="27" customHeight="1" s="120">
+      <c r="B56" s="140" t="inlineStr">
         <is>
           <t>TOTAL OF:</t>
         </is>
       </c>
-      <c r="D56" s="141" t="inlineStr">
+      <c r="C56" s="140" t="inlineStr">
         <is>
           <t>22 PALLETS</t>
         </is>
       </c>
-      <c r="F56" s="142">
+      <c r="F56" s="141">
         <f>SUM(F22:F29,F34:F45,F50:F54)</f>
         <v/>
       </c>
-      <c r="G56" s="143">
+      <c r="G56" s="142">
         <f>SUM(G22:G29,G34:G45,G50:G54)</f>
         <v/>
       </c>
-      <c r="H56" s="143">
+      <c r="H56" s="142">
         <f>SUM(H22:H29,H34:H45,H50:H54)</f>
         <v/>
       </c>
-      <c r="I56" s="143">
+      <c r="I56" s="142">
         <f>SUM(I22:I29,I34:I45,I50:I54)</f>
         <v/>
       </c>
-      <c r="J56" s="144">
+      <c r="J56" s="143">
         <f>SUM(J22:J29,J34:J45,J50:J54)</f>
         <v/>
       </c>
@@ -5215,71 +5308,71 @@
       <c r="I57" s="20" t="n"/>
       <c r="J57" s="32" t="n"/>
     </row>
-    <row r="58" ht="35.1" customHeight="1" s="121">
-      <c r="A58" s="87" t="inlineStr">
+    <row r="58" ht="35.1" customHeight="1" s="120">
+      <c r="A58" s="86" t="inlineStr">
         <is>
           <t xml:space="preserve">Country of Original Cambodia </t>
         </is>
       </c>
-      <c r="E58" s="87" t="n"/>
-      <c r="F58" s="87" t="n"/>
+      <c r="E58" s="86" t="n"/>
+      <c r="F58" s="86" t="n"/>
       <c r="G58" s="6" t="n"/>
       <c r="H58" s="6" t="n"/>
       <c r="I58" s="6" t="n"/>
-      <c r="J58" s="91" t="n"/>
+      <c r="J58" s="80" t="n"/>
       <c r="K58" s="6" t="n"/>
       <c r="L58" s="6" t="n"/>
       <c r="M58" s="33" t="n"/>
     </row>
-    <row r="59" ht="72" customHeight="1" s="121">
+    <row r="59" ht="72" customHeight="1" s="120">
       <c r="A59" s="22" t="inlineStr">
         <is>
           <t>Manufacture:</t>
         </is>
       </c>
       <c r="B59" s="22" t="n"/>
-      <c r="C59" s="88" t="inlineStr">
+      <c r="C59" s="87" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="E59" s="88" t="n"/>
-      <c r="F59" s="88" t="n"/>
-      <c r="G59" s="88" t="n"/>
-      <c r="H59" s="88" t="n"/>
+      <c r="E59" s="87" t="n"/>
+      <c r="F59" s="87" t="n"/>
+      <c r="G59" s="87" t="n"/>
+      <c r="H59" s="87" t="n"/>
       <c r="I59" s="6" t="n"/>
-      <c r="J59" s="91" t="n"/>
+      <c r="J59" s="80" t="n"/>
       <c r="K59" s="6" t="n"/>
       <c r="L59" s="6" t="n"/>
       <c r="M59" s="33" t="n"/>
     </row>
-    <row r="60" ht="48" customHeight="1" s="121">
-      <c r="A60" s="89" t="inlineStr">
+    <row r="60" ht="48" customHeight="1" s="120">
+      <c r="A60" s="88" t="inlineStr">
         <is>
           <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
                                           /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
-      <c r="E60" s="89" t="n"/>
-      <c r="F60" s="89" t="n"/>
-      <c r="G60" s="89" t="n"/>
-      <c r="H60" s="89" t="n"/>
-      <c r="I60" s="89" t="n"/>
-      <c r="J60" s="91" t="n"/>
-      <c r="K60" s="84" t="n"/>
-      <c r="L60" s="84" t="n"/>
+      <c r="E60" s="88" t="n"/>
+      <c r="F60" s="88" t="n"/>
+      <c r="G60" s="88" t="n"/>
+      <c r="H60" s="88" t="n"/>
+      <c r="I60" s="88" t="n"/>
+      <c r="J60" s="80" t="n"/>
+      <c r="K60" s="83" t="n"/>
+      <c r="L60" s="83" t="n"/>
       <c r="M60" s="33" t="n"/>
     </row>
-    <row r="61" ht="30" customHeight="1" s="121">
-      <c r="A61" s="84" t="inlineStr">
+    <row r="61" ht="30" customHeight="1" s="120">
+      <c r="A61" s="83" t="inlineStr">
         <is>
           <t>A/C NO:100001100764430</t>
         </is>
       </c>
     </row>
-    <row r="62" ht="32.1" customHeight="1" s="121">
-      <c r="A62" s="84" t="inlineStr">
+    <row r="62" ht="32.1" customHeight="1" s="120">
+      <c r="A62" s="83" t="inlineStr">
         <is>
           <t>SWIFT CODE  ：BKCHKHPPXXX</t>
         </is>
@@ -5293,7 +5386,7 @@
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
-      <c r="J63" s="91" t="n"/>
+      <c r="J63" s="80" t="n"/>
     </row>
     <row r="64">
       <c r="G64" s="6" t="n"/>
@@ -5309,7 +5402,7 @@
       <c r="G66" s="6" t="n"/>
       <c r="H66" s="6" t="n"/>
       <c r="I66" s="6" t="n"/>
-      <c r="K66" s="94" t="n"/>
+      <c r="K66" s="90" t="n"/>
     </row>
     <row r="67">
       <c r="G67" s="6" t="n"/>
@@ -5450,7 +5543,7 @@
     <row r="197"/>
     <row r="198"/>
     <row r="199"/>
-    <row r="200" ht="42" customHeight="1" s="121"/>
+    <row r="200" ht="42" customHeight="1" s="120"/>
   </sheetData>
   <mergeCells count="52">
     <mergeCell ref="I32:I33"/>

</xml_diff>

<commit_message>
adding git ignore and other update file
</commit_message>
<xml_diff>
--- a/invoice_gen/result.xlsx
+++ b/invoice_gen/result.xlsx
@@ -25,7 +25,7 @@
     <numFmt numFmtId="164" formatCode="[$USD]\ #,##0.00;[$USD]\ \-#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$-409]dd/mmm/yy;@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="167" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="167" formatCode="##,00.00"/>
   </numFmts>
   <fonts count="47">
     <font>
@@ -386,39 +386,6 @@
         <color rgb="00000000"/>
       </right>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="00000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="00000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="00000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="00000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
     <border/>
     <border>
       <left/>
@@ -453,6 +420,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
@@ -466,7 +466,7 @@
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -768,15 +768,13 @@
     <xf numFmtId="0" fontId="46" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="46" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="46" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="167" fontId="45" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -813,7 +811,7 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="44" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="44" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -825,21 +823,14 @@
     <xf numFmtId="167" fontId="43" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="44" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="44" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="44" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="3" fontId="43" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -852,13 +843,7 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="43" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="43" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="43" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="167" fontId="43" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1396,7 +1381,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:XFD200"/>
+  <dimension ref="A1:XFD202"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
@@ -1558,7 +1543,7 @@
     <row r="13" ht="26.1" customFormat="1" customHeight="1" s="97">
       <c r="A13" s="101" t="inlineStr">
         <is>
-          <t>1.NAME OF COMMODITY AND SPECIFICATION:</t>
+          <t>1.NAME OF COMMODITY AND SPEFOBICATION:</t>
         </is>
       </c>
       <c r="B13" s="101" t="n"/>
@@ -1645,12 +1630,13 @@
       </c>
       <c r="B16" s="107" t="inlineStr">
         <is>
-          <t>YNGY25022</t>
+          <t>GYOJY_M25371/GYOJY_M25374
+YNGY25022/YNGY25028</t>
         </is>
       </c>
       <c r="C16" s="107" t="inlineStr">
         <is>
-          <t>M1243</t>
+          <t>M1243/Nick Dove</t>
         </is>
       </c>
       <c r="D16" s="108" t="inlineStr">
@@ -1659,348 +1645,288 @@
         </is>
       </c>
       <c r="E16" s="109" t="n">
-        <v>10045.4</v>
-      </c>
-      <c r="F16" s="109" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="G16" s="109">
-        <f>F16*E16</f>
+        <v>225927.8</v>
+      </c>
+      <c r="F16" s="109">
+        <f>G16/E16</f>
         <v/>
       </c>
-    </row>
-    <row r="17" ht="30" customFormat="1" customHeight="1" s="48">
-      <c r="A17" s="107" t="n">
-        <v>2</v>
-      </c>
-      <c r="B17" s="107" t="inlineStr">
-        <is>
-          <t>YNGY25028</t>
-        </is>
-      </c>
-      <c r="C17" s="107" t="inlineStr">
-        <is>
-          <t>M1243</t>
-        </is>
-      </c>
+      <c r="G16" s="109" t="n">
+        <v>259081.023</v>
+      </c>
+    </row>
+    <row r="17" ht="36" customFormat="1" customHeight="1" s="48">
+      <c r="A17" s="110" t="inlineStr">
+        <is>
+          <t>TOTAL:</t>
+        </is>
+      </c>
+      <c r="B17" s="111" t="n"/>
+      <c r="C17" s="110" t="n"/>
       <c r="D17" s="110" t="n"/>
-      <c r="E17" s="109" t="n">
-        <v>40074.3</v>
-      </c>
-      <c r="F17" s="109" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="G17" s="109">
-        <f>F17*E17</f>
+      <c r="E17" s="112">
+        <f>SUM(E16:E16)</f>
         <v/>
       </c>
-    </row>
-    <row r="18" ht="30" customFormat="1" customHeight="1" s="48">
-      <c r="A18" s="107" t="n">
-        <v>3</v>
-      </c>
-      <c r="B18" s="107" t="inlineStr">
-        <is>
-          <t>YNGY25028</t>
-        </is>
-      </c>
-      <c r="C18" s="107" t="inlineStr">
-        <is>
-          <t>M1243</t>
-        </is>
-      </c>
-      <c r="D18" s="110" t="n"/>
-      <c r="E18" s="109" t="n">
-        <v>475</v>
-      </c>
-      <c r="F18" s="109" t="n">
-        <v>0.91</v>
-      </c>
-      <c r="G18" s="109">
-        <f>F18*E18</f>
+      <c r="F17" s="110" t="n"/>
+      <c r="G17" s="112">
+        <f>SUM(G16:G16)</f>
         <v/>
       </c>
     </row>
-    <row r="19" ht="30" customFormat="1" customHeight="1" s="48">
-      <c r="A19" s="107" t="n">
-        <v>4</v>
-      </c>
-      <c r="B19" s="107" t="inlineStr">
-        <is>
-          <t>GYOJY_M25371</t>
-        </is>
-      </c>
-      <c r="C19" s="107" t="inlineStr">
-        <is>
-          <t>Nick Dove</t>
-        </is>
-      </c>
-      <c r="D19" s="110" t="n"/>
-      <c r="E19" s="109" t="n">
-        <v>136378.1</v>
-      </c>
-      <c r="F19" s="109" t="n">
-        <v>1.15</v>
-      </c>
-      <c r="G19" s="109">
-        <f>F19*E19</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" ht="30" customFormat="1" customHeight="1" s="48">
-      <c r="A20" s="107" t="n">
-        <v>5</v>
-      </c>
-      <c r="B20" s="107" t="inlineStr">
-        <is>
-          <t>GYOJY_M25371</t>
-        </is>
-      </c>
-      <c r="C20" s="107" t="inlineStr">
-        <is>
-          <t>Nick Dove</t>
-        </is>
-      </c>
-      <c r="D20" s="110" t="n"/>
-      <c r="E20" s="109" t="n">
-        <v>113.7</v>
-      </c>
-      <c r="F20" s="109" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="G20" s="109">
-        <f>F20*E20</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" ht="30" customFormat="1" customHeight="1" s="48">
-      <c r="A21" s="107" t="n">
-        <v>6</v>
-      </c>
-      <c r="B21" s="107" t="inlineStr">
-        <is>
-          <t>GYOJY_M25374</t>
-        </is>
-      </c>
-      <c r="C21" s="107" t="inlineStr">
-        <is>
-          <t>Nick Dove</t>
-        </is>
-      </c>
-      <c r="D21" s="110" t="n"/>
-      <c r="E21" s="109" t="n">
-        <v>38430</v>
-      </c>
-      <c r="F21" s="109" t="n">
-        <v>1.15</v>
-      </c>
-      <c r="G21" s="109">
-        <f>F21*E21</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" ht="30" customFormat="1" customHeight="1" s="48">
-      <c r="A22" s="107" t="n">
-        <v>7</v>
-      </c>
-      <c r="B22" s="107" t="inlineStr">
-        <is>
-          <t>GYOJY_M25374</t>
-        </is>
-      </c>
-      <c r="C22" s="107" t="inlineStr">
-        <is>
-          <t>Nick Dove</t>
-        </is>
-      </c>
-      <c r="D22" s="111" t="n"/>
-      <c r="E22" s="109" t="n">
-        <v>411.3</v>
-      </c>
-      <c r="F22" s="109" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="G22" s="109">
-        <f>F22*E22</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" ht="36" customFormat="1" customHeight="1" s="48">
-      <c r="A23" s="112" t="inlineStr">
-        <is>
-          <t>TOTAL:</t>
-        </is>
-      </c>
-      <c r="B23" s="113" t="n"/>
-      <c r="C23" s="112" t="n"/>
-      <c r="D23" s="112" t="n"/>
-      <c r="E23" s="114">
-        <f>SUM(E16:E22)</f>
-        <v/>
-      </c>
-      <c r="F23" s="112" t="n"/>
-      <c r="G23" s="114">
-        <f>SUM(G16:G22)</f>
-        <v/>
+    <row r="18" ht="28.9" customFormat="1" customHeight="1" s="48">
+      <c r="A18" s="65" t="inlineStr">
+        <is>
+          <t>FOB:</t>
+        </is>
+      </c>
+      <c r="B18" s="66" t="inlineStr">
+        <is>
+          <t>BAVET</t>
+        </is>
+      </c>
+      <c r="D18" s="66" t="n"/>
+      <c r="E18" s="67" t="n"/>
+      <c r="F18" s="67" t="n"/>
+      <c r="G18" s="67" t="n"/>
+    </row>
+    <row r="19" ht="28.9" customFormat="1" customHeight="1" s="48">
+      <c r="A19" s="67" t="inlineStr">
+        <is>
+          <t>Term of Payment: 100% TT after shipment</t>
+        </is>
+      </c>
+      <c r="B19" s="67" t="n"/>
+      <c r="C19" s="67" t="n"/>
+      <c r="D19" s="67" t="n"/>
+      <c r="E19" s="67" t="n"/>
+      <c r="F19" s="67" t="n"/>
+      <c r="G19" s="67" t="n"/>
+    </row>
+    <row r="20" ht="62.1" customFormat="1" customHeight="1" s="48">
+      <c r="A20" s="67" t="inlineStr">
+        <is>
+          <t>Transaction method: FOB(USD)</t>
+        </is>
+      </c>
+      <c r="B20" s="67" t="n"/>
+      <c r="C20" s="67" t="n"/>
+      <c r="D20" s="67" t="n"/>
+      <c r="E20" s="67" t="n"/>
+      <c r="F20" s="67" t="n"/>
+      <c r="G20" s="67" t="n"/>
+    </row>
+    <row r="21" ht="44.1" customFormat="1" customHeight="1" s="48">
+      <c r="A21" s="67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beneficiary bank information: </t>
+        </is>
+      </c>
+      <c r="B21" s="67" t="n"/>
+      <c r="C21" s="67" t="n"/>
+      <c r="D21" s="67" t="n"/>
+      <c r="E21" s="67" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
+        </is>
+      </c>
+      <c r="F21" s="67" t="n"/>
+      <c r="G21" s="67" t="n"/>
+    </row>
+    <row r="22" ht="62.1" customFormat="1" customHeight="1" s="48">
+      <c r="A22" s="67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beneficiary Bank' s Name: </t>
+        </is>
+      </c>
+      <c r="B22" s="67" t="n"/>
+      <c r="C22" s="67" t="n"/>
+      <c r="D22" s="67" t="n"/>
+      <c r="E22" s="73" t="inlineStr">
+        <is>
+          <t>BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH /BANK OF CHINA PHNOM PENH BRANCH</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" ht="44.1" customFormat="1" customHeight="1" s="48">
+      <c r="A23" s="67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bank Address:  </t>
+        </is>
+      </c>
+      <c r="B23" s="67" t="n"/>
+      <c r="C23" s="67" t="n"/>
+      <c r="D23" s="67" t="n"/>
+      <c r="E23" s="73" t="inlineStr">
+        <is>
+          <t>1st AND 2nd FLOOR,CANADIA TOWER,No.315 ANDDUONG ST.,PHNOM PEMH,CAMBODIA.</t>
+        </is>
       </c>
     </row>
     <row r="24" ht="28.9" customFormat="1" customHeight="1" s="48">
-      <c r="A24" s="65" t="inlineStr">
-        <is>
-          <t>DAP:</t>
-        </is>
-      </c>
-      <c r="B24" s="66" t="inlineStr">
-        <is>
-          <t>BINH DUONG</t>
-        </is>
-      </c>
-      <c r="D24" s="66" t="n"/>
-      <c r="E24" s="67" t="n"/>
-      <c r="F24" s="67" t="n"/>
-      <c r="G24" s="67" t="n"/>
+      <c r="A24" s="67" t="inlineStr">
+        <is>
+          <t>Bank account :</t>
+        </is>
+      </c>
+      <c r="B24" s="67" t="n"/>
+      <c r="C24" s="67" t="n"/>
+      <c r="D24" s="67" t="n"/>
+      <c r="E24" s="74" t="inlineStr">
+        <is>
+          <t>100001100764430</t>
+        </is>
+      </c>
     </row>
     <row r="25" ht="28.9" customFormat="1" customHeight="1" s="43">
       <c r="A25" s="67" t="inlineStr">
         <is>
-          <t>Term of Payment: 100% TT after shipment</t>
+          <t>SWIFT CODE  ：</t>
         </is>
       </c>
       <c r="B25" s="67" t="n"/>
       <c r="C25" s="67" t="n"/>
       <c r="D25" s="67" t="n"/>
-      <c r="E25" s="67" t="n"/>
+      <c r="E25" s="67" t="inlineStr">
+        <is>
+          <t>BKCHKHPPXXX</t>
+        </is>
+      </c>
       <c r="F25" s="67" t="n"/>
       <c r="G25" s="67" t="n"/>
     </row>
     <row r="26" ht="57" customFormat="1" customHeight="1" s="43">
-      <c r="A26" s="67" t="inlineStr">
-        <is>
-          <t>Transaction method: DAP(USD)</t>
-        </is>
-      </c>
+      <c r="A26" s="67" t="n"/>
       <c r="B26" s="67" t="n"/>
       <c r="C26" s="67" t="n"/>
       <c r="D26" s="67" t="n"/>
       <c r="E26" s="67" t="n"/>
       <c r="F26" s="67" t="n"/>
       <c r="G26" s="67" t="n"/>
-    </row>
-    <row r="27" ht="39" customFormat="1" customHeight="1" s="115">
-      <c r="A27" s="67" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Beneficiary bank information: </t>
-        </is>
-      </c>
-      <c r="B27" s="67" t="n"/>
-      <c r="C27" s="67" t="n"/>
-      <c r="D27" s="67" t="n"/>
-      <c r="E27" s="67" t="inlineStr">
+      <c r="H26" s="67" t="n"/>
+    </row>
+    <row r="27" ht="39" customFormat="1" customHeight="1" s="113">
+      <c r="B27" s="68" t="inlineStr">
+        <is>
+          <t>The Buyer:</t>
+        </is>
+      </c>
+      <c r="F27" s="68" t="inlineStr">
+        <is>
+          <t>The Seller:</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="57" customFormat="1" customHeight="1" s="113">
+      <c r="A28" s="75" t="inlineStr">
+        <is>
+          <t>MOTO INNOVATION VIETNAM LIMITED COMPANY</t>
+        </is>
+      </c>
+      <c r="D28" s="75" t="n"/>
+      <c r="E28" s="75" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
         </is>
       </c>
-      <c r="F27" s="67" t="n"/>
-      <c r="G27" s="67" t="n"/>
-    </row>
-    <row r="28" ht="62.1" customFormat="1" customHeight="1" s="115">
-      <c r="A28" s="67" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Beneficiary Bank' s Name: </t>
-        </is>
-      </c>
-      <c r="B28" s="67" t="n"/>
-      <c r="C28" s="67" t="n"/>
-      <c r="D28" s="67" t="n"/>
-      <c r="E28" s="73" t="inlineStr">
-        <is>
-          <t>BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH /BANK OF CHINA PHNOM PENH BRANCH</t>
-        </is>
-      </c>
-    </row>
-    <row r="29" ht="44.1" customFormat="1" customHeight="1" s="115">
-      <c r="A29" s="67" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Bank Address:  </t>
-        </is>
-      </c>
-      <c r="B29" s="67" t="n"/>
-      <c r="C29" s="67" t="n"/>
-      <c r="D29" s="67" t="n"/>
-      <c r="E29" s="73" t="inlineStr">
-        <is>
-          <t>1st AND 2nd FLOOR,CANADIA TOWER,No.315 ANDDUONG ST.,PHNOM PEMH,CAMBODIA.</t>
-        </is>
-      </c>
-    </row>
-    <row r="30" ht="28.9" customFormat="1" customHeight="1" s="115">
-      <c r="A30" s="67" t="inlineStr">
-        <is>
-          <t>Bank account :</t>
-        </is>
-      </c>
-      <c r="B30" s="67" t="n"/>
-      <c r="C30" s="67" t="n"/>
-      <c r="D30" s="67" t="n"/>
-      <c r="E30" s="74" t="inlineStr">
-        <is>
-          <t>100001100764430</t>
-        </is>
-      </c>
-    </row>
-    <row r="31" ht="39" customFormat="1" customHeight="1" s="115">
-      <c r="A31" s="67" t="inlineStr">
-        <is>
-          <t>SWIFT CODE  ：</t>
-        </is>
-      </c>
-      <c r="B31" s="67" t="n"/>
-      <c r="C31" s="67" t="n"/>
-      <c r="D31" s="67" t="n"/>
-      <c r="E31" s="67" t="inlineStr">
-        <is>
-          <t>BKCHKHPPXXX</t>
-        </is>
-      </c>
-      <c r="F31" s="67" t="n"/>
-      <c r="G31" s="67" t="n"/>
-    </row>
-    <row r="32" ht="39" customFormat="1" customHeight="1" s="116">
-      <c r="A32" s="67" t="n"/>
-      <c r="B32" s="67" t="n"/>
-      <c r="C32" s="67" t="n"/>
-      <c r="D32" s="67" t="n"/>
-      <c r="E32" s="67" t="n"/>
-      <c r="F32" s="67" t="n"/>
-      <c r="G32" s="67" t="n"/>
-      <c r="H32" s="67" t="n"/>
-    </row>
-    <row r="33" ht="39" customFormat="1" customHeight="1" s="116">
-      <c r="B33" s="68" t="inlineStr">
-        <is>
-          <t>The Buyer:</t>
-        </is>
-      </c>
-      <c r="F33" s="68" t="inlineStr">
-        <is>
-          <t>The Seller:</t>
-        </is>
-      </c>
-    </row>
-    <row r="34" ht="57" customFormat="1" customHeight="1" s="116">
-      <c r="A34" s="75" t="inlineStr">
-        <is>
-          <t>MOTO INNOVATION VIETNAM LIMITED COMPANY</t>
-        </is>
-      </c>
-      <c r="D34" s="75" t="n"/>
-      <c r="E34" s="75" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
-        </is>
-      </c>
-    </row>
-    <row r="35" ht="39" customFormat="1" customHeight="1" s="116">
+    </row>
+    <row r="29" ht="39" customFormat="1" customHeight="1" s="113">
+      <c r="A29" s="54" t="n"/>
+      <c r="B29" s="54" t="n"/>
+      <c r="C29" s="54" t="n"/>
+      <c r="D29" s="54" t="n"/>
+      <c r="E29" s="54" t="n"/>
+      <c r="F29" s="54" t="n"/>
+      <c r="G29" s="54" t="n"/>
+      <c r="H29" s="54" t="n"/>
+      <c r="I29" s="54" t="n"/>
+      <c r="J29" s="54" t="n"/>
+      <c r="K29" s="54" t="n"/>
+      <c r="L29" s="54" t="n"/>
+      <c r="M29" s="54" t="n"/>
+      <c r="XFD29" s="54" t="n"/>
+    </row>
+    <row r="30" ht="39" customFormat="1" customHeight="1" s="113">
+      <c r="A30" s="54" t="n"/>
+      <c r="B30" s="54" t="n"/>
+      <c r="C30" s="54" t="n"/>
+      <c r="D30" s="54" t="n"/>
+      <c r="E30" s="54" t="n"/>
+      <c r="F30" s="54" t="n"/>
+      <c r="G30" s="54" t="n"/>
+      <c r="H30" s="54" t="n"/>
+      <c r="I30" s="54" t="n"/>
+      <c r="J30" s="54" t="n"/>
+      <c r="K30" s="54" t="n"/>
+      <c r="L30" s="54" t="n"/>
+      <c r="M30" s="54" t="n"/>
+      <c r="XFD30" s="54" t="n"/>
+    </row>
+    <row r="31" ht="39" customFormat="1" customHeight="1" s="113">
+      <c r="A31" s="54" t="n"/>
+      <c r="B31" s="54" t="n"/>
+      <c r="C31" s="54" t="n"/>
+      <c r="D31" s="54" t="n"/>
+      <c r="E31" s="54" t="n"/>
+      <c r="F31" s="54" t="n"/>
+      <c r="G31" s="54" t="n"/>
+      <c r="H31" s="54" t="n"/>
+      <c r="I31" s="54" t="n"/>
+      <c r="J31" s="54" t="n"/>
+      <c r="K31" s="54" t="n"/>
+      <c r="L31" s="54" t="n"/>
+      <c r="M31" s="54" t="n"/>
+      <c r="XFD31" s="54" t="n"/>
+    </row>
+    <row r="32" ht="39" customFormat="1" customHeight="1" s="114">
+      <c r="A32" s="54" t="n"/>
+      <c r="B32" s="54" t="n"/>
+      <c r="C32" s="54" t="n"/>
+      <c r="D32" s="54" t="n"/>
+      <c r="E32" s="54" t="n"/>
+      <c r="F32" s="54" t="n"/>
+      <c r="G32" s="54" t="n"/>
+      <c r="H32" s="54" t="n"/>
+      <c r="I32" s="54" t="n"/>
+      <c r="J32" s="54" t="n"/>
+      <c r="K32" s="54" t="n"/>
+      <c r="L32" s="54" t="n"/>
+      <c r="M32" s="54" t="n"/>
+      <c r="XFD32" s="54" t="n"/>
+    </row>
+    <row r="33" ht="39" customFormat="1" customHeight="1" s="114">
+      <c r="A33" s="54" t="n"/>
+      <c r="B33" s="54" t="n"/>
+      <c r="C33" s="54" t="n"/>
+      <c r="D33" s="54" t="n"/>
+      <c r="E33" s="54" t="n"/>
+      <c r="F33" s="54" t="n"/>
+      <c r="G33" s="54" t="n"/>
+      <c r="H33" s="54" t="n"/>
+      <c r="I33" s="54" t="n"/>
+      <c r="J33" s="54" t="n"/>
+      <c r="K33" s="54" t="n"/>
+      <c r="L33" s="54" t="n"/>
+      <c r="M33" s="54" t="n"/>
+      <c r="XFD33" s="54" t="n"/>
+    </row>
+    <row r="34" ht="39" customFormat="1" customHeight="1" s="114">
+      <c r="A34" s="54" t="n"/>
+      <c r="B34" s="54" t="n"/>
+      <c r="C34" s="54" t="n"/>
+      <c r="D34" s="54" t="n"/>
+      <c r="E34" s="54" t="n"/>
+      <c r="F34" s="54" t="n"/>
+      <c r="G34" s="54" t="n"/>
+      <c r="H34" s="54" t="n"/>
+      <c r="I34" s="54" t="n"/>
+      <c r="J34" s="54" t="n"/>
+      <c r="K34" s="54" t="n"/>
+      <c r="L34" s="54" t="n"/>
+      <c r="M34" s="54" t="n"/>
+      <c r="XFD34" s="54" t="n"/>
+    </row>
+    <row r="35" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A35" s="54" t="n"/>
       <c r="B35" s="54" t="n"/>
       <c r="C35" s="54" t="n"/>
@@ -2016,7 +1942,7 @@
       <c r="M35" s="54" t="n"/>
       <c r="XFD35" s="54" t="n"/>
     </row>
-    <row r="36" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="36" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A36" s="54" t="n"/>
       <c r="B36" s="54" t="n"/>
       <c r="C36" s="54" t="n"/>
@@ -2032,7 +1958,7 @@
       <c r="M36" s="54" t="n"/>
       <c r="XFD36" s="54" t="n"/>
     </row>
-    <row r="37" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="37" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A37" s="54" t="n"/>
       <c r="B37" s="54" t="n"/>
       <c r="C37" s="54" t="n"/>
@@ -2048,7 +1974,7 @@
       <c r="M37" s="54" t="n"/>
       <c r="XFD37" s="54" t="n"/>
     </row>
-    <row r="38" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="38" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A38" s="54" t="n"/>
       <c r="B38" s="54" t="n"/>
       <c r="C38" s="54" t="n"/>
@@ -2064,7 +1990,7 @@
       <c r="M38" s="54" t="n"/>
       <c r="XFD38" s="54" t="n"/>
     </row>
-    <row r="39" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="39" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A39" s="54" t="n"/>
       <c r="B39" s="54" t="n"/>
       <c r="C39" s="54" t="n"/>
@@ -2080,7 +2006,7 @@
       <c r="M39" s="54" t="n"/>
       <c r="XFD39" s="54" t="n"/>
     </row>
-    <row r="40" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="40" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A40" s="54" t="n"/>
       <c r="B40" s="54" t="n"/>
       <c r="C40" s="54" t="n"/>
@@ -2096,7 +2022,7 @@
       <c r="M40" s="54" t="n"/>
       <c r="XFD40" s="54" t="n"/>
     </row>
-    <row r="41" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="41" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A41" s="54" t="n"/>
       <c r="B41" s="54" t="n"/>
       <c r="C41" s="54" t="n"/>
@@ -2112,7 +2038,7 @@
       <c r="M41" s="54" t="n"/>
       <c r="XFD41" s="54" t="n"/>
     </row>
-    <row r="42" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="42" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A42" s="54" t="n"/>
       <c r="B42" s="54" t="n"/>
       <c r="C42" s="54" t="n"/>
@@ -2128,7 +2054,7 @@
       <c r="M42" s="54" t="n"/>
       <c r="XFD42" s="54" t="n"/>
     </row>
-    <row r="43" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="43" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A43" s="54" t="n"/>
       <c r="B43" s="54" t="n"/>
       <c r="C43" s="54" t="n"/>
@@ -2144,7 +2070,7 @@
       <c r="M43" s="54" t="n"/>
       <c r="XFD43" s="54" t="n"/>
     </row>
-    <row r="44" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="44" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A44" s="54" t="n"/>
       <c r="B44" s="54" t="n"/>
       <c r="C44" s="54" t="n"/>
@@ -2160,7 +2086,7 @@
       <c r="M44" s="54" t="n"/>
       <c r="XFD44" s="54" t="n"/>
     </row>
-    <row r="45" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="45" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A45" s="54" t="n"/>
       <c r="B45" s="54" t="n"/>
       <c r="C45" s="54" t="n"/>
@@ -2176,7 +2102,7 @@
       <c r="M45" s="54" t="n"/>
       <c r="XFD45" s="54" t="n"/>
     </row>
-    <row r="46" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="46" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A46" s="54" t="n"/>
       <c r="B46" s="54" t="n"/>
       <c r="C46" s="54" t="n"/>
@@ -2192,7 +2118,7 @@
       <c r="M46" s="54" t="n"/>
       <c r="XFD46" s="54" t="n"/>
     </row>
-    <row r="47" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="47" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A47" s="54" t="n"/>
       <c r="B47" s="54" t="n"/>
       <c r="C47" s="54" t="n"/>
@@ -2208,7 +2134,7 @@
       <c r="M47" s="54" t="n"/>
       <c r="XFD47" s="54" t="n"/>
     </row>
-    <row r="48" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="48" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A48" s="54" t="n"/>
       <c r="B48" s="54" t="n"/>
       <c r="C48" s="54" t="n"/>
@@ -2224,7 +2150,7 @@
       <c r="M48" s="54" t="n"/>
       <c r="XFD48" s="54" t="n"/>
     </row>
-    <row r="49" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="49" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A49" s="54" t="n"/>
       <c r="B49" s="54" t="n"/>
       <c r="C49" s="54" t="n"/>
@@ -2240,7 +2166,7 @@
       <c r="M49" s="54" t="n"/>
       <c r="XFD49" s="54" t="n"/>
     </row>
-    <row r="50" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="50" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A50" s="54" t="n"/>
       <c r="B50" s="54" t="n"/>
       <c r="C50" s="54" t="n"/>
@@ -2256,7 +2182,7 @@
       <c r="M50" s="54" t="n"/>
       <c r="XFD50" s="54" t="n"/>
     </row>
-    <row r="51" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="51" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A51" s="54" t="n"/>
       <c r="B51" s="54" t="n"/>
       <c r="C51" s="54" t="n"/>
@@ -2272,7 +2198,7 @@
       <c r="M51" s="54" t="n"/>
       <c r="XFD51" s="54" t="n"/>
     </row>
-    <row r="52" ht="39" customFormat="1" customHeight="1" s="117">
+    <row r="52" ht="39" customFormat="1" customHeight="1" s="115">
       <c r="A52" s="54" t="n"/>
       <c r="B52" s="54" t="n"/>
       <c r="C52" s="54" t="n"/>
@@ -2288,7 +2214,7 @@
       <c r="M52" s="54" t="n"/>
       <c r="XFD52" s="54" t="n"/>
     </row>
-    <row r="53" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="53" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A53" s="54" t="n"/>
       <c r="B53" s="54" t="n"/>
       <c r="C53" s="54" t="n"/>
@@ -2304,7 +2230,7 @@
       <c r="M53" s="54" t="n"/>
       <c r="XFD53" s="54" t="n"/>
     </row>
-    <row r="54" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="54" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A54" s="54" t="n"/>
       <c r="B54" s="54" t="n"/>
       <c r="C54" s="54" t="n"/>
@@ -2316,11 +2242,9 @@
       <c r="I54" s="54" t="n"/>
       <c r="J54" s="54" t="n"/>
       <c r="K54" s="54" t="n"/>
-      <c r="L54" s="54" t="n"/>
-      <c r="M54" s="54" t="n"/>
       <c r="XFD54" s="54" t="n"/>
     </row>
-    <row r="55" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="55" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A55" s="54" t="n"/>
       <c r="B55" s="54" t="n"/>
       <c r="C55" s="54" t="n"/>
@@ -2336,7 +2260,7 @@
       <c r="M55" s="54" t="n"/>
       <c r="XFD55" s="54" t="n"/>
     </row>
-    <row r="56" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="56" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A56" s="54" t="n"/>
       <c r="B56" s="54" t="n"/>
       <c r="C56" s="54" t="n"/>
@@ -2352,7 +2276,7 @@
       <c r="M56" s="54" t="n"/>
       <c r="XFD56" s="54" t="n"/>
     </row>
-    <row r="57" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="57" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A57" s="54" t="n"/>
       <c r="B57" s="54" t="n"/>
       <c r="C57" s="54" t="n"/>
@@ -2368,7 +2292,7 @@
       <c r="M57" s="54" t="n"/>
       <c r="XFD57" s="54" t="n"/>
     </row>
-    <row r="58" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="58" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A58" s="54" t="n"/>
       <c r="B58" s="54" t="n"/>
       <c r="C58" s="54" t="n"/>
@@ -2384,7 +2308,7 @@
       <c r="M58" s="54" t="n"/>
       <c r="XFD58" s="54" t="n"/>
     </row>
-    <row r="59" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="59" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A59" s="54" t="n"/>
       <c r="B59" s="54" t="n"/>
       <c r="C59" s="54" t="n"/>
@@ -2400,7 +2324,7 @@
       <c r="M59" s="54" t="n"/>
       <c r="XFD59" s="54" t="n"/>
     </row>
-    <row r="60" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="60" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A60" s="54" t="n"/>
       <c r="B60" s="54" t="n"/>
       <c r="C60" s="54" t="n"/>
@@ -2412,9 +2336,11 @@
       <c r="I60" s="54" t="n"/>
       <c r="J60" s="54" t="n"/>
       <c r="K60" s="54" t="n"/>
+      <c r="L60" s="54" t="n"/>
+      <c r="M60" s="54" t="n"/>
       <c r="XFD60" s="54" t="n"/>
     </row>
-    <row r="61" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="61" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A61" s="54" t="n"/>
       <c r="B61" s="54" t="n"/>
       <c r="C61" s="54" t="n"/>
@@ -2430,7 +2356,7 @@
       <c r="M61" s="54" t="n"/>
       <c r="XFD61" s="54" t="n"/>
     </row>
-    <row r="62" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="62" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A62" s="54" t="n"/>
       <c r="B62" s="54" t="n"/>
       <c r="C62" s="54" t="n"/>
@@ -2438,15 +2364,12 @@
       <c r="E62" s="54" t="n"/>
       <c r="F62" s="54" t="n"/>
       <c r="G62" s="54" t="n"/>
-      <c r="H62" s="54" t="n"/>
-      <c r="I62" s="54" t="n"/>
       <c r="J62" s="54" t="n"/>
       <c r="K62" s="54" t="n"/>
       <c r="L62" s="54" t="n"/>
-      <c r="M62" s="54" t="n"/>
       <c r="XFD62" s="54" t="n"/>
     </row>
-    <row r="63" customFormat="1" s="118">
+    <row r="63" customFormat="1" s="116">
       <c r="A63" s="54" t="n"/>
       <c r="B63" s="54" t="n"/>
       <c r="C63" s="54" t="n"/>
@@ -2454,15 +2377,12 @@
       <c r="E63" s="54" t="n"/>
       <c r="F63" s="54" t="n"/>
       <c r="G63" s="54" t="n"/>
-      <c r="H63" s="54" t="n"/>
-      <c r="I63" s="54" t="n"/>
       <c r="J63" s="54" t="n"/>
       <c r="K63" s="54" t="n"/>
       <c r="L63" s="54" t="n"/>
-      <c r="M63" s="54" t="n"/>
       <c r="XFD63" s="54" t="n"/>
     </row>
-    <row r="64" customFormat="1" s="118">
+    <row r="64" customFormat="1" s="116">
       <c r="A64" s="54" t="n"/>
       <c r="B64" s="54" t="n"/>
       <c r="C64" s="54" t="n"/>
@@ -2470,15 +2390,12 @@
       <c r="E64" s="54" t="n"/>
       <c r="F64" s="54" t="n"/>
       <c r="G64" s="54" t="n"/>
-      <c r="H64" s="54" t="n"/>
-      <c r="I64" s="54" t="n"/>
       <c r="J64" s="54" t="n"/>
       <c r="K64" s="54" t="n"/>
       <c r="L64" s="54" t="n"/>
-      <c r="M64" s="54" t="n"/>
       <c r="XFD64" s="54" t="n"/>
     </row>
-    <row r="65" customFormat="1" s="118">
+    <row r="65" customFormat="1" s="116">
       <c r="A65" s="54" t="n"/>
       <c r="B65" s="54" t="n"/>
       <c r="C65" s="54" t="n"/>
@@ -2494,7 +2411,7 @@
       <c r="M65" s="54" t="n"/>
       <c r="XFD65" s="54" t="n"/>
     </row>
-    <row r="66" customFormat="1" s="118">
+    <row r="66" customFormat="1" s="116">
       <c r="A66" s="54" t="n"/>
       <c r="B66" s="54" t="n"/>
       <c r="C66" s="54" t="n"/>
@@ -2510,7 +2427,7 @@
       <c r="M66" s="54" t="n"/>
       <c r="XFD66" s="54" t="n"/>
     </row>
-    <row r="67" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="67" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A67" s="54" t="n"/>
       <c r="B67" s="54" t="n"/>
       <c r="C67" s="54" t="n"/>
@@ -2526,7 +2443,7 @@
       <c r="M67" s="54" t="n"/>
       <c r="XFD67" s="54" t="n"/>
     </row>
-    <row r="68" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="68" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A68" s="54" t="n"/>
       <c r="B68" s="54" t="n"/>
       <c r="C68" s="54" t="n"/>
@@ -2534,12 +2451,15 @@
       <c r="E68" s="54" t="n"/>
       <c r="F68" s="54" t="n"/>
       <c r="G68" s="54" t="n"/>
+      <c r="H68" s="54" t="n"/>
+      <c r="I68" s="54" t="n"/>
       <c r="J68" s="54" t="n"/>
       <c r="K68" s="54" t="n"/>
       <c r="L68" s="54" t="n"/>
+      <c r="M68" s="54" t="n"/>
       <c r="XFD68" s="54" t="n"/>
     </row>
-    <row r="69" ht="39" customFormat="1" customHeight="1" s="116">
+    <row r="69" ht="39" customFormat="1" customHeight="1" s="114">
       <c r="A69" s="54" t="n"/>
       <c r="B69" s="54" t="n"/>
       <c r="C69" s="54" t="n"/>
@@ -2552,7 +2472,7 @@
       <c r="L69" s="54" t="n"/>
       <c r="XFD69" s="54" t="n"/>
     </row>
-    <row r="70" customFormat="1" s="118">
+    <row r="70" customFormat="1" s="116">
       <c r="A70" s="54" t="n"/>
       <c r="B70" s="54" t="n"/>
       <c r="C70" s="54" t="n"/>
@@ -2565,7 +2485,7 @@
       <c r="L70" s="54" t="n"/>
       <c r="XFD70" s="54" t="n"/>
     </row>
-    <row r="71" customFormat="1" s="118">
+    <row r="71" customFormat="1" s="116">
       <c r="A71" s="54" t="n"/>
       <c r="B71" s="54" t="n"/>
       <c r="C71" s="54" t="n"/>
@@ -2573,15 +2493,12 @@
       <c r="E71" s="54" t="n"/>
       <c r="F71" s="54" t="n"/>
       <c r="G71" s="54" t="n"/>
-      <c r="H71" s="54" t="n"/>
-      <c r="I71" s="54" t="n"/>
       <c r="J71" s="54" t="n"/>
       <c r="K71" s="54" t="n"/>
       <c r="L71" s="54" t="n"/>
-      <c r="M71" s="54" t="n"/>
       <c r="XFD71" s="54" t="n"/>
     </row>
-    <row r="72" customFormat="1" s="118">
+    <row r="72" customFormat="1" s="116">
       <c r="A72" s="54" t="n"/>
       <c r="B72" s="54" t="n"/>
       <c r="C72" s="54" t="n"/>
@@ -2597,7 +2514,7 @@
       <c r="M72" s="54" t="n"/>
       <c r="XFD72" s="54" t="n"/>
     </row>
-    <row r="73" customFormat="1" s="118">
+    <row r="73" customFormat="1" s="116">
       <c r="A73" s="54" t="n"/>
       <c r="B73" s="54" t="n"/>
       <c r="C73" s="54" t="n"/>
@@ -2613,7 +2530,7 @@
       <c r="M73" s="54" t="n"/>
       <c r="XFD73" s="54" t="n"/>
     </row>
-    <row r="74" customFormat="1" s="118">
+    <row r="74" customFormat="1" s="116">
       <c r="A74" s="54" t="n"/>
       <c r="B74" s="54" t="n"/>
       <c r="C74" s="54" t="n"/>
@@ -2629,7 +2546,7 @@
       <c r="M74" s="54" t="n"/>
       <c r="XFD74" s="54" t="n"/>
     </row>
-    <row r="75" ht="31.5" customFormat="1" customHeight="1" s="119">
+    <row r="75" ht="31.5" customFormat="1" customHeight="1" s="117">
       <c r="A75" s="54" t="n"/>
       <c r="B75" s="54" t="n"/>
       <c r="C75" s="54" t="n"/>
@@ -2637,12 +2554,15 @@
       <c r="E75" s="54" t="n"/>
       <c r="F75" s="54" t="n"/>
       <c r="G75" s="54" t="n"/>
+      <c r="H75" s="54" t="n"/>
+      <c r="I75" s="54" t="n"/>
       <c r="J75" s="54" t="n"/>
       <c r="K75" s="54" t="n"/>
       <c r="L75" s="54" t="n"/>
+      <c r="M75" s="54" t="n"/>
       <c r="XFD75" s="54" t="n"/>
     </row>
-    <row r="76" customFormat="1" s="118">
+    <row r="76" customFormat="1" s="116">
       <c r="A76" s="54" t="n"/>
       <c r="B76" s="54" t="n"/>
       <c r="C76" s="54" t="n"/>
@@ -2650,9 +2570,12 @@
       <c r="E76" s="54" t="n"/>
       <c r="F76" s="54" t="n"/>
       <c r="G76" s="54" t="n"/>
+      <c r="H76" s="54" t="n"/>
+      <c r="I76" s="54" t="n"/>
       <c r="J76" s="54" t="n"/>
       <c r="K76" s="54" t="n"/>
       <c r="L76" s="54" t="n"/>
+      <c r="M76" s="54" t="n"/>
       <c r="XFD76" s="54" t="n"/>
     </row>
     <row r="77">
@@ -2663,9 +2586,8 @@
       <c r="E77" s="54" t="n"/>
       <c r="F77" s="54" t="n"/>
       <c r="G77" s="54" t="n"/>
-      <c r="J77" s="54" t="n"/>
-      <c r="K77" s="54" t="n"/>
-      <c r="L77" s="54" t="n"/>
+      <c r="H77" s="54" t="n"/>
+      <c r="I77" s="54" t="n"/>
       <c r="XFD77" s="54" t="n"/>
     </row>
     <row r="78">
@@ -2684,98 +2606,12 @@
       <c r="M78" s="54" t="n"/>
       <c r="XFD78" s="54" t="n"/>
     </row>
-    <row r="79">
-      <c r="A79" s="54" t="n"/>
-      <c r="B79" s="54" t="n"/>
-      <c r="C79" s="54" t="n"/>
-      <c r="D79" s="54" t="n"/>
-      <c r="E79" s="54" t="n"/>
-      <c r="F79" s="54" t="n"/>
-      <c r="G79" s="54" t="n"/>
-      <c r="H79" s="54" t="n"/>
-      <c r="I79" s="54" t="n"/>
-      <c r="J79" s="54" t="n"/>
-      <c r="K79" s="54" t="n"/>
-      <c r="L79" s="54" t="n"/>
-      <c r="M79" s="54" t="n"/>
-      <c r="XFD79" s="54" t="n"/>
-    </row>
-    <row r="80">
-      <c r="A80" s="54" t="n"/>
-      <c r="B80" s="54" t="n"/>
-      <c r="C80" s="54" t="n"/>
-      <c r="D80" s="54" t="n"/>
-      <c r="E80" s="54" t="n"/>
-      <c r="F80" s="54" t="n"/>
-      <c r="G80" s="54" t="n"/>
-      <c r="H80" s="54" t="n"/>
-      <c r="I80" s="54" t="n"/>
-      <c r="J80" s="54" t="n"/>
-      <c r="K80" s="54" t="n"/>
-      <c r="L80" s="54" t="n"/>
-      <c r="M80" s="54" t="n"/>
-      <c r="XFD80" s="54" t="n"/>
-    </row>
-    <row r="81" customFormat="1" s="54">
-      <c r="A81" s="54" t="n"/>
-      <c r="B81" s="54" t="n"/>
-      <c r="C81" s="54" t="n"/>
-      <c r="D81" s="54" t="n"/>
-      <c r="E81" s="54" t="n"/>
-      <c r="F81" s="54" t="n"/>
-      <c r="G81" s="54" t="n"/>
-      <c r="H81" s="54" t="n"/>
-      <c r="I81" s="54" t="n"/>
-      <c r="J81" s="54" t="n"/>
-      <c r="K81" s="54" t="n"/>
-      <c r="L81" s="54" t="n"/>
-      <c r="M81" s="54" t="n"/>
-      <c r="XFD81" s="54" t="n"/>
-    </row>
-    <row r="82" customFormat="1" s="54">
-      <c r="A82" s="54" t="n"/>
-      <c r="B82" s="54" t="n"/>
-      <c r="C82" s="54" t="n"/>
-      <c r="D82" s="54" t="n"/>
-      <c r="E82" s="54" t="n"/>
-      <c r="F82" s="54" t="n"/>
-      <c r="G82" s="54" t="n"/>
-      <c r="H82" s="54" t="n"/>
-      <c r="I82" s="54" t="n"/>
-      <c r="J82" s="54" t="n"/>
-      <c r="K82" s="54" t="n"/>
-      <c r="L82" s="54" t="n"/>
-      <c r="M82" s="54" t="n"/>
-      <c r="XFD82" s="54" t="n"/>
-    </row>
-    <row r="83" customFormat="1" s="54">
-      <c r="A83" s="54" t="n"/>
-      <c r="B83" s="54" t="n"/>
-      <c r="C83" s="54" t="n"/>
-      <c r="D83" s="54" t="n"/>
-      <c r="E83" s="54" t="n"/>
-      <c r="F83" s="54" t="n"/>
-      <c r="G83" s="54" t="n"/>
-      <c r="H83" s="54" t="n"/>
-      <c r="I83" s="54" t="n"/>
-      <c r="XFD83" s="54" t="n"/>
-    </row>
-    <row r="84" customFormat="1" s="54">
-      <c r="A84" s="54" t="n"/>
-      <c r="B84" s="54" t="n"/>
-      <c r="C84" s="54" t="n"/>
-      <c r="D84" s="54" t="n"/>
-      <c r="E84" s="54" t="n"/>
-      <c r="F84" s="54" t="n"/>
-      <c r="G84" s="54" t="n"/>
-      <c r="H84" s="54" t="n"/>
-      <c r="I84" s="54" t="n"/>
-      <c r="J84" s="54" t="n"/>
-      <c r="K84" s="54" t="n"/>
-      <c r="L84" s="54" t="n"/>
-      <c r="M84" s="54" t="n"/>
-      <c r="XFD84" s="54" t="n"/>
-    </row>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81" customFormat="1" s="54"/>
+    <row r="82" customFormat="1" s="54"/>
+    <row r="83" customFormat="1" s="54"/>
+    <row r="84" customFormat="1" s="54"/>
     <row r="85" customFormat="1" s="54"/>
     <row r="86"/>
     <row r="87"/>
@@ -2892,20 +2728,23 @@
     <row r="198"/>
     <row r="199"/>
     <row r="200"/>
+    <row r="201"/>
+    <row r="202"/>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="A28:C28"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E24:G24"/>
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E23:G23"/>
     <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D16:D22"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="E21:G21"/>
     <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E20:G20"/>
   </mergeCells>
   <pageMargins left="1.0625" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" scale="36"/>
@@ -2919,7 +2758,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N200"/>
+  <dimension ref="A1:P206"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
@@ -2941,61 +2780,61 @@
     <col width="7.140625" customWidth="1" style="90" min="13" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="38.25" customHeight="1" s="120">
+    <row r="1" ht="38.25" customHeight="1" s="118">
       <c r="A1" s="79" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="24" customHeight="1" s="120">
+    <row r="2" ht="24" customHeight="1" s="118">
       <c r="A2" s="80" t="inlineStr">
         <is>
           <t xml:space="preserve"> XIN BAVET SEZ, Road No. 316A, Trapeang Bon and  Prey Kokir  Villages, Prey Kokir  Commune, Chantrea District, </t>
         </is>
       </c>
     </row>
-    <row r="3" ht="17.25" customHeight="1" s="120">
+    <row r="3" ht="17.25" customHeight="1" s="118">
       <c r="A3" s="81" t="inlineStr">
         <is>
           <t>Svay Rieng Province, Kingdom of Cambodia.</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="17.25" customHeight="1" s="120">
+    <row r="4" ht="17.25" customHeight="1" s="118">
       <c r="A4" s="81" t="inlineStr">
         <is>
           <t>VAT:L001-901903209</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="25.5" customHeight="1" s="120">
+    <row r="5" ht="25.5" customHeight="1" s="118">
       <c r="A5" s="82" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="B5" s="121" t="n"/>
-      <c r="C5" s="121" t="n"/>
-      <c r="D5" s="121" t="n"/>
-      <c r="E5" s="121" t="n"/>
-      <c r="F5" s="121" t="n"/>
-      <c r="G5" s="121" t="n"/>
-    </row>
-    <row r="6" ht="69" customHeight="1" s="120">
+      <c r="B5" s="119" t="n"/>
+      <c r="C5" s="119" t="n"/>
+      <c r="D5" s="119" t="n"/>
+      <c r="E5" s="119" t="n"/>
+      <c r="F5" s="119" t="n"/>
+      <c r="G5" s="119" t="n"/>
+    </row>
+    <row r="6" ht="69" customHeight="1" s="118">
       <c r="A6" s="84" t="inlineStr">
         <is>
           <t>INVOICE</t>
         </is>
       </c>
-      <c r="B6" s="122" t="n"/>
-      <c r="C6" s="122" t="n"/>
-      <c r="D6" s="122" t="n"/>
-      <c r="E6" s="122" t="n"/>
-      <c r="F6" s="122" t="n"/>
-      <c r="G6" s="122" t="n"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1" s="120">
+      <c r="B6" s="120" t="n"/>
+      <c r="C6" s="120" t="n"/>
+      <c r="D6" s="120" t="n"/>
+      <c r="E6" s="120" t="n"/>
+      <c r="F6" s="120" t="n"/>
+      <c r="G6" s="120" t="n"/>
+    </row>
+    <row r="7" ht="14.25" customHeight="1" s="118">
       <c r="A7" s="6" t="n"/>
       <c r="B7" s="6" t="n"/>
       <c r="C7" s="6" t="n"/>
@@ -3012,7 +2851,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="30" customHeight="1" s="120">
+    <row r="8" ht="30" customHeight="1" s="118">
       <c r="A8" s="36" t="inlineStr">
         <is>
           <t>EXPORTER:</t>
@@ -3037,7 +2876,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="21" customHeight="1" s="120">
+    <row r="9" ht="21" customHeight="1" s="118">
       <c r="A9" s="31" t="n"/>
       <c r="B9" s="31" t="inlineStr">
         <is>
@@ -3052,11 +2891,11 @@
           <t>Date:</t>
         </is>
       </c>
-      <c r="G9" s="123" t="n">
+      <c r="G9" s="121" t="n">
         <v>45906</v>
       </c>
     </row>
-    <row r="10" ht="22.5" customHeight="1" s="120">
+    <row r="10" ht="22.5" customHeight="1" s="118">
       <c r="A10" s="31" t="n"/>
       <c r="B10" s="31" t="inlineStr">
         <is>
@@ -3068,16 +2907,16 @@
       <c r="E10" s="31" t="n"/>
       <c r="F10" s="30" t="inlineStr">
         <is>
-          <t>DAP:</t>
+          <t>FOB:</t>
         </is>
       </c>
       <c r="G10" s="15" t="inlineStr">
         <is>
-          <t>BINH DUONG</t>
-        </is>
-      </c>
-    </row>
-    <row r="11" ht="20.25" customHeight="1" s="120">
+          <t>BAVET</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="20.25" customHeight="1" s="118">
       <c r="A11" s="31" t="n"/>
       <c r="B11" s="31" t="inlineStr">
         <is>
@@ -3090,7 +2929,7 @@
       <c r="F11" s="6" t="n"/>
       <c r="G11" s="80" t="n"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1" s="120">
+    <row r="12" ht="15.75" customHeight="1" s="118">
       <c r="A12" s="6" t="n"/>
       <c r="B12" s="6" t="n"/>
       <c r="C12" s="6" t="n"/>
@@ -3099,13 +2938,13 @@
       <c r="F12" s="6" t="n"/>
       <c r="G12" s="80" t="n"/>
     </row>
-    <row r="13" ht="25.5" customHeight="1" s="120">
+    <row r="13" ht="25.5" customHeight="1" s="118">
       <c r="B13" s="38" t="n"/>
       <c r="E13" s="39" t="n"/>
       <c r="F13" s="39" t="n"/>
       <c r="G13" s="32" t="n"/>
     </row>
-    <row r="14" ht="25.5" customHeight="1" s="120">
+    <row r="14" ht="25.5" customHeight="1" s="118">
       <c r="A14" s="11" t="inlineStr">
         <is>
           <t>CONSIGNEE :</t>
@@ -3121,7 +2960,7 @@
       <c r="E14" s="12" t="n"/>
       <c r="F14" s="12" t="n"/>
     </row>
-    <row r="15" ht="25.5" customHeight="1" s="120">
+    <row r="15" ht="25.5" customHeight="1" s="118">
       <c r="A15" s="10" t="n"/>
       <c r="B15" s="85" t="inlineStr">
         <is>
@@ -3130,7 +2969,7 @@
       </c>
       <c r="F15" s="14" t="n"/>
     </row>
-    <row r="16" ht="25.5" customHeight="1" s="120">
+    <row r="16" ht="25.5" customHeight="1" s="118">
       <c r="A16" s="10" t="n"/>
       <c r="B16" s="15" t="inlineStr">
         <is>
@@ -3142,7 +2981,7 @@
       <c r="E16" s="12" t="n"/>
       <c r="F16" s="12" t="n"/>
     </row>
-    <row r="17" ht="24" customHeight="1" s="120">
+    <row r="17" ht="24" customHeight="1" s="118">
       <c r="A17" s="16" t="n"/>
       <c r="B17" s="15" t="inlineStr">
         <is>
@@ -3154,7 +2993,7 @@
       <c r="E17" s="1" t="n"/>
       <c r="F17" s="17" t="n"/>
     </row>
-    <row r="18" ht="26.1" customHeight="1" s="120">
+    <row r="18" ht="26.1" customHeight="1" s="118">
       <c r="A18" s="16" t="n"/>
       <c r="B18" s="15" t="inlineStr">
         <is>
@@ -3166,7 +3005,7 @@
       <c r="E18" s="1" t="n"/>
       <c r="F18" s="17" t="n"/>
     </row>
-    <row r="19" ht="27.75" customHeight="1" s="120">
+    <row r="19" ht="27.75" customHeight="1" s="118">
       <c r="A19" s="16" t="inlineStr">
         <is>
           <t xml:space="preserve">SHIP: </t>
@@ -3182,371 +3021,258 @@
       <c r="E19" s="1" t="n"/>
       <c r="F19" s="17" t="n"/>
     </row>
-    <row r="20" ht="27.75" customHeight="1" s="120">
+    <row r="20" ht="27.75" customHeight="1" s="118">
       <c r="A20" s="18" t="n"/>
       <c r="B20" s="18" t="n"/>
     </row>
-    <row r="21" ht="35" customHeight="1" s="120">
-      <c r="A21" s="124" t="inlineStr">
+    <row r="21" ht="35" customHeight="1" s="118">
+      <c r="A21" s="122" t="inlineStr">
         <is>
           <t>Mark &amp; Nº</t>
         </is>
       </c>
-      <c r="B21" s="124" t="inlineStr">
+      <c r="B21" s="122" t="inlineStr">
         <is>
           <t>P.O. Nº</t>
         </is>
       </c>
-      <c r="C21" s="124" t="inlineStr">
+      <c r="C21" s="122" t="inlineStr">
         <is>
           <t>ITEM Nº</t>
         </is>
       </c>
-      <c r="D21" s="124" t="inlineStr">
+      <c r="D21" s="122" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="E21" s="124" t="inlineStr">
+      <c r="E21" s="122" t="inlineStr">
         <is>
           <t>Quantity
 (SF)</t>
         </is>
       </c>
-      <c r="F21" s="124" t="inlineStr">
+      <c r="F21" s="122" t="inlineStr">
         <is>
           <t>Unit Price
 (USD)</t>
         </is>
       </c>
-      <c r="G21" s="124" t="inlineStr">
+      <c r="G21" s="122" t="inlineStr">
         <is>
           <t>Amount(USD)</t>
         </is>
       </c>
     </row>
-    <row r="22" ht="35" customHeight="1" s="120">
-      <c r="A22" s="125" t="inlineStr">
+    <row r="22" ht="35" customHeight="1" s="118">
+      <c r="A22" s="123" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B22" s="126" t="inlineStr">
-        <is>
-          <t>YNGY25022</t>
-        </is>
-      </c>
-      <c r="C22" s="126" t="inlineStr">
-        <is>
-          <t>M1243</t>
-        </is>
-      </c>
-      <c r="D22" s="127" t="inlineStr">
+      <c r="B22" s="124" t="inlineStr">
+        <is>
+          <t>GYOJY_M25371/GYOJY_M25374
+YNGY25022/YNGY25028</t>
+        </is>
+      </c>
+      <c r="C22" s="124" t="inlineStr">
+        <is>
+          <t>M1243/Nick Dove</t>
+        </is>
+      </c>
+      <c r="D22" s="125" t="inlineStr">
         <is>
           <t>LEATHER</t>
         </is>
       </c>
-      <c r="E22" s="128" t="n">
-        <v>10045.4</v>
-      </c>
-      <c r="F22" s="128" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="G22" s="128">
-        <f>F22*E22</f>
+      <c r="E22" s="126" t="n">
+        <v>225927.8</v>
+      </c>
+      <c r="F22" s="126">
+        <f>G22/E22</f>
         <v/>
       </c>
-    </row>
-    <row r="23" ht="35" customHeight="1" s="120">
-      <c r="A23" s="129" t="inlineStr">
+      <c r="G22" s="126" t="n">
+        <v>259081.023</v>
+      </c>
+    </row>
+    <row r="23" ht="35" customHeight="1" s="118">
+      <c r="A23" s="127" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B23" s="126" t="inlineStr">
-        <is>
-          <t>YNGY25028</t>
-        </is>
-      </c>
-      <c r="C23" s="126" t="inlineStr">
-        <is>
-          <t>M1243</t>
-        </is>
-      </c>
-      <c r="D23" s="110" t="n"/>
-      <c r="E23" s="128" t="n">
-        <v>40074.3</v>
-      </c>
-      <c r="F23" s="128" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="G23" s="128">
-        <f>F23*E23</f>
+      <c r="B23" s="124" t="n"/>
+      <c r="C23" s="124" t="n"/>
+      <c r="D23" s="125" t="n"/>
+      <c r="E23" s="126" t="n"/>
+      <c r="F23" s="126" t="n"/>
+      <c r="G23" s="126" t="n"/>
+    </row>
+    <row r="24" ht="35" customHeight="1" s="118">
+      <c r="A24" s="127" t="inlineStr">
+        <is>
+          <t>Case Qty:</t>
+        </is>
+      </c>
+      <c r="B24" s="124" t="n"/>
+      <c r="C24" s="124" t="n"/>
+      <c r="D24" s="125" t="n"/>
+      <c r="E24" s="126" t="n"/>
+      <c r="F24" s="126" t="n"/>
+      <c r="G24" s="126" t="n"/>
+    </row>
+    <row r="25" ht="35" customHeight="1" s="118">
+      <c r="A25" s="127" t="inlineStr">
+        <is>
+          <t>MADE IN CAMBODIA</t>
+        </is>
+      </c>
+      <c r="B25" s="124" t="n"/>
+      <c r="C25" s="124" t="n"/>
+      <c r="D25" s="125" t="n"/>
+      <c r="E25" s="126" t="n"/>
+      <c r="F25" s="126" t="n"/>
+      <c r="G25" s="126" t="n"/>
+    </row>
+    <row r="26" ht="35" customFormat="1" customHeight="1" s="2">
+      <c r="A26" s="125" t="n"/>
+      <c r="B26" s="124" t="inlineStr">
+        <is>
+          <t>HS.CODE: 4107.12.00</t>
+        </is>
+      </c>
+      <c r="C26" s="125" t="n"/>
+      <c r="D26" s="125" t="n"/>
+      <c r="E26" s="126" t="n"/>
+      <c r="F26" s="126" t="n"/>
+      <c r="G26" s="126" t="n"/>
+    </row>
+    <row r="27" ht="35" customHeight="1" s="118">
+      <c r="A27" s="128" t="n"/>
+      <c r="B27" s="128" t="inlineStr">
+        <is>
+          <t>TOTAL OF:</t>
+        </is>
+      </c>
+      <c r="C27" s="128" t="inlineStr">
+        <is>
+          <t>22 PALLETS</t>
+        </is>
+      </c>
+      <c r="D27" s="128" t="n"/>
+      <c r="E27" s="129">
+        <f>SUM(E22:E25)</f>
         <v/>
       </c>
-    </row>
-    <row r="24" ht="35" customHeight="1" s="120">
-      <c r="A24" s="129" t="inlineStr">
-        <is>
-          <t>Case Qty:</t>
-        </is>
-      </c>
-      <c r="B24" s="126" t="inlineStr">
-        <is>
-          <t>YNGY25028</t>
-        </is>
-      </c>
-      <c r="C24" s="126" t="inlineStr">
-        <is>
-          <t>M1243</t>
-        </is>
-      </c>
-      <c r="D24" s="110" t="n"/>
-      <c r="E24" s="128" t="n">
-        <v>475</v>
-      </c>
-      <c r="F24" s="128" t="n">
-        <v>0.91</v>
-      </c>
-      <c r="G24" s="128">
-        <f>F24*E24</f>
+      <c r="F27" s="128" t="n"/>
+      <c r="G27" s="129">
+        <f>SUM(G22:G25)</f>
         <v/>
       </c>
     </row>
-    <row r="25" ht="35" customHeight="1" s="120">
-      <c r="A25" s="129" t="inlineStr">
-        <is>
-          <t>MADE IN CAMBODIA</t>
-        </is>
-      </c>
-      <c r="B25" s="126" t="inlineStr">
-        <is>
-          <t>GYOJY_M25371</t>
-        </is>
-      </c>
-      <c r="C25" s="126" t="inlineStr">
-        <is>
-          <t>Nick Dove</t>
-        </is>
-      </c>
-      <c r="D25" s="110" t="n"/>
-      <c r="E25" s="128" t="n">
-        <v>136378.1</v>
-      </c>
-      <c r="F25" s="128" t="n">
-        <v>1.15</v>
-      </c>
-      <c r="G25" s="128">
-        <f>F25*E25</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26" ht="35" customFormat="1" customHeight="1" s="2">
-      <c r="A26" s="129" t="n"/>
-      <c r="B26" s="126" t="inlineStr">
-        <is>
-          <t>GYOJY_M25371</t>
-        </is>
-      </c>
-      <c r="C26" s="126" t="inlineStr">
-        <is>
-          <t>Nick Dove</t>
-        </is>
-      </c>
-      <c r="D26" s="110" t="n"/>
-      <c r="E26" s="128" t="n">
-        <v>113.7</v>
-      </c>
-      <c r="F26" s="128" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="G26" s="128">
-        <f>F26*E26</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" ht="35" customHeight="1" s="120">
-      <c r="A27" s="129" t="n"/>
-      <c r="B27" s="126" t="inlineStr">
-        <is>
-          <t>GYOJY_M25374</t>
-        </is>
-      </c>
-      <c r="C27" s="126" t="inlineStr">
-        <is>
-          <t>Nick Dove</t>
-        </is>
-      </c>
-      <c r="D27" s="110" t="n"/>
-      <c r="E27" s="128" t="n">
-        <v>38430</v>
-      </c>
-      <c r="F27" s="128" t="n">
-        <v>1.15</v>
-      </c>
-      <c r="G27" s="128">
-        <f>F27*E27</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" ht="35" customHeight="1" s="120">
-      <c r="A28" s="129" t="n"/>
-      <c r="B28" s="126" t="inlineStr">
-        <is>
-          <t>GYOJY_M25374</t>
-        </is>
-      </c>
-      <c r="C28" s="126" t="inlineStr">
-        <is>
-          <t>Nick Dove</t>
-        </is>
-      </c>
-      <c r="D28" s="111" t="n"/>
-      <c r="E28" s="128" t="n">
-        <v>411.3</v>
-      </c>
-      <c r="F28" s="128" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="G28" s="128">
-        <f>F28*E28</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" ht="35" customHeight="1" s="120">
-      <c r="A29" s="127" t="n"/>
-      <c r="B29" s="126" t="inlineStr">
-        <is>
-          <t>HS.CODE: 4107.12.00</t>
-        </is>
-      </c>
-      <c r="C29" s="127" t="n"/>
-      <c r="D29" s="127" t="n"/>
-      <c r="E29" s="128" t="n"/>
-      <c r="F29" s="128" t="n"/>
-      <c r="G29" s="128" t="n"/>
-    </row>
-    <row r="30" ht="35" customHeight="1" s="120">
-      <c r="A30" s="130" t="n"/>
-      <c r="B30" s="130" t="inlineStr">
-        <is>
-          <t>TOTAL OF:</t>
-        </is>
-      </c>
-      <c r="C30" s="130" t="inlineStr">
-        <is>
-          <t>22 PALLETS</t>
-        </is>
-      </c>
-      <c r="D30" s="130" t="n"/>
-      <c r="E30" s="131">
-        <f>SUM(E22:E28)</f>
-        <v/>
-      </c>
-      <c r="F30" s="130" t="n"/>
-      <c r="G30" s="131">
-        <f>SUM(G22:G28)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" ht="42" customHeight="1" s="120">
-      <c r="A31" s="86" t="inlineStr">
+    <row r="28" ht="42" customHeight="1" s="118">
+      <c r="A28" s="86" t="inlineStr">
         <is>
           <t xml:space="preserve">Country of Original Cambodia </t>
         </is>
       </c>
-      <c r="D31" s="86" t="n"/>
-      <c r="E31" s="6" t="n"/>
-      <c r="F31" s="6" t="n"/>
-      <c r="G31" s="80" t="n"/>
-    </row>
-    <row r="32" ht="61.5" customHeight="1" s="120">
-      <c r="A32" s="22" t="inlineStr">
+      <c r="D28" s="86" t="n"/>
+      <c r="E28" s="6" t="n"/>
+      <c r="F28" s="6" t="n"/>
+      <c r="G28" s="80" t="n"/>
+    </row>
+    <row r="29" ht="61.5" customHeight="1" s="118">
+      <c r="A29" s="22" t="inlineStr">
         <is>
           <t>Manufacture:</t>
         </is>
       </c>
-      <c r="B32" s="87" t="inlineStr">
+      <c r="B29" s="87" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="D32" s="87" t="n"/>
-      <c r="E32" s="87" t="n"/>
-      <c r="F32" s="6" t="n"/>
-      <c r="G32" s="80" t="n"/>
-    </row>
-    <row r="33" ht="44.1" customHeight="1" s="120">
-      <c r="A33" s="88" t="inlineStr">
+      <c r="D29" s="87" t="n"/>
+      <c r="E29" s="87" t="n"/>
+      <c r="F29" s="6" t="n"/>
+      <c r="G29" s="80" t="n"/>
+    </row>
+    <row r="30" ht="44.1" customHeight="1" s="118">
+      <c r="A30" s="88" t="inlineStr">
         <is>
           <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
                                                   /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
-      <c r="D33" s="88" t="n"/>
-      <c r="E33" s="88" t="n"/>
-      <c r="F33" s="88" t="n"/>
+      <c r="D30" s="88" t="n"/>
+      <c r="E30" s="88" t="n"/>
+      <c r="F30" s="88" t="n"/>
+      <c r="G30" s="80" t="n"/>
+    </row>
+    <row r="31" ht="24.75" customHeight="1" s="118">
+      <c r="A31" s="83" t="inlineStr">
+        <is>
+          <t>A/C NO:100001100764430</t>
+        </is>
+      </c>
+    </row>
+    <row r="32" ht="27" customHeight="1" s="118">
+      <c r="A32" s="83" t="inlineStr">
+        <is>
+          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
+        </is>
+      </c>
+    </row>
+    <row r="33" ht="27.75" customHeight="1" s="118">
+      <c r="E33" s="31" t="n"/>
+      <c r="F33" s="33" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
+        </is>
+      </c>
       <c r="G33" s="80" t="n"/>
     </row>
-    <row r="34" ht="24.75" customHeight="1" s="120">
-      <c r="A34" s="83" t="inlineStr">
-        <is>
-          <t>A/C NO:100001100764430</t>
-        </is>
-      </c>
-    </row>
-    <row r="35" ht="27" customHeight="1" s="120">
-      <c r="A35" s="83" t="inlineStr">
-        <is>
-          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
-        </is>
-      </c>
-    </row>
-    <row r="36" ht="21" customHeight="1" s="120">
-      <c r="E36" s="31" t="n"/>
-      <c r="F36" s="33" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
-        </is>
-      </c>
-      <c r="G36" s="80" t="n"/>
-    </row>
-    <row r="37" ht="21" customHeight="1" s="120">
+    <row r="34" ht="27.75" customHeight="1" s="118">
+      <c r="E34" s="6" t="n"/>
+      <c r="F34" s="34" t="inlineStr">
+        <is>
+          <t>Sign &amp; Stamp</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" ht="24.75" customHeight="1" s="118">
+      <c r="E35" s="6" t="n"/>
+      <c r="F35" s="6" t="n"/>
+    </row>
+    <row r="36" ht="21" customHeight="1" s="118">
+      <c r="E36" s="6" t="n"/>
+      <c r="F36" s="6" t="n"/>
+    </row>
+    <row r="37" ht="21" customHeight="1" s="118">
       <c r="E37" s="6" t="n"/>
-      <c r="F37" s="34" t="inlineStr">
-        <is>
-          <t>Sign &amp; Stamp</t>
-        </is>
-      </c>
-    </row>
-    <row r="38" ht="21" customHeight="1" s="120">
-      <c r="E38" s="6" t="n"/>
-      <c r="F38" s="6" t="n"/>
-    </row>
-    <row r="39" ht="21" customHeight="1" s="120">
-      <c r="E39" s="6" t="n"/>
-      <c r="F39" s="6" t="n"/>
-    </row>
-    <row r="40" ht="21" customHeight="1" s="120">
-      <c r="E40" s="6" t="n"/>
-      <c r="F40" s="40" t="inlineStr">
+      <c r="F37" s="40" t="inlineStr">
         <is>
           <t>ZENG XUELI</t>
         </is>
       </c>
-      <c r="G40" s="35" t="n"/>
-    </row>
-    <row r="41" ht="21" customHeight="1" s="120"/>
-    <row r="42" ht="21" customHeight="1" s="120"/>
-    <row r="43" ht="21" customHeight="1" s="120"/>
-    <row r="44" ht="25.5" customHeight="1" s="120"/>
-    <row r="45" ht="21" customHeight="1" s="120"/>
-    <row r="46" ht="21" customHeight="1" s="120"/>
-    <row r="47" ht="21" customHeight="1" s="120"/>
-    <row r="48" ht="21" customHeight="1" s="120"/>
-    <row r="49" ht="21" customHeight="1" s="120"/>
-    <row r="50" ht="17.25" customHeight="1" s="120"/>
+      <c r="G37" s="35" t="n"/>
+    </row>
+    <row r="38" ht="21" customHeight="1" s="118"/>
+    <row r="39" ht="21" customHeight="1" s="118"/>
+    <row r="40" ht="21" customHeight="1" s="118"/>
+    <row r="41" ht="21" customHeight="1" s="118"/>
+    <row r="42" ht="21" customHeight="1" s="118"/>
+    <row r="43" ht="21" customHeight="1" s="118"/>
+    <row r="44" ht="25.5" customHeight="1" s="118"/>
+    <row r="45" ht="21" customHeight="1" s="118"/>
+    <row r="46" ht="21" customHeight="1" s="118"/>
+    <row r="47" ht="21" customHeight="1" s="118"/>
+    <row r="48" ht="21" customHeight="1" s="118"/>
+    <row r="49" ht="21" customHeight="1" s="118"/>
+    <row r="50" ht="17.25" customHeight="1" s="118"/>
     <row r="51"/>
     <row r="52"/>
     <row r="53"/>
@@ -3558,7 +3284,7 @@
     <row r="59"/>
     <row r="60"/>
     <row r="61"/>
-    <row r="62" ht="15" customHeight="1" s="120"/>
+    <row r="62" ht="15" customHeight="1" s="118"/>
     <row r="63"/>
     <row r="64"/>
     <row r="65"/>
@@ -3697,22 +3423,27 @@
     <row r="198"/>
     <row r="199"/>
     <row r="200"/>
+    <row r="201"/>
+    <row r="202"/>
+    <row r="203"/>
+    <row r="204"/>
+    <row r="205"/>
+    <row r="206"/>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A33:C33"/>
+  <mergeCells count="13">
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A28:C28"/>
     <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="A31:G31"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A6:G6"/>
-    <mergeCell ref="D22:D28"/>
-    <mergeCell ref="B30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="A35:G35"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="A30:C30"/>
     <mergeCell ref="A5:G5"/>
+    <mergeCell ref="B27"/>
   </mergeCells>
   <conditionalFormatting sqref="J22:J34">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>
@@ -3731,7 +3462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N200"/>
+  <dimension ref="A1:P237"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A8" zoomScale="85" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
@@ -3759,7 +3490,7 @@
     <col width="7.140625" customWidth="1" style="90" min="18" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="38.25" customHeight="1" s="120">
+    <row r="1" ht="38.25" customHeight="1" s="118">
       <c r="A1" s="79" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
@@ -3768,7 +3499,7 @@
       <c r="K1" s="26" t="n"/>
       <c r="L1" s="26" t="n"/>
     </row>
-    <row r="2" ht="24" customHeight="1" s="120">
+    <row r="2" ht="24" customHeight="1" s="118">
       <c r="A2" s="80" t="inlineStr">
         <is>
           <t xml:space="preserve"> XIN BAVET SEZ, Road No. 316A, Trapeang Bon and  Prey Kokir  Villages, Prey Kokir  Commune, Chantrea District, </t>
@@ -3777,7 +3508,7 @@
       <c r="K2" s="6" t="n"/>
       <c r="L2" s="6" t="n"/>
     </row>
-    <row r="3" ht="25.5" customHeight="1" s="120">
+    <row r="3" ht="25.5" customHeight="1" s="118">
       <c r="A3" s="81" t="inlineStr">
         <is>
           <t>Svay Rieng Province, Kingdom of Cambodia.</t>
@@ -3786,7 +3517,7 @@
       <c r="K3" s="83" t="n"/>
       <c r="L3" s="83" t="n"/>
     </row>
-    <row r="4" ht="25.5" customHeight="1" s="120">
+    <row r="4" ht="25.5" customHeight="1" s="118">
       <c r="A4" s="89" t="inlineStr">
         <is>
           <t>VAT:L001-901903209</t>
@@ -3795,43 +3526,43 @@
       <c r="K4" s="83" t="n"/>
       <c r="L4" s="83" t="n"/>
     </row>
-    <row r="5" ht="21.95" customHeight="1" s="120">
+    <row r="5" ht="21.95" customHeight="1" s="118">
       <c r="A5" s="82" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="B5" s="121" t="n"/>
-      <c r="C5" s="121" t="n"/>
-      <c r="D5" s="121" t="n"/>
-      <c r="E5" s="121" t="n"/>
-      <c r="F5" s="121" t="n"/>
-      <c r="G5" s="121" t="n"/>
-      <c r="H5" s="121" t="n"/>
-      <c r="I5" s="121" t="n"/>
-      <c r="J5" s="121" t="n"/>
+      <c r="B5" s="119" t="n"/>
+      <c r="C5" s="119" t="n"/>
+      <c r="D5" s="119" t="n"/>
+      <c r="E5" s="119" t="n"/>
+      <c r="F5" s="119" t="n"/>
+      <c r="G5" s="119" t="n"/>
+      <c r="H5" s="119" t="n"/>
+      <c r="I5" s="119" t="n"/>
+      <c r="J5" s="119" t="n"/>
       <c r="K5" s="83" t="n"/>
       <c r="L5" s="83" t="n"/>
     </row>
-    <row r="6" ht="54" customHeight="1" s="120">
+    <row r="6" ht="54" customHeight="1" s="118">
       <c r="A6" s="84" t="inlineStr">
         <is>
           <t>PACKING LIST</t>
         </is>
       </c>
-      <c r="B6" s="122" t="n"/>
-      <c r="C6" s="122" t="n"/>
-      <c r="D6" s="122" t="n"/>
-      <c r="E6" s="122" t="n"/>
-      <c r="F6" s="122" t="n"/>
-      <c r="G6" s="122" t="n"/>
-      <c r="H6" s="122" t="n"/>
-      <c r="I6" s="122" t="n"/>
-      <c r="J6" s="122" t="n"/>
+      <c r="B6" s="120" t="n"/>
+      <c r="C6" s="120" t="n"/>
+      <c r="D6" s="120" t="n"/>
+      <c r="E6" s="120" t="n"/>
+      <c r="F6" s="120" t="n"/>
+      <c r="G6" s="120" t="n"/>
+      <c r="H6" s="120" t="n"/>
+      <c r="I6" s="120" t="n"/>
+      <c r="J6" s="120" t="n"/>
       <c r="K6" s="27" t="n"/>
       <c r="L6" s="27" t="n"/>
     </row>
-    <row r="7" ht="18.95" customHeight="1" s="120">
+    <row r="7" ht="18.95" customHeight="1" s="118">
       <c r="A7" s="6" t="n"/>
       <c r="B7" s="6" t="n"/>
       <c r="C7" s="6" t="n"/>
@@ -3851,7 +3582,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="30" customHeight="1" s="120">
+    <row r="8" ht="30" customHeight="1" s="118">
       <c r="A8" s="7" t="inlineStr">
         <is>
           <t>EXPORTER:</t>
@@ -3878,7 +3609,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="21" customHeight="1" s="120">
+    <row r="9" ht="21" customHeight="1" s="118">
       <c r="A9" s="10" t="n"/>
       <c r="B9" s="10" t="inlineStr">
         <is>
@@ -3895,11 +3626,11 @@
           <t>Date:</t>
         </is>
       </c>
-      <c r="J9" s="123" t="n">
+      <c r="J9" s="121" t="n">
         <v>45906</v>
       </c>
     </row>
-    <row r="10" ht="22.5" customHeight="1" s="120">
+    <row r="10" ht="22.5" customHeight="1" s="118">
       <c r="A10" s="10" t="n"/>
       <c r="B10" s="10" t="inlineStr">
         <is>
@@ -3913,17 +3644,17 @@
       <c r="H10" s="6" t="n"/>
       <c r="I10" s="30" t="inlineStr">
         <is>
-          <t>DAP:</t>
+          <t>FOB:</t>
         </is>
       </c>
       <c r="J10" s="15" t="inlineStr">
         <is>
-          <t>BINH DUONG</t>
+          <t>BAVET</t>
         </is>
       </c>
       <c r="K10" s="31" t="n"/>
     </row>
-    <row r="11" ht="20.25" customHeight="1" s="120">
+    <row r="11" ht="20.25" customHeight="1" s="118">
       <c r="A11" s="10" t="n"/>
       <c r="B11" s="10" t="inlineStr">
         <is>
@@ -3940,7 +3671,7 @@
       <c r="K11" s="6" t="n"/>
       <c r="L11" s="6" t="n"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1" s="120">
+    <row r="12" ht="15.75" customHeight="1" s="118">
       <c r="A12" s="10" t="n"/>
       <c r="B12" s="10" t="n"/>
       <c r="C12" s="10" t="n"/>
@@ -3954,7 +3685,7 @@
       <c r="K12" s="6" t="n"/>
       <c r="L12" s="6" t="n"/>
     </row>
-    <row r="13" ht="25.5" customHeight="1" s="120">
+    <row r="13" ht="25.5" customHeight="1" s="118">
       <c r="A13" s="11" t="inlineStr">
         <is>
           <t>CONSIGNEE :</t>
@@ -3972,7 +3703,7 @@
       <c r="H13" s="4" t="n"/>
       <c r="J13" s="90" t="n"/>
     </row>
-    <row r="14" ht="25.5" customHeight="1" s="120">
+    <row r="14" ht="25.5" customHeight="1" s="118">
       <c r="A14" s="10" t="n"/>
       <c r="B14" s="85" t="inlineStr">
         <is>
@@ -3983,7 +3714,7 @@
       <c r="H14" s="4" t="n"/>
       <c r="J14" s="90" t="n"/>
     </row>
-    <row r="15" ht="25.5" customHeight="1" s="120">
+    <row r="15" ht="25.5" customHeight="1" s="118">
       <c r="A15" s="10" t="n"/>
       <c r="B15" s="15" t="inlineStr">
         <is>
@@ -3997,7 +3728,7 @@
       <c r="H15" s="4" t="n"/>
       <c r="J15" s="90" t="n"/>
     </row>
-    <row r="16" ht="24" customHeight="1" s="120">
+    <row r="16" ht="24" customHeight="1" s="118">
       <c r="A16" s="16" t="n"/>
       <c r="B16" s="15" t="inlineStr">
         <is>
@@ -4011,7 +3742,7 @@
       <c r="H16" s="4" t="n"/>
       <c r="J16" s="90" t="n"/>
     </row>
-    <row r="17" ht="26.1" customHeight="1" s="120">
+    <row r="17" ht="26.1" customHeight="1" s="118">
       <c r="A17" s="16" t="n"/>
       <c r="B17" s="15" t="inlineStr">
         <is>
@@ -4025,7 +3756,7 @@
       <c r="H17" s="4" t="n"/>
       <c r="J17" s="90" t="n"/>
     </row>
-    <row r="18" ht="27.75" customHeight="1" s="120">
+    <row r="18" ht="27.75" customHeight="1" s="118">
       <c r="A18" s="16" t="inlineStr">
         <is>
           <t xml:space="preserve">SHIP: </t>
@@ -4043,1251 +3774,1251 @@
       <c r="H18" s="4" t="n"/>
       <c r="J18" s="90" t="n"/>
     </row>
-    <row r="19" ht="27.75" customHeight="1" s="120">
+    <row r="19" ht="27.75" customHeight="1" s="118">
       <c r="A19" s="18" t="n"/>
       <c r="B19" s="18" t="n"/>
       <c r="C19" s="18" t="n"/>
     </row>
-    <row r="20" ht="27" customHeight="1" s="120">
-      <c r="A20" s="124" t="inlineStr">
+    <row r="20" ht="27" customHeight="1" s="118">
+      <c r="A20" s="122" t="inlineStr">
         <is>
           <t>Mark &amp; Nº</t>
         </is>
       </c>
-      <c r="B20" s="124" t="inlineStr">
+      <c r="B20" s="122" t="inlineStr">
         <is>
           <t>PALLET
-N.</t>
-        </is>
-      </c>
-      <c r="C20" s="124" t="inlineStr">
+NO.</t>
+        </is>
+      </c>
+      <c r="C20" s="122" t="inlineStr">
         <is>
           <t>P.O Nº</t>
         </is>
       </c>
-      <c r="D20" s="124" t="inlineStr">
+      <c r="D20" s="122" t="inlineStr">
         <is>
           <t>ITEM Nº</t>
         </is>
       </c>
-      <c r="E20" s="124" t="inlineStr">
+      <c r="E20" s="122" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="F20" s="124" t="inlineStr">
+      <c r="F20" s="122" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="G20" s="113" t="n"/>
-      <c r="H20" s="124" t="inlineStr">
+      <c r="G20" s="111" t="n"/>
+      <c r="H20" s="122" t="inlineStr">
         <is>
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="I20" s="124" t="inlineStr">
+      <c r="I20" s="122" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
         </is>
       </c>
-      <c r="J20" s="124" t="inlineStr">
+      <c r="J20" s="122" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
       </c>
     </row>
-    <row r="21" ht="27" customHeight="1" s="120">
-      <c r="A21" s="111" t="n"/>
-      <c r="B21" s="111" t="n"/>
-      <c r="C21" s="111" t="n"/>
-      <c r="D21" s="111" t="n"/>
-      <c r="E21" s="111" t="n"/>
-      <c r="F21" s="124" t="inlineStr">
+    <row r="21" ht="27" customHeight="1" s="118">
+      <c r="A21" s="130" t="n"/>
+      <c r="B21" s="130" t="n"/>
+      <c r="C21" s="130" t="n"/>
+      <c r="D21" s="130" t="n"/>
+      <c r="E21" s="130" t="n"/>
+      <c r="F21" s="122" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
       </c>
-      <c r="G21" s="124" t="inlineStr">
+      <c r="G21" s="122" t="inlineStr">
         <is>
           <t>SF</t>
         </is>
       </c>
-      <c r="H21" s="111" t="n"/>
-      <c r="I21" s="111" t="n"/>
-      <c r="J21" s="111" t="n"/>
-    </row>
-    <row r="22" ht="27" customHeight="1" s="120">
-      <c r="A22" s="132" t="inlineStr">
+      <c r="H21" s="130" t="n"/>
+      <c r="I21" s="130" t="n"/>
+      <c r="J21" s="130" t="n"/>
+    </row>
+    <row r="22" ht="27" customHeight="1" s="118">
+      <c r="A22" s="131" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B22" s="127" t="inlineStr">
+      <c r="B22" s="125" t="inlineStr">
         <is>
           <t>1-7</t>
         </is>
       </c>
-      <c r="C22" s="126" t="inlineStr">
+      <c r="C22" s="124" t="inlineStr">
         <is>
           <t>YNGY25022</t>
         </is>
       </c>
-      <c r="D22" s="126" t="inlineStr">
+      <c r="D22" s="124" t="inlineStr">
         <is>
           <t>M1243</t>
         </is>
       </c>
-      <c r="E22" s="126" t="inlineStr">
+      <c r="E22" s="124" t="inlineStr">
         <is>
           <t>LEATHER</t>
         </is>
       </c>
-      <c r="F22" s="133" t="n">
+      <c r="F22" s="126" t="n">
         <v>195</v>
       </c>
-      <c r="G22" s="134" t="n">
+      <c r="G22" s="126" t="n">
         <v>10045.4</v>
       </c>
-      <c r="H22" s="134" t="n">
+      <c r="H22" s="126" t="n">
         <v>804</v>
       </c>
-      <c r="I22" s="134" t="n">
+      <c r="I22" s="126" t="n">
         <v>759</v>
       </c>
-      <c r="J22" s="135" t="n">
+      <c r="J22" s="126" t="n">
         <v>2.4948</v>
       </c>
     </row>
-    <row r="23" ht="27" customHeight="1" s="120">
-      <c r="A23" s="136" t="inlineStr">
+    <row r="23" ht="27" customHeight="1" s="118">
+      <c r="A23" s="132" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B23" s="127" t="inlineStr">
+      <c r="B23" s="125" t="inlineStr">
         <is>
           <t>2-7</t>
         </is>
       </c>
-      <c r="C23" s="126" t="inlineStr">
+      <c r="C23" s="124" t="inlineStr">
         <is>
           <t>YNGY25028</t>
         </is>
       </c>
-      <c r="D23" s="126" t="inlineStr">
+      <c r="D23" s="124" t="inlineStr">
         <is>
           <t>M1243</t>
         </is>
       </c>
-      <c r="E23" s="110" t="n"/>
-      <c r="F23" s="133" t="n">
+      <c r="E23" s="133" t="n"/>
+      <c r="F23" s="126" t="n">
         <v>215</v>
       </c>
-      <c r="G23" s="134" t="n">
+      <c r="G23" s="126" t="n">
         <v>11181.6</v>
       </c>
-      <c r="H23" s="134" t="n">
+      <c r="H23" s="126" t="n">
         <v>887</v>
       </c>
-      <c r="I23" s="134" t="n">
+      <c r="I23" s="126" t="n">
         <v>842</v>
       </c>
-      <c r="J23" s="135" t="n">
+      <c r="J23" s="126" t="n">
         <v>2.772</v>
       </c>
     </row>
-    <row r="24" ht="27" customHeight="1" s="120">
-      <c r="A24" s="136" t="inlineStr">
+    <row r="24" ht="27" customHeight="1" s="118">
+      <c r="A24" s="132" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B24" s="127" t="inlineStr">
+      <c r="B24" s="125" t="inlineStr">
         <is>
           <t>3-7</t>
         </is>
       </c>
-      <c r="C24" s="126" t="inlineStr">
+      <c r="C24" s="124" t="inlineStr">
         <is>
           <t>YNGY25028</t>
         </is>
       </c>
-      <c r="D24" s="126" t="inlineStr">
+      <c r="D24" s="124" t="inlineStr">
         <is>
           <t>M1243</t>
         </is>
       </c>
-      <c r="E24" s="110" t="n"/>
-      <c r="F24" s="133" t="n">
+      <c r="E24" s="133" t="n"/>
+      <c r="F24" s="126" t="n">
         <v>210</v>
       </c>
-      <c r="G24" s="134" t="n">
+      <c r="G24" s="126" t="n">
         <v>10982.8</v>
       </c>
-      <c r="H24" s="134" t="n">
+      <c r="H24" s="126" t="n">
         <v>866.5</v>
       </c>
-      <c r="I24" s="134" t="n">
+      <c r="I24" s="126" t="n">
         <v>821.5</v>
       </c>
-      <c r="J24" s="135" t="n">
+      <c r="J24" s="126" t="n">
         <v>2.6532</v>
       </c>
     </row>
     <row r="25" ht="27" customFormat="1" customHeight="1" s="2">
-      <c r="A25" s="136" t="inlineStr">
+      <c r="A25" s="132" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B25" s="127" t="inlineStr">
+      <c r="B25" s="125" t="inlineStr">
         <is>
           <t>4-7</t>
         </is>
       </c>
-      <c r="C25" s="126" t="inlineStr">
+      <c r="C25" s="124" t="inlineStr">
         <is>
           <t>YNGY25028</t>
         </is>
       </c>
-      <c r="D25" s="126" t="inlineStr">
+      <c r="D25" s="124" t="inlineStr">
         <is>
           <t>M1243</t>
         </is>
       </c>
-      <c r="E25" s="110" t="n"/>
-      <c r="F25" s="133" t="n">
+      <c r="E25" s="133" t="n"/>
+      <c r="F25" s="126" t="n">
         <v>210</v>
       </c>
-      <c r="G25" s="134" t="n">
+      <c r="G25" s="126" t="n">
         <v>11087.8</v>
       </c>
-      <c r="H25" s="134" t="n">
+      <c r="H25" s="126" t="n">
         <v>878.5</v>
       </c>
-      <c r="I25" s="134" t="n">
+      <c r="I25" s="126" t="n">
         <v>833.5</v>
       </c>
-      <c r="J25" s="135" t="n">
+      <c r="J25" s="126" t="n">
         <v>2.8512</v>
       </c>
     </row>
-    <row r="26" ht="27" customHeight="1" s="120">
-      <c r="A26" s="136" t="n"/>
-      <c r="B26" s="127" t="inlineStr">
+    <row r="26" ht="27" customHeight="1" s="118">
+      <c r="A26" s="132" t="n"/>
+      <c r="B26" s="125" t="inlineStr">
         <is>
           <t>5-7</t>
         </is>
       </c>
-      <c r="C26" s="126" t="inlineStr">
+      <c r="C26" s="124" t="inlineStr">
         <is>
           <t>YNGY25028</t>
         </is>
       </c>
-      <c r="D26" s="126" t="inlineStr">
+      <c r="D26" s="124" t="inlineStr">
         <is>
           <t>M1243</t>
         </is>
       </c>
-      <c r="E26" s="110" t="n"/>
-      <c r="F26" s="133" t="n">
+      <c r="E26" s="133" t="n"/>
+      <c r="F26" s="126" t="n">
         <v>130</v>
       </c>
-      <c r="G26" s="134" t="n">
+      <c r="G26" s="126" t="n">
         <v>6822.1</v>
       </c>
-      <c r="H26" s="134" t="n">
+      <c r="H26" s="126" t="n">
         <v>555.7971</v>
       </c>
-      <c r="I26" s="134" t="n">
+      <c r="I26" s="126" t="n">
         <v>513.4058</v>
       </c>
-      <c r="J26" s="135" t="n">
+      <c r="J26" s="126" t="n">
         <v>2.1637</v>
       </c>
     </row>
-    <row r="27" ht="27" customHeight="1" s="120">
-      <c r="A27" s="136" t="n"/>
-      <c r="B27" s="111" t="n"/>
-      <c r="C27" s="126" t="inlineStr">
+    <row r="27" ht="27" customHeight="1" s="118">
+      <c r="A27" s="132" t="n"/>
+      <c r="B27" s="130" t="n"/>
+      <c r="C27" s="124" t="inlineStr">
         <is>
           <t>YNGY25028</t>
         </is>
       </c>
-      <c r="D27" s="126" t="inlineStr">
+      <c r="D27" s="124" t="inlineStr">
         <is>
           <t>M1243</t>
         </is>
       </c>
-      <c r="E27" s="110" t="n"/>
-      <c r="F27" s="133" t="n">
+      <c r="E27" s="133" t="n"/>
+      <c r="F27" s="126" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="134" t="n">
+      <c r="G27" s="126" t="n">
         <v>475</v>
       </c>
-      <c r="H27" s="134" t="n">
+      <c r="H27" s="126" t="n">
         <v>34.2029</v>
       </c>
-      <c r="I27" s="134" t="n">
+      <c r="I27" s="126" t="n">
         <v>31.5942</v>
       </c>
-      <c r="J27" s="135" t="n">
+      <c r="J27" s="126" t="n">
         <v>0.1331</v>
       </c>
     </row>
-    <row r="28" ht="27" customHeight="1" s="120">
-      <c r="A28" s="136" t="n"/>
-      <c r="B28" s="127" t="inlineStr">
+    <row r="28" ht="27" customHeight="1" s="118">
+      <c r="A28" s="132" t="n"/>
+      <c r="B28" s="125" t="inlineStr">
         <is>
           <t>6-7</t>
         </is>
       </c>
-      <c r="C28" s="126" t="inlineStr">
+      <c r="C28" s="124" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D28" s="126" t="inlineStr">
+      <c r="D28" s="124" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E28" s="110" t="n"/>
-      <c r="F28" s="133" t="n">
+      <c r="E28" s="133" t="n"/>
+      <c r="F28" s="126" t="n">
         <v>220</v>
       </c>
-      <c r="G28" s="134" t="n">
+      <c r="G28" s="126" t="n">
         <v>10205.7</v>
       </c>
-      <c r="H28" s="134" t="n">
+      <c r="H28" s="126" t="n">
         <v>820</v>
       </c>
-      <c r="I28" s="134" t="n">
+      <c r="I28" s="126" t="n">
         <v>775</v>
       </c>
-      <c r="J28" s="135" t="n">
+      <c r="J28" s="126" t="n">
         <v>2.4948</v>
       </c>
     </row>
-    <row r="29" ht="27" customHeight="1" s="120">
-      <c r="A29" s="136" t="n"/>
-      <c r="B29" s="127" t="inlineStr">
+    <row r="29" ht="27" customHeight="1" s="118">
+      <c r="A29" s="132" t="n"/>
+      <c r="B29" s="125" t="inlineStr">
         <is>
           <t>7-7</t>
         </is>
       </c>
-      <c r="C29" s="126" t="inlineStr">
+      <c r="C29" s="124" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D29" s="126" t="inlineStr">
+      <c r="D29" s="124" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E29" s="111" t="n"/>
-      <c r="F29" s="133" t="n">
+      <c r="E29" s="130" t="n"/>
+      <c r="F29" s="126" t="n">
         <v>215</v>
       </c>
-      <c r="G29" s="134" t="n">
+      <c r="G29" s="126" t="n">
         <v>10012.8</v>
       </c>
-      <c r="H29" s="134" t="n">
+      <c r="H29" s="126" t="n">
         <v>797.5</v>
       </c>
-      <c r="I29" s="134" t="n">
+      <c r="I29" s="126" t="n">
         <v>752.5</v>
       </c>
-      <c r="J29" s="135" t="n">
+      <c r="J29" s="126" t="n">
         <v>2.772</v>
       </c>
     </row>
-    <row r="30" ht="27" customHeight="1" s="120">
-      <c r="A30" s="130" t="n"/>
-      <c r="B30" s="130" t="inlineStr">
+    <row r="30" ht="27" customHeight="1" s="118">
+      <c r="A30" s="128" t="n"/>
+      <c r="B30" s="128" t="inlineStr">
         <is>
           <t>TOTAL:</t>
         </is>
       </c>
-      <c r="C30" s="130" t="inlineStr">
+      <c r="C30" s="128" t="inlineStr">
         <is>
           <t>7 PALLETS</t>
         </is>
       </c>
-      <c r="D30" s="130" t="n"/>
-      <c r="E30" s="130" t="n"/>
-      <c r="F30" s="137">
+      <c r="D30" s="128" t="n"/>
+      <c r="E30" s="128" t="n"/>
+      <c r="F30" s="134">
         <f>SUM(F22:F29)</f>
         <v/>
       </c>
-      <c r="G30" s="138">
+      <c r="G30" s="135">
         <f>SUM(G22:G29)</f>
         <v/>
       </c>
-      <c r="H30" s="138">
+      <c r="H30" s="135">
         <f>SUM(H22:H29)</f>
         <v/>
       </c>
-      <c r="I30" s="138">
+      <c r="I30" s="135">
         <f>SUM(I22:I29)</f>
         <v/>
       </c>
-      <c r="J30" s="139">
+      <c r="J30" s="136">
         <f>SUM(J22:J29)</f>
         <v/>
       </c>
     </row>
-    <row r="31" ht="27" customHeight="1" s="120"/>
-    <row r="32" ht="27" customHeight="1" s="120">
-      <c r="A32" s="124" t="inlineStr">
+    <row r="31" ht="27" customHeight="1" s="118"/>
+    <row r="32" ht="27" customHeight="1" s="118">
+      <c r="A32" s="122" t="inlineStr">
         <is>
           <t>Mark &amp; Nº</t>
         </is>
       </c>
-      <c r="B32" s="124" t="inlineStr">
+      <c r="B32" s="122" t="inlineStr">
         <is>
           <t>PALLET
-N.</t>
-        </is>
-      </c>
-      <c r="C32" s="124" t="inlineStr">
+NO.</t>
+        </is>
+      </c>
+      <c r="C32" s="122" t="inlineStr">
         <is>
           <t>P.O Nº</t>
         </is>
       </c>
-      <c r="D32" s="124" t="inlineStr">
+      <c r="D32" s="122" t="inlineStr">
         <is>
           <t>ITEM Nº</t>
         </is>
       </c>
-      <c r="E32" s="124" t="inlineStr">
+      <c r="E32" s="122" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="F32" s="124" t="inlineStr">
+      <c r="F32" s="122" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="G32" s="113" t="n"/>
-      <c r="H32" s="124" t="inlineStr">
+      <c r="G32" s="111" t="n"/>
+      <c r="H32" s="122" t="inlineStr">
         <is>
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="I32" s="124" t="inlineStr">
+      <c r="I32" s="122" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
         </is>
       </c>
-      <c r="J32" s="124" t="inlineStr">
+      <c r="J32" s="122" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
       </c>
     </row>
-    <row r="33" ht="27" customHeight="1" s="120">
-      <c r="A33" s="111" t="n"/>
-      <c r="B33" s="111" t="n"/>
-      <c r="C33" s="111" t="n"/>
-      <c r="D33" s="111" t="n"/>
-      <c r="E33" s="111" t="n"/>
-      <c r="F33" s="124" t="inlineStr">
+    <row r="33" ht="27" customHeight="1" s="118">
+      <c r="A33" s="130" t="n"/>
+      <c r="B33" s="130" t="n"/>
+      <c r="C33" s="130" t="n"/>
+      <c r="D33" s="130" t="n"/>
+      <c r="E33" s="130" t="n"/>
+      <c r="F33" s="122" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
       </c>
-      <c r="G33" s="124" t="inlineStr">
+      <c r="G33" s="122" t="inlineStr">
         <is>
           <t>SF</t>
         </is>
       </c>
-      <c r="H33" s="111" t="n"/>
-      <c r="I33" s="111" t="n"/>
-      <c r="J33" s="111" t="n"/>
-    </row>
-    <row r="34" ht="27" customHeight="1" s="120">
-      <c r="A34" s="132" t="inlineStr">
+      <c r="H33" s="130" t="n"/>
+      <c r="I33" s="130" t="n"/>
+      <c r="J33" s="130" t="n"/>
+    </row>
+    <row r="34" ht="27" customHeight="1" s="118">
+      <c r="A34" s="131" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B34" s="127" t="inlineStr">
+      <c r="B34" s="125" t="inlineStr">
         <is>
           <t>1-11</t>
         </is>
       </c>
-      <c r="C34" s="126" t="inlineStr">
+      <c r="C34" s="124" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D34" s="126" t="inlineStr">
+      <c r="D34" s="124" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E34" s="126" t="inlineStr">
+      <c r="E34" s="124" t="inlineStr">
         <is>
           <t>LEATHER</t>
         </is>
       </c>
-      <c r="F34" s="133" t="n">
+      <c r="F34" s="126" t="n">
         <v>225</v>
       </c>
-      <c r="G34" s="134" t="n">
+      <c r="G34" s="126" t="n">
         <v>10166.7</v>
       </c>
-      <c r="H34" s="134" t="n">
+      <c r="H34" s="126" t="n">
         <v>805.5</v>
       </c>
-      <c r="I34" s="134" t="n">
+      <c r="I34" s="126" t="n">
         <v>760.5</v>
       </c>
-      <c r="J34" s="135" t="n">
+      <c r="J34" s="126" t="n">
         <v>2.4948</v>
       </c>
     </row>
-    <row r="35" ht="27" customHeight="1" s="120">
-      <c r="A35" s="136" t="inlineStr">
+    <row r="35" ht="27" customHeight="1" s="118">
+      <c r="A35" s="132" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B35" s="127" t="inlineStr">
+      <c r="B35" s="125" t="inlineStr">
         <is>
           <t>2-11</t>
         </is>
       </c>
-      <c r="C35" s="126" t="inlineStr">
+      <c r="C35" s="124" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D35" s="126" t="inlineStr">
+      <c r="D35" s="124" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E35" s="110" t="n"/>
-      <c r="F35" s="133" t="n">
+      <c r="E35" s="133" t="n"/>
+      <c r="F35" s="126" t="n">
         <v>225</v>
       </c>
-      <c r="G35" s="134" t="n">
+      <c r="G35" s="126" t="n">
         <v>10363.9</v>
       </c>
-      <c r="H35" s="134" t="n">
+      <c r="H35" s="126" t="n">
         <v>818.5</v>
       </c>
-      <c r="I35" s="134" t="n">
+      <c r="I35" s="126" t="n">
         <v>773.5</v>
       </c>
-      <c r="J35" s="135" t="n">
+      <c r="J35" s="126" t="n">
         <v>2.5344</v>
       </c>
     </row>
-    <row r="36" ht="27" customHeight="1" s="120">
-      <c r="A36" s="136" t="inlineStr">
+    <row r="36" ht="27" customHeight="1" s="118">
+      <c r="A36" s="132" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B36" s="127" t="inlineStr">
+      <c r="B36" s="125" t="inlineStr">
         <is>
           <t>3-11</t>
         </is>
       </c>
-      <c r="C36" s="126" t="inlineStr">
+      <c r="C36" s="124" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D36" s="126" t="inlineStr">
+      <c r="D36" s="124" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E36" s="110" t="n"/>
-      <c r="F36" s="133" t="n">
+      <c r="E36" s="133" t="n"/>
+      <c r="F36" s="126" t="n">
         <v>220</v>
       </c>
-      <c r="G36" s="134" t="n">
+      <c r="G36" s="126" t="n">
         <v>10090.5</v>
       </c>
-      <c r="H36" s="134" t="n">
+      <c r="H36" s="126" t="n">
         <v>809</v>
       </c>
-      <c r="I36" s="134" t="n">
+      <c r="I36" s="126" t="n">
         <v>764</v>
       </c>
-      <c r="J36" s="135" t="n">
+      <c r="J36" s="126" t="n">
         <v>2.6136</v>
       </c>
     </row>
-    <row r="37" ht="27" customHeight="1" s="120">
-      <c r="A37" s="136" t="inlineStr">
+    <row r="37" ht="27" customHeight="1" s="118">
+      <c r="A37" s="132" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B37" s="127" t="inlineStr">
+      <c r="B37" s="125" t="inlineStr">
         <is>
           <t>4-11</t>
         </is>
       </c>
-      <c r="C37" s="126" t="inlineStr">
+      <c r="C37" s="124" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D37" s="126" t="inlineStr">
+      <c r="D37" s="124" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E37" s="110" t="n"/>
-      <c r="F37" s="133" t="n">
+      <c r="E37" s="133" t="n"/>
+      <c r="F37" s="126" t="n">
         <v>194</v>
       </c>
-      <c r="G37" s="134" t="n">
+      <c r="G37" s="126" t="n">
         <v>8956.4</v>
       </c>
-      <c r="H37" s="134" t="n">
+      <c r="H37" s="126" t="n">
         <v>711.5</v>
       </c>
-      <c r="I37" s="134" t="n">
+      <c r="I37" s="126" t="n">
         <v>666.5</v>
       </c>
-      <c r="J37" s="135" t="n">
+      <c r="J37" s="126" t="n">
         <v>2.3364</v>
       </c>
     </row>
-    <row r="38" ht="27" customHeight="1" s="120">
-      <c r="A38" s="136" t="n"/>
-      <c r="B38" s="127" t="inlineStr">
+    <row r="38" ht="27" customHeight="1" s="118">
+      <c r="A38" s="132" t="n"/>
+      <c r="B38" s="125" t="inlineStr">
         <is>
           <t>5-11</t>
         </is>
       </c>
-      <c r="C38" s="126" t="inlineStr">
+      <c r="C38" s="124" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D38" s="126" t="inlineStr">
+      <c r="D38" s="124" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E38" s="110" t="n"/>
-      <c r="F38" s="133" t="n">
+      <c r="E38" s="133" t="n"/>
+      <c r="F38" s="126" t="n">
         <v>220</v>
       </c>
-      <c r="G38" s="134" t="n">
+      <c r="G38" s="126" t="n">
         <v>10072.8</v>
       </c>
-      <c r="H38" s="134" t="n">
+      <c r="H38" s="126" t="n">
         <v>789.5</v>
       </c>
-      <c r="I38" s="134" t="n">
+      <c r="I38" s="126" t="n">
         <v>744.5</v>
       </c>
-      <c r="J38" s="135" t="n">
+      <c r="J38" s="126" t="n">
         <v>2.2968</v>
       </c>
     </row>
-    <row r="39" ht="27" customHeight="1" s="120">
-      <c r="A39" s="136" t="n"/>
-      <c r="B39" s="127" t="inlineStr">
+    <row r="39" ht="27" customHeight="1" s="118">
+      <c r="A39" s="132" t="n"/>
+      <c r="B39" s="125" t="inlineStr">
         <is>
           <t>6-11</t>
         </is>
       </c>
-      <c r="C39" s="126" t="inlineStr">
+      <c r="C39" s="124" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D39" s="126" t="inlineStr">
+      <c r="D39" s="124" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E39" s="110" t="n"/>
-      <c r="F39" s="133" t="n">
+      <c r="E39" s="133" t="n"/>
+      <c r="F39" s="126" t="n">
         <v>255</v>
       </c>
-      <c r="G39" s="134" t="n">
+      <c r="G39" s="126" t="n">
         <v>11907.9</v>
       </c>
-      <c r="H39" s="134" t="n">
+      <c r="H39" s="126" t="n">
         <v>939</v>
       </c>
-      <c r="I39" s="134" t="n">
+      <c r="I39" s="126" t="n">
         <v>894</v>
       </c>
-      <c r="J39" s="135" t="n">
+      <c r="J39" s="126" t="n">
         <v>2.772</v>
       </c>
     </row>
-    <row r="40" ht="27" customHeight="1" s="120">
-      <c r="A40" s="136" t="n"/>
-      <c r="B40" s="127" t="inlineStr">
+    <row r="40" ht="27" customHeight="1" s="118">
+      <c r="A40" s="132" t="n"/>
+      <c r="B40" s="125" t="inlineStr">
         <is>
           <t>7-11</t>
         </is>
       </c>
-      <c r="C40" s="126" t="inlineStr">
+      <c r="C40" s="124" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D40" s="126" t="inlineStr">
+      <c r="D40" s="124" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E40" s="110" t="n"/>
-      <c r="F40" s="133" t="n">
+      <c r="E40" s="133" t="n"/>
+      <c r="F40" s="126" t="n">
         <v>245</v>
       </c>
-      <c r="G40" s="134" t="n">
+      <c r="G40" s="126" t="n">
         <v>11152.3</v>
       </c>
-      <c r="H40" s="134" t="n">
+      <c r="H40" s="126" t="n">
         <v>879.7278</v>
       </c>
-      <c r="I40" s="134" t="n">
+      <c r="I40" s="126" t="n">
         <v>835.2722</v>
       </c>
-      <c r="J40" s="135" t="n">
+      <c r="J40" s="126" t="n">
         <v>2.5037</v>
       </c>
     </row>
-    <row r="41" ht="27" customHeight="1" s="120">
-      <c r="A41" s="136" t="n"/>
-      <c r="B41" s="111" t="n"/>
-      <c r="C41" s="126" t="inlineStr">
+    <row r="41" ht="27" customHeight="1" s="118">
+      <c r="A41" s="132" t="n"/>
+      <c r="B41" s="130" t="n"/>
+      <c r="C41" s="124" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D41" s="126" t="inlineStr">
+      <c r="D41" s="124" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E41" s="110" t="n"/>
-      <c r="F41" s="133" t="n">
+      <c r="E41" s="133" t="n"/>
+      <c r="F41" s="126" t="n">
         <v>3</v>
       </c>
-      <c r="G41" s="134" t="n">
+      <c r="G41" s="126" t="n">
         <v>113.7</v>
       </c>
-      <c r="H41" s="134" t="n">
+      <c r="H41" s="126" t="n">
         <v>10.7722</v>
       </c>
-      <c r="I41" s="134" t="n">
+      <c r="I41" s="126" t="n">
         <v>10.2278</v>
       </c>
-      <c r="J41" s="135" t="n">
+      <c r="J41" s="126" t="n">
         <v>0.0307</v>
       </c>
     </row>
-    <row r="42" ht="27" customHeight="1" s="120">
-      <c r="A42" s="136" t="n"/>
-      <c r="B42" s="127" t="inlineStr">
+    <row r="42" ht="27" customHeight="1" s="118">
+      <c r="A42" s="132" t="n"/>
+      <c r="B42" s="125" t="inlineStr">
         <is>
           <t>8-11</t>
         </is>
       </c>
-      <c r="C42" s="126" t="inlineStr">
+      <c r="C42" s="124" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D42" s="126" t="inlineStr">
+      <c r="D42" s="124" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E42" s="110" t="n"/>
-      <c r="F42" s="133" t="n">
+      <c r="E42" s="133" t="n"/>
+      <c r="F42" s="126" t="n">
         <v>232</v>
       </c>
-      <c r="G42" s="134" t="n">
+      <c r="G42" s="126" t="n">
         <v>11138.3</v>
       </c>
-      <c r="H42" s="134" t="n">
+      <c r="H42" s="126" t="n">
         <v>872.5</v>
       </c>
-      <c r="I42" s="134" t="n">
+      <c r="I42" s="126" t="n">
         <v>827.5</v>
       </c>
-      <c r="J42" s="135" t="n">
+      <c r="J42" s="126" t="n">
         <v>2.5344</v>
       </c>
     </row>
-    <row r="43" ht="27" customHeight="1" s="120">
-      <c r="A43" s="136" t="n"/>
-      <c r="B43" s="127" t="inlineStr">
+    <row r="43" ht="27" customHeight="1" s="118">
+      <c r="A43" s="132" t="n"/>
+      <c r="B43" s="125" t="inlineStr">
         <is>
           <t>9-11</t>
         </is>
       </c>
-      <c r="C43" s="126" t="inlineStr">
+      <c r="C43" s="124" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D43" s="126" t="inlineStr">
+      <c r="D43" s="124" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E43" s="110" t="n"/>
-      <c r="F43" s="133" t="n">
+      <c r="E43" s="133" t="n"/>
+      <c r="F43" s="126" t="n">
         <v>210</v>
       </c>
-      <c r="G43" s="134" t="n">
+      <c r="G43" s="126" t="n">
         <v>9969.5</v>
       </c>
-      <c r="H43" s="134" t="n">
+      <c r="H43" s="126" t="n">
         <v>786.5</v>
       </c>
-      <c r="I43" s="134" t="n">
+      <c r="I43" s="126" t="n">
         <v>741.5</v>
       </c>
-      <c r="J43" s="135" t="n">
+      <c r="J43" s="126" t="n">
         <v>2.376</v>
       </c>
     </row>
-    <row r="44" ht="27" customHeight="1" s="120">
-      <c r="A44" s="136" t="n"/>
-      <c r="B44" s="127" t="inlineStr">
+    <row r="44" ht="27" customHeight="1" s="118">
+      <c r="A44" s="132" t="n"/>
+      <c r="B44" s="125" t="inlineStr">
         <is>
           <t>10-11</t>
         </is>
       </c>
-      <c r="C44" s="126" t="inlineStr">
+      <c r="C44" s="124" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D44" s="126" t="inlineStr">
+      <c r="D44" s="124" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E44" s="110" t="n"/>
-      <c r="F44" s="133" t="n">
+      <c r="E44" s="133" t="n"/>
+      <c r="F44" s="126" t="n">
         <v>235</v>
       </c>
-      <c r="G44" s="134" t="n">
+      <c r="G44" s="126" t="n">
         <v>11202.6</v>
       </c>
-      <c r="H44" s="134" t="n">
+      <c r="H44" s="126" t="n">
         <v>884</v>
       </c>
-      <c r="I44" s="134" t="n">
+      <c r="I44" s="126" t="n">
         <v>839</v>
       </c>
-      <c r="J44" s="135" t="n">
+      <c r="J44" s="126" t="n">
         <v>2.376</v>
       </c>
     </row>
-    <row r="45" ht="27" customHeight="1" s="120">
-      <c r="A45" s="136" t="n"/>
-      <c r="B45" s="127" t="inlineStr">
+    <row r="45" ht="27" customHeight="1" s="118">
+      <c r="A45" s="132" t="n"/>
+      <c r="B45" s="125" t="inlineStr">
         <is>
           <t>11-11</t>
         </is>
       </c>
-      <c r="C45" s="126" t="inlineStr">
+      <c r="C45" s="124" t="inlineStr">
         <is>
           <t>GYOJY_M25371</t>
         </is>
       </c>
-      <c r="D45" s="126" t="inlineStr">
+      <c r="D45" s="124" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E45" s="111" t="n"/>
-      <c r="F45" s="133" t="n">
+      <c r="E45" s="130" t="n"/>
+      <c r="F45" s="126" t="n">
         <v>235</v>
       </c>
-      <c r="G45" s="134" t="n">
+      <c r="G45" s="126" t="n">
         <v>11138.7</v>
       </c>
-      <c r="H45" s="134" t="n">
+      <c r="H45" s="126" t="n">
         <v>878</v>
       </c>
-      <c r="I45" s="134" t="n">
+      <c r="I45" s="126" t="n">
         <v>833</v>
       </c>
-      <c r="J45" s="135" t="n">
+      <c r="J45" s="126" t="n">
         <v>2.376</v>
       </c>
     </row>
-    <row r="46" ht="27" customHeight="1" s="120">
-      <c r="A46" s="130" t="n"/>
-      <c r="B46" s="130" t="inlineStr">
+    <row r="46" ht="27" customHeight="1" s="118">
+      <c r="A46" s="128" t="n"/>
+      <c r="B46" s="128" t="inlineStr">
         <is>
           <t>TOTAL:</t>
         </is>
       </c>
-      <c r="C46" s="130" t="inlineStr">
+      <c r="C46" s="128" t="inlineStr">
         <is>
           <t>11 PALLETS</t>
         </is>
       </c>
-      <c r="D46" s="130" t="n"/>
-      <c r="E46" s="130" t="n"/>
-      <c r="F46" s="137">
+      <c r="D46" s="128" t="n"/>
+      <c r="E46" s="128" t="n"/>
+      <c r="F46" s="134">
         <f>SUM(F34:F45)</f>
         <v/>
       </c>
-      <c r="G46" s="138">
+      <c r="G46" s="135">
         <f>SUM(G34:G45)</f>
         <v/>
       </c>
-      <c r="H46" s="138">
+      <c r="H46" s="135">
         <f>SUM(H34:H45)</f>
         <v/>
       </c>
-      <c r="I46" s="138">
+      <c r="I46" s="135">
         <f>SUM(I34:I45)</f>
         <v/>
       </c>
-      <c r="J46" s="139">
+      <c r="J46" s="136">
         <f>SUM(J34:J45)</f>
         <v/>
       </c>
     </row>
-    <row r="47" ht="27" customHeight="1" s="120"/>
-    <row r="48" ht="27" customHeight="1" s="120">
-      <c r="A48" s="124" t="inlineStr">
+    <row r="47" ht="27" customHeight="1" s="118"/>
+    <row r="48" ht="27" customHeight="1" s="118">
+      <c r="A48" s="122" t="inlineStr">
         <is>
           <t>Mark &amp; Nº</t>
         </is>
       </c>
-      <c r="B48" s="124" t="inlineStr">
+      <c r="B48" s="122" t="inlineStr">
         <is>
           <t>PALLET
-N.</t>
-        </is>
-      </c>
-      <c r="C48" s="124" t="inlineStr">
+NO.</t>
+        </is>
+      </c>
+      <c r="C48" s="122" t="inlineStr">
         <is>
           <t>P.O Nº</t>
         </is>
       </c>
-      <c r="D48" s="124" t="inlineStr">
+      <c r="D48" s="122" t="inlineStr">
         <is>
           <t>ITEM Nº</t>
         </is>
       </c>
-      <c r="E48" s="124" t="inlineStr">
+      <c r="E48" s="122" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="F48" s="124" t="inlineStr">
+      <c r="F48" s="122" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="G48" s="113" t="n"/>
-      <c r="H48" s="124" t="inlineStr">
+      <c r="G48" s="111" t="n"/>
+      <c r="H48" s="122" t="inlineStr">
         <is>
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="I48" s="124" t="inlineStr">
+      <c r="I48" s="122" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
         </is>
       </c>
-      <c r="J48" s="124" t="inlineStr">
+      <c r="J48" s="122" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
       </c>
     </row>
-    <row r="49" ht="27" customHeight="1" s="120">
-      <c r="A49" s="111" t="n"/>
-      <c r="B49" s="111" t="n"/>
-      <c r="C49" s="111" t="n"/>
-      <c r="D49" s="111" t="n"/>
-      <c r="E49" s="111" t="n"/>
-      <c r="F49" s="124" t="inlineStr">
+    <row r="49" ht="27" customHeight="1" s="118">
+      <c r="A49" s="130" t="n"/>
+      <c r="B49" s="130" t="n"/>
+      <c r="C49" s="130" t="n"/>
+      <c r="D49" s="130" t="n"/>
+      <c r="E49" s="130" t="n"/>
+      <c r="F49" s="122" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
       </c>
-      <c r="G49" s="124" t="inlineStr">
+      <c r="G49" s="122" t="inlineStr">
         <is>
           <t>SF</t>
         </is>
       </c>
-      <c r="H49" s="111" t="n"/>
-      <c r="I49" s="111" t="n"/>
-      <c r="J49" s="111" t="n"/>
-    </row>
-    <row r="50" ht="27" customHeight="1" s="120">
-      <c r="A50" s="132" t="inlineStr">
+      <c r="H49" s="130" t="n"/>
+      <c r="I49" s="130" t="n"/>
+      <c r="J49" s="130" t="n"/>
+    </row>
+    <row r="50" ht="27" customHeight="1" s="118">
+      <c r="A50" s="131" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B50" s="127" t="inlineStr">
+      <c r="B50" s="125" t="inlineStr">
         <is>
           <t>1-4</t>
         </is>
       </c>
-      <c r="C50" s="126" t="inlineStr">
+      <c r="C50" s="124" t="inlineStr">
         <is>
           <t>GYOJY_M25374</t>
         </is>
       </c>
-      <c r="D50" s="126" t="inlineStr">
+      <c r="D50" s="124" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E50" s="126" t="inlineStr">
+      <c r="E50" s="124" t="inlineStr">
         <is>
           <t>LEATHER</t>
         </is>
       </c>
-      <c r="F50" s="133" t="n">
+      <c r="F50" s="126" t="n">
         <v>240</v>
       </c>
-      <c r="G50" s="134" t="n">
+      <c r="G50" s="126" t="n">
         <v>11235.9</v>
       </c>
-      <c r="H50" s="134" t="n">
+      <c r="H50" s="126" t="n">
         <v>874.5</v>
       </c>
-      <c r="I50" s="134" t="n">
+      <c r="I50" s="126" t="n">
         <v>829.5</v>
       </c>
-      <c r="J50" s="135" t="n">
+      <c r="J50" s="126" t="n">
         <v>2.772</v>
       </c>
     </row>
-    <row r="51" ht="27" customHeight="1" s="120">
-      <c r="A51" s="136" t="inlineStr">
+    <row r="51" ht="27" customHeight="1" s="118">
+      <c r="A51" s="132" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B51" s="127" t="inlineStr">
+      <c r="B51" s="125" t="inlineStr">
         <is>
           <t>2-4</t>
         </is>
       </c>
-      <c r="C51" s="126" t="inlineStr">
+      <c r="C51" s="124" t="inlineStr">
         <is>
           <t>GYOJY_M25374</t>
         </is>
       </c>
-      <c r="D51" s="126" t="inlineStr">
+      <c r="D51" s="124" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E51" s="110" t="n"/>
-      <c r="F51" s="133" t="n">
+      <c r="E51" s="133" t="n"/>
+      <c r="F51" s="126" t="n">
         <v>230</v>
       </c>
-      <c r="G51" s="134" t="n">
+      <c r="G51" s="126" t="n">
         <v>11142</v>
       </c>
-      <c r="H51" s="134" t="n">
+      <c r="H51" s="126" t="n">
         <v>865.5</v>
       </c>
-      <c r="I51" s="134" t="n">
+      <c r="I51" s="126" t="n">
         <v>820.5</v>
       </c>
-      <c r="J51" s="135" t="n">
+      <c r="J51" s="126" t="n">
         <v>2.6136</v>
       </c>
     </row>
-    <row r="52" ht="27" customHeight="1" s="120">
-      <c r="A52" s="136" t="inlineStr">
+    <row r="52" ht="27" customHeight="1" s="118">
+      <c r="A52" s="132" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B52" s="127" t="inlineStr">
+      <c r="B52" s="125" t="inlineStr">
         <is>
           <t>3-4</t>
         </is>
       </c>
-      <c r="C52" s="126" t="inlineStr">
+      <c r="C52" s="124" t="inlineStr">
         <is>
           <t>GYOJY_M25374</t>
         </is>
       </c>
-      <c r="D52" s="126" t="inlineStr">
+      <c r="D52" s="124" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E52" s="110" t="n"/>
-      <c r="F52" s="133" t="n">
+      <c r="E52" s="133" t="n"/>
+      <c r="F52" s="126" t="n">
         <v>235</v>
       </c>
-      <c r="G52" s="134" t="n">
+      <c r="G52" s="126" t="n">
         <v>11237.6</v>
       </c>
-      <c r="H52" s="134" t="n">
+      <c r="H52" s="126" t="n">
         <v>868.5</v>
       </c>
-      <c r="I52" s="134" t="n">
+      <c r="I52" s="126" t="n">
         <v>823.5</v>
       </c>
-      <c r="J52" s="135" t="n">
+      <c r="J52" s="126" t="n">
         <v>2.574</v>
       </c>
     </row>
-    <row r="53" ht="27" customHeight="1" s="120">
-      <c r="A53" s="136" t="inlineStr">
+    <row r="53" ht="27" customHeight="1" s="118">
+      <c r="A53" s="132" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B53" s="127" t="inlineStr">
+      <c r="B53" s="125" t="inlineStr">
         <is>
           <t>4-4</t>
         </is>
       </c>
-      <c r="C53" s="126" t="inlineStr">
+      <c r="C53" s="124" t="inlineStr">
         <is>
           <t>GYOJY_M25374</t>
         </is>
       </c>
-      <c r="D53" s="126" t="inlineStr">
+      <c r="D53" s="124" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E53" s="110" t="n"/>
-      <c r="F53" s="133" t="n">
+      <c r="E53" s="133" t="n"/>
+      <c r="F53" s="126" t="n">
         <v>99</v>
       </c>
-      <c r="G53" s="134" t="n">
+      <c r="G53" s="126" t="n">
         <v>4814.5</v>
       </c>
-      <c r="H53" s="134" t="n">
+      <c r="H53" s="126" t="n">
         <v>401.5</v>
       </c>
-      <c r="I53" s="134" t="n">
+      <c r="I53" s="126" t="n">
         <v>360.25</v>
       </c>
-      <c r="J53" s="135" t="n">
+      <c r="J53" s="126" t="n">
         <v>2.178</v>
       </c>
     </row>
-    <row r="54" ht="27" customHeight="1" s="120">
-      <c r="A54" s="136" t="n"/>
-      <c r="B54" s="111" t="n"/>
-      <c r="C54" s="126" t="inlineStr">
+    <row r="54" ht="27" customHeight="1" s="118">
+      <c r="A54" s="132" t="n"/>
+      <c r="B54" s="130" t="n"/>
+      <c r="C54" s="124" t="inlineStr">
         <is>
           <t>GYOJY_M25374</t>
         </is>
       </c>
-      <c r="D54" s="126" t="inlineStr">
+      <c r="D54" s="124" t="inlineStr">
         <is>
           <t>Nick Dove</t>
         </is>
       </c>
-      <c r="E54" s="111" t="n"/>
-      <c r="F54" s="133" t="n">
+      <c r="E54" s="130" t="n"/>
+      <c r="F54" s="126" t="n">
         <v>9</v>
       </c>
-      <c r="G54" s="134" t="n">
+      <c r="G54" s="126" t="n">
         <v>411.3</v>
       </c>
-      <c r="H54" s="134" t="n">
+      <c r="H54" s="126" t="n">
         <v>36.5</v>
       </c>
-      <c r="I54" s="134" t="n">
+      <c r="I54" s="126" t="n">
         <v>32.75</v>
       </c>
-      <c r="J54" s="135" t="n">
+      <c r="J54" s="126" t="n">
         <v>0.198</v>
       </c>
     </row>
-    <row r="55" ht="27" customHeight="1" s="120">
-      <c r="A55" s="130" t="n"/>
-      <c r="B55" s="130" t="inlineStr">
+    <row r="55" ht="27" customHeight="1" s="118">
+      <c r="A55" s="128" t="n"/>
+      <c r="B55" s="128" t="inlineStr">
         <is>
           <t>TOTAL:</t>
         </is>
       </c>
-      <c r="C55" s="130" t="inlineStr">
+      <c r="C55" s="128" t="inlineStr">
         <is>
           <t>4 PALLETS</t>
         </is>
       </c>
-      <c r="D55" s="130" t="n"/>
-      <c r="E55" s="130" t="n"/>
-      <c r="F55" s="137">
+      <c r="D55" s="128" t="n"/>
+      <c r="E55" s="128" t="n"/>
+      <c r="F55" s="134">
         <f>SUM(F50:F54)</f>
         <v/>
       </c>
-      <c r="G55" s="138">
+      <c r="G55" s="135">
         <f>SUM(G50:G54)</f>
         <v/>
       </c>
-      <c r="H55" s="138">
+      <c r="H55" s="135">
         <f>SUM(H50:H54)</f>
         <v/>
       </c>
-      <c r="I55" s="138">
+      <c r="I55" s="135">
         <f>SUM(I50:I54)</f>
         <v/>
       </c>
-      <c r="J55" s="139">
+      <c r="J55" s="136">
         <f>SUM(J50:J54)</f>
         <v/>
       </c>
     </row>
-    <row r="56" ht="27" customHeight="1" s="120">
-      <c r="B56" s="140" t="inlineStr">
+    <row r="56" ht="27" customHeight="1" s="118">
+      <c r="B56" s="137" t="inlineStr">
         <is>
           <t>TOTAL OF:</t>
         </is>
       </c>
-      <c r="C56" s="140" t="inlineStr">
+      <c r="C56" s="137" t="inlineStr">
         <is>
           <t>22 PALLETS</t>
         </is>
       </c>
-      <c r="F56" s="141">
+      <c r="F56" s="138">
         <f>SUM(F22:F29,F34:F45,F50:F54)</f>
         <v/>
       </c>
-      <c r="G56" s="142">
+      <c r="G56" s="138">
         <f>SUM(G22:G29,G34:G45,G50:G54)</f>
         <v/>
       </c>
-      <c r="H56" s="142">
+      <c r="H56" s="138">
         <f>SUM(H22:H29,H34:H45,H50:H54)</f>
         <v/>
       </c>
-      <c r="I56" s="142">
+      <c r="I56" s="138">
         <f>SUM(I22:I29,I34:I45,I50:I54)</f>
         <v/>
       </c>
-      <c r="J56" s="143">
+      <c r="J56" s="138">
         <f>SUM(J22:J29,J34:J45,J50:J54)</f>
         <v/>
       </c>
@@ -5308,7 +5039,7 @@
       <c r="I57" s="20" t="n"/>
       <c r="J57" s="32" t="n"/>
     </row>
-    <row r="58" ht="35.1" customHeight="1" s="120">
+    <row r="58" ht="35.1" customHeight="1" s="118">
       <c r="A58" s="86" t="inlineStr">
         <is>
           <t xml:space="preserve">Country of Original Cambodia </t>
@@ -5324,7 +5055,7 @@
       <c r="L58" s="6" t="n"/>
       <c r="M58" s="33" t="n"/>
     </row>
-    <row r="59" ht="72" customHeight="1" s="120">
+    <row r="59" ht="72" customHeight="1" s="118">
       <c r="A59" s="22" t="inlineStr">
         <is>
           <t>Manufacture:</t>
@@ -5347,7 +5078,7 @@
       <c r="L59" s="6" t="n"/>
       <c r="M59" s="33" t="n"/>
     </row>
-    <row r="60" ht="48" customHeight="1" s="120">
+    <row r="60" ht="48" customHeight="1" s="118">
       <c r="A60" s="88" t="inlineStr">
         <is>
           <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
@@ -5364,14 +5095,14 @@
       <c r="L60" s="83" t="n"/>
       <c r="M60" s="33" t="n"/>
     </row>
-    <row r="61" ht="30" customHeight="1" s="120">
+    <row r="61" ht="30" customHeight="1" s="118">
       <c r="A61" s="83" t="inlineStr">
         <is>
           <t>A/C NO:100001100764430</t>
         </is>
       </c>
     </row>
-    <row r="62" ht="32.1" customHeight="1" s="120">
+    <row r="62" ht="32.1" customHeight="1" s="118">
       <c r="A62" s="83" t="inlineStr">
         <is>
           <t>SWIFT CODE  ：BKCHKHPPXXX</t>
@@ -5543,7 +5274,44 @@
     <row r="197"/>
     <row r="198"/>
     <row r="199"/>
-    <row r="200" ht="42" customHeight="1" s="120"/>
+    <row r="200" ht="42" customHeight="1" s="118"/>
+    <row r="201"/>
+    <row r="202"/>
+    <row r="203"/>
+    <row r="204"/>
+    <row r="205"/>
+    <row r="206"/>
+    <row r="207"/>
+    <row r="208"/>
+    <row r="209"/>
+    <row r="210"/>
+    <row r="211"/>
+    <row r="212"/>
+    <row r="213"/>
+    <row r="214"/>
+    <row r="215"/>
+    <row r="216"/>
+    <row r="217"/>
+    <row r="218"/>
+    <row r="219"/>
+    <row r="220"/>
+    <row r="221"/>
+    <row r="222"/>
+    <row r="223"/>
+    <row r="224"/>
+    <row r="225"/>
+    <row r="226"/>
+    <row r="227"/>
+    <row r="228"/>
+    <row r="229"/>
+    <row r="230"/>
+    <row r="231"/>
+    <row r="232"/>
+    <row r="233"/>
+    <row r="234"/>
+    <row r="235"/>
+    <row r="236"/>
+    <row r="237"/>
   </sheetData>
   <mergeCells count="52">
     <mergeCell ref="I32:I33"/>

</xml_diff>

<commit_message>
adding new feature that allow verticle merging for same value ajection
</commit_message>
<xml_diff>
--- a/invoice_gen/result.xlsx
+++ b/invoice_gen/result.xlsx
@@ -280,7 +280,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -359,6 +359,39 @@
         <color rgb="00000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
@@ -367,7 +400,7 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -653,9 +686,11 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2014,21 +2049,9 @@
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B23" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C23" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D23" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B23" s="103" t="n"/>
+      <c r="C23" s="103" t="n"/>
+      <c r="D23" s="103" t="n"/>
       <c r="E23" s="99" t="n">
         <v>153</v>
       </c>
@@ -2048,21 +2071,9 @@
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B24" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C24" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D24" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B24" s="103" t="n"/>
+      <c r="C24" s="103" t="n"/>
+      <c r="D24" s="103" t="n"/>
       <c r="E24" s="99" t="n">
         <v>156</v>
       </c>
@@ -2082,21 +2093,9 @@
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B25" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C25" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D25" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B25" s="103" t="n"/>
+      <c r="C25" s="103" t="n"/>
+      <c r="D25" s="103" t="n"/>
       <c r="E25" s="99" t="n">
         <v>145</v>
       </c>
@@ -2112,21 +2111,9 @@
     </row>
     <row r="26" ht="27" customHeight="1" s="83">
       <c r="A26" s="102" t="n"/>
-      <c r="B26" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C26" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D26" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B26" s="103" t="n"/>
+      <c r="C26" s="103" t="n"/>
+      <c r="D26" s="103" t="n"/>
       <c r="E26" s="99" t="n">
         <v>166</v>
       </c>
@@ -2142,21 +2129,9 @@
     </row>
     <row r="27" ht="27" customHeight="1" s="83">
       <c r="A27" s="102" t="n"/>
-      <c r="B27" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C27" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D27" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B27" s="103" t="n"/>
+      <c r="C27" s="103" t="n"/>
+      <c r="D27" s="103" t="n"/>
       <c r="E27" s="99" t="n">
         <v>156</v>
       </c>
@@ -2172,21 +2147,9 @@
     </row>
     <row r="28" ht="27" customHeight="1" s="83">
       <c r="A28" s="102" t="n"/>
-      <c r="B28" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C28" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D28" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B28" s="103" t="n"/>
+      <c r="C28" s="103" t="n"/>
+      <c r="D28" s="103" t="n"/>
       <c r="E28" s="99" t="n">
         <v>149</v>
       </c>
@@ -2202,21 +2165,9 @@
     </row>
     <row r="29" ht="27" customHeight="1" s="83">
       <c r="A29" s="102" t="n"/>
-      <c r="B29" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C29" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D29" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B29" s="103" t="n"/>
+      <c r="C29" s="103" t="n"/>
+      <c r="D29" s="103" t="n"/>
       <c r="E29" s="99" t="n">
         <v>157</v>
       </c>
@@ -2232,21 +2183,9 @@
     </row>
     <row r="30" ht="27" customHeight="1" s="83">
       <c r="A30" s="102" t="n"/>
-      <c r="B30" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C30" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D30" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B30" s="103" t="n"/>
+      <c r="C30" s="103" t="n"/>
+      <c r="D30" s="103" t="n"/>
       <c r="E30" s="99" t="n">
         <v>148</v>
       </c>
@@ -2262,21 +2201,9 @@
     </row>
     <row r="31" ht="27" customHeight="1" s="83">
       <c r="A31" s="102" t="n"/>
-      <c r="B31" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C31" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D31" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B31" s="103" t="n"/>
+      <c r="C31" s="103" t="n"/>
+      <c r="D31" s="103" t="n"/>
       <c r="E31" s="99" t="n">
         <v>157</v>
       </c>
@@ -2292,21 +2219,9 @@
     </row>
     <row r="32" ht="27" customHeight="1" s="83">
       <c r="A32" s="102" t="n"/>
-      <c r="B32" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C32" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D32" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B32" s="103" t="n"/>
+      <c r="C32" s="103" t="n"/>
+      <c r="D32" s="103" t="n"/>
       <c r="E32" s="99" t="n">
         <v>172</v>
       </c>
@@ -2322,21 +2237,9 @@
     </row>
     <row r="33" ht="27" customHeight="1" s="83">
       <c r="A33" s="102" t="n"/>
-      <c r="B33" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C33" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D33" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B33" s="103" t="n"/>
+      <c r="C33" s="103" t="n"/>
+      <c r="D33" s="103" t="n"/>
       <c r="E33" s="99" t="n">
         <v>130</v>
       </c>
@@ -2351,22 +2254,10 @@
       </c>
     </row>
     <row r="34" ht="27" customHeight="1" s="83">
-      <c r="A34" s="103" t="n"/>
-      <c r="B34" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C34" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D34" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="A34" s="104" t="n"/>
+      <c r="B34" s="105" t="n"/>
+      <c r="C34" s="105" t="n"/>
+      <c r="D34" s="105" t="n"/>
       <c r="E34" s="99" t="n">
         <v>158</v>
       </c>
@@ -2381,31 +2272,31 @@
       </c>
     </row>
     <row r="35" ht="35" customHeight="1" s="83">
-      <c r="A35" s="104" t="n"/>
-      <c r="B35" s="104" t="inlineStr">
+      <c r="A35" s="106" t="n"/>
+      <c r="B35" s="106" t="inlineStr">
         <is>
           <t>SUB TOTAL:</t>
         </is>
       </c>
-      <c r="C35" s="104" t="inlineStr">
+      <c r="C35" s="106" t="inlineStr">
         <is>
           <t>13 PALLETS</t>
         </is>
       </c>
-      <c r="D35" s="104" t="n"/>
-      <c r="E35" s="104">
+      <c r="D35" s="106" t="n"/>
+      <c r="E35" s="106">
         <f>SUM(E22:E34)</f>
         <v/>
       </c>
-      <c r="F35" s="104">
+      <c r="F35" s="106">
         <f>SUM(F22:F34)</f>
         <v/>
       </c>
-      <c r="G35" s="104">
+      <c r="G35" s="106">
         <f>SUM(G22:G34)</f>
         <v/>
       </c>
-      <c r="H35" s="104">
+      <c r="H35" s="106">
         <f>SUM(H22:H34)</f>
         <v/>
       </c>
@@ -2492,21 +2383,9 @@
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B39" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C39" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D39" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B39" s="103" t="n"/>
+      <c r="C39" s="103" t="n"/>
+      <c r="D39" s="103" t="n"/>
       <c r="E39" s="99" t="n">
         <v>173</v>
       </c>
@@ -2526,21 +2405,9 @@
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B40" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C40" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D40" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B40" s="103" t="n"/>
+      <c r="C40" s="103" t="n"/>
+      <c r="D40" s="103" t="n"/>
       <c r="E40" s="99" t="n">
         <v>195</v>
       </c>
@@ -2560,21 +2427,9 @@
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B41" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C41" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D41" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B41" s="103" t="n"/>
+      <c r="C41" s="103" t="n"/>
+      <c r="D41" s="103" t="n"/>
       <c r="E41" s="99" t="n">
         <v>155</v>
       </c>
@@ -2590,21 +2445,9 @@
     </row>
     <row r="42" ht="27" customHeight="1" s="83">
       <c r="A42" s="102" t="n"/>
-      <c r="B42" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C42" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D42" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B42" s="103" t="n"/>
+      <c r="C42" s="103" t="n"/>
+      <c r="D42" s="103" t="n"/>
       <c r="E42" s="99" t="n">
         <v>152</v>
       </c>
@@ -2620,21 +2463,9 @@
     </row>
     <row r="43" ht="27" customHeight="1" s="83">
       <c r="A43" s="102" t="n"/>
-      <c r="B43" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C43" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D43" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B43" s="103" t="n"/>
+      <c r="C43" s="103" t="n"/>
+      <c r="D43" s="103" t="n"/>
       <c r="E43" s="99" t="n">
         <v>154</v>
       </c>
@@ -2650,21 +2481,9 @@
     </row>
     <row r="44" ht="27" customHeight="1" s="83">
       <c r="A44" s="102" t="n"/>
-      <c r="B44" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C44" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D44" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B44" s="103" t="n"/>
+      <c r="C44" s="103" t="n"/>
+      <c r="D44" s="103" t="n"/>
       <c r="E44" s="99" t="n">
         <v>138</v>
       </c>
@@ -2680,21 +2499,9 @@
     </row>
     <row r="45" ht="27" customHeight="1" s="83">
       <c r="A45" s="102" t="n"/>
-      <c r="B45" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C45" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D45" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B45" s="103" t="n"/>
+      <c r="C45" s="103" t="n"/>
+      <c r="D45" s="103" t="n"/>
       <c r="E45" s="99" t="n">
         <v>150</v>
       </c>
@@ -2710,21 +2517,9 @@
     </row>
     <row r="46" ht="27" customHeight="1" s="83">
       <c r="A46" s="102" t="n"/>
-      <c r="B46" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C46" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D46" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B46" s="103" t="n"/>
+      <c r="C46" s="103" t="n"/>
+      <c r="D46" s="103" t="n"/>
       <c r="E46" s="99" t="n">
         <v>139</v>
       </c>
@@ -2740,21 +2535,9 @@
     </row>
     <row r="47" ht="27" customHeight="1" s="83">
       <c r="A47" s="102" t="n"/>
-      <c r="B47" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C47" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D47" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B47" s="103" t="n"/>
+      <c r="C47" s="103" t="n"/>
+      <c r="D47" s="103" t="n"/>
       <c r="E47" s="99" t="n">
         <v>183</v>
       </c>
@@ -2770,21 +2553,9 @@
     </row>
     <row r="48" ht="27" customHeight="1" s="83">
       <c r="A48" s="102" t="n"/>
-      <c r="B48" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C48" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D48" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B48" s="103" t="n"/>
+      <c r="C48" s="103" t="n"/>
+      <c r="D48" s="103" t="n"/>
       <c r="E48" s="99" t="n">
         <v>148</v>
       </c>
@@ -2800,21 +2571,9 @@
     </row>
     <row r="49" ht="27" customHeight="1" s="83">
       <c r="A49" s="102" t="n"/>
-      <c r="B49" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C49" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D49" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B49" s="103" t="n"/>
+      <c r="C49" s="103" t="n"/>
+      <c r="D49" s="103" t="n"/>
       <c r="E49" s="99" t="n">
         <v>137</v>
       </c>
@@ -2829,22 +2588,10 @@
       </c>
     </row>
     <row r="50" ht="27" customHeight="1" s="83">
-      <c r="A50" s="103" t="n"/>
-      <c r="B50" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C50" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D50" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="A50" s="104" t="n"/>
+      <c r="B50" s="105" t="n"/>
+      <c r="C50" s="105" t="n"/>
+      <c r="D50" s="105" t="n"/>
       <c r="E50" s="99" t="n">
         <v>174</v>
       </c>
@@ -2859,31 +2606,31 @@
       </c>
     </row>
     <row r="51" ht="35" customHeight="1" s="83">
-      <c r="A51" s="104" t="n"/>
-      <c r="B51" s="104" t="inlineStr">
+      <c r="A51" s="106" t="n"/>
+      <c r="B51" s="106" t="inlineStr">
         <is>
           <t>SUB TOTAL:</t>
         </is>
       </c>
-      <c r="C51" s="104" t="inlineStr">
+      <c r="C51" s="106" t="inlineStr">
         <is>
           <t>13 PALLETS</t>
         </is>
       </c>
-      <c r="D51" s="104" t="n"/>
-      <c r="E51" s="104">
+      <c r="D51" s="106" t="n"/>
+      <c r="E51" s="106">
         <f>SUM(E38:E50)</f>
         <v/>
       </c>
-      <c r="F51" s="104">
+      <c r="F51" s="106">
         <f>SUM(F38:F50)</f>
         <v/>
       </c>
-      <c r="G51" s="104">
+      <c r="G51" s="106">
         <f>SUM(G38:G50)</f>
         <v/>
       </c>
-      <c r="H51" s="104">
+      <c r="H51" s="106">
         <f>SUM(H38:H50)</f>
         <v/>
       </c>
@@ -2970,21 +2717,9 @@
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B55" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C55" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D55" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B55" s="103" t="n"/>
+      <c r="C55" s="103" t="n"/>
+      <c r="D55" s="103" t="n"/>
       <c r="E55" s="99" t="n">
         <v>160</v>
       </c>
@@ -3004,21 +2739,9 @@
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B56" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C56" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D56" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B56" s="103" t="n"/>
+      <c r="C56" s="103" t="n"/>
+      <c r="D56" s="103" t="n"/>
       <c r="E56" s="99" t="n">
         <v>157</v>
       </c>
@@ -3038,21 +2761,9 @@
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B57" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C57" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D57" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B57" s="103" t="n"/>
+      <c r="C57" s="103" t="n"/>
+      <c r="D57" s="103" t="n"/>
       <c r="E57" s="99" t="n">
         <v>163</v>
       </c>
@@ -3068,21 +2779,9 @@
     </row>
     <row r="58" ht="27" customHeight="1" s="83">
       <c r="A58" s="102" t="n"/>
-      <c r="B58" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C58" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D58" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B58" s="103" t="n"/>
+      <c r="C58" s="103" t="n"/>
+      <c r="D58" s="103" t="n"/>
       <c r="E58" s="99" t="n">
         <v>149</v>
       </c>
@@ -3098,21 +2797,9 @@
     </row>
     <row r="59" ht="27" customHeight="1" s="83">
       <c r="A59" s="102" t="n"/>
-      <c r="B59" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C59" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D59" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B59" s="103" t="n"/>
+      <c r="C59" s="103" t="n"/>
+      <c r="D59" s="103" t="n"/>
       <c r="E59" s="99" t="n">
         <v>156</v>
       </c>
@@ -3128,21 +2815,9 @@
     </row>
     <row r="60" ht="27" customHeight="1" s="83">
       <c r="A60" s="102" t="n"/>
-      <c r="B60" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C60" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D60" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B60" s="103" t="n"/>
+      <c r="C60" s="103" t="n"/>
+      <c r="D60" s="103" t="n"/>
       <c r="E60" s="99" t="n">
         <v>142</v>
       </c>
@@ -3158,21 +2833,9 @@
     </row>
     <row r="61" ht="27" customHeight="1" s="83">
       <c r="A61" s="102" t="n"/>
-      <c r="B61" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C61" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D61" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B61" s="103" t="n"/>
+      <c r="C61" s="103" t="n"/>
+      <c r="D61" s="103" t="n"/>
       <c r="E61" s="99" t="n">
         <v>151</v>
       </c>
@@ -3188,21 +2851,9 @@
     </row>
     <row r="62" ht="27" customHeight="1" s="83">
       <c r="A62" s="102" t="n"/>
-      <c r="B62" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C62" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D62" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B62" s="103" t="n"/>
+      <c r="C62" s="103" t="n"/>
+      <c r="D62" s="103" t="n"/>
       <c r="E62" s="99" t="n">
         <v>159</v>
       </c>
@@ -3218,21 +2869,9 @@
     </row>
     <row r="63" ht="27" customHeight="1" s="83">
       <c r="A63" s="102" t="n"/>
-      <c r="B63" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C63" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D63" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B63" s="103" t="n"/>
+      <c r="C63" s="103" t="n"/>
+      <c r="D63" s="103" t="n"/>
       <c r="E63" s="99" t="n">
         <v>170</v>
       </c>
@@ -3248,21 +2887,9 @@
     </row>
     <row r="64" ht="27" customHeight="1" s="83">
       <c r="A64" s="102" t="n"/>
-      <c r="B64" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C64" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D64" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="B64" s="103" t="n"/>
+      <c r="C64" s="103" t="n"/>
+      <c r="D64" s="103" t="n"/>
       <c r="E64" s="99" t="n">
         <v>156</v>
       </c>
@@ -3277,22 +2904,10 @@
       </c>
     </row>
     <row r="65" ht="27" customHeight="1" s="83">
-      <c r="A65" s="103" t="n"/>
-      <c r="B65" s="98" t="inlineStr">
-        <is>
-          <t>TH25020</t>
-        </is>
-      </c>
-      <c r="C65" s="98" t="inlineStr">
-        <is>
-          <t>split hide</t>
-        </is>
-      </c>
-      <c r="D65" s="98" t="inlineStr">
-        <is>
-          <t>wet blue split</t>
-        </is>
-      </c>
+      <c r="A65" s="104" t="n"/>
+      <c r="B65" s="105" t="n"/>
+      <c r="C65" s="105" t="n"/>
+      <c r="D65" s="105" t="n"/>
       <c r="E65" s="99" t="n">
         <v>164</v>
       </c>
@@ -3307,61 +2922,61 @@
       </c>
     </row>
     <row r="66" ht="35" customHeight="1" s="83">
-      <c r="A66" s="104" t="n"/>
-      <c r="B66" s="104" t="inlineStr">
+      <c r="A66" s="106" t="n"/>
+      <c r="B66" s="106" t="inlineStr">
         <is>
           <t>SUB TOTAL:</t>
         </is>
       </c>
-      <c r="C66" s="104" t="inlineStr">
+      <c r="C66" s="106" t="inlineStr">
         <is>
           <t>12 PALLETS</t>
         </is>
       </c>
-      <c r="D66" s="104" t="n"/>
-      <c r="E66" s="104">
+      <c r="D66" s="106" t="n"/>
+      <c r="E66" s="106">
         <f>SUM(E54:E65)</f>
         <v/>
       </c>
-      <c r="F66" s="104">
+      <c r="F66" s="106">
         <f>SUM(F54:F65)</f>
         <v/>
       </c>
-      <c r="G66" s="104">
+      <c r="G66" s="106">
         <f>SUM(G54:G65)</f>
         <v/>
       </c>
-      <c r="H66" s="104">
+      <c r="H66" s="106">
         <f>SUM(H54:H65)</f>
         <v/>
       </c>
     </row>
     <row r="67" ht="35" customHeight="1" s="83">
-      <c r="A67" s="104" t="n"/>
-      <c r="B67" s="104" t="inlineStr">
+      <c r="A67" s="106" t="n"/>
+      <c r="B67" s="106" t="inlineStr">
         <is>
           <t>GRAND TOTAL:</t>
         </is>
       </c>
-      <c r="C67" s="104" t="inlineStr">
+      <c r="C67" s="106" t="inlineStr">
         <is>
           <t>38 PALLETS</t>
         </is>
       </c>
-      <c r="D67" s="104" t="n"/>
-      <c r="E67" s="104">
+      <c r="D67" s="106" t="n"/>
+      <c r="E67" s="106">
         <f>SUM(E22:E34,E38:E50,E54:E65)</f>
         <v/>
       </c>
-      <c r="F67" s="104">
+      <c r="F67" s="106">
         <f>SUM(F22:F34,F38:F50,F54:F65)</f>
         <v/>
       </c>
-      <c r="G67" s="104">
+      <c r="G67" s="106">
         <f>SUM(G22:G34,G38:G50,G54:G65)</f>
         <v/>
       </c>
-      <c r="H67" s="104">
+      <c r="H67" s="106">
         <f>SUM(H22:H34,H38:H50,H54:H65)</f>
         <v/>
       </c>
@@ -3605,17 +3220,26 @@
     <row r="199"/>
     <row r="200" ht="27" customHeight="1" s="83"/>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B73:I73"/>
+  <mergeCells count="19">
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A74:I74"/>
+    <mergeCell ref="B54:B65"/>
+    <mergeCell ref="D54:D65"/>
+    <mergeCell ref="C22:C34"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A5:I5"/>
+    <mergeCell ref="B38:B50"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="C54:C65"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="B73:I73"/>
+    <mergeCell ref="C38:C50"/>
+    <mergeCell ref="A200:B200"/>
+    <mergeCell ref="D38:D50"/>
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A3:I3"/>
     <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A74:I74"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A200:B200"/>
+    <mergeCell ref="B22:B34"/>
+    <mergeCell ref="D22:D34"/>
   </mergeCells>
   <conditionalFormatting sqref="N22:N34">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>
@@ -3757,7 +3381,7 @@
           <t>Date:</t>
         </is>
       </c>
-      <c r="G9" s="105">
+      <c r="G9" s="107">
         <f>'Packing list'!I9</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
fix the static row now has no border at the top and bottom
</commit_message>
<xml_diff>
--- a/invoice_gen/result.xlsx
+++ b/invoice_gen/result.xlsx
@@ -280,7 +280,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -336,28 +336,6 @@
       <right style="thin">
         <color rgb="00000000"/>
       </right>
-      <top style="thin">
-        <color rgb="00000000"/>
-      </top>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="00000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="00000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="00000000"/>
-      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -400,7 +378,7 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -683,14 +661,8 @@
     <xf numFmtId="2" fontId="39" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2044,14 +2016,14 @@
       </c>
     </row>
     <row r="23" ht="27" customHeight="1" s="83">
-      <c r="A23" s="102" t="inlineStr">
+      <c r="A23" s="97" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B23" s="103" t="n"/>
-      <c r="C23" s="103" t="n"/>
-      <c r="D23" s="103" t="n"/>
+      <c r="B23" s="102" t="n"/>
+      <c r="C23" s="102" t="n"/>
+      <c r="D23" s="102" t="n"/>
       <c r="E23" s="99" t="n">
         <v>153</v>
       </c>
@@ -2066,14 +2038,14 @@
       </c>
     </row>
     <row r="24" ht="27" customHeight="1" s="83">
-      <c r="A24" s="102" t="inlineStr">
+      <c r="A24" s="97" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B24" s="103" t="n"/>
-      <c r="C24" s="103" t="n"/>
-      <c r="D24" s="103" t="n"/>
+      <c r="B24" s="102" t="n"/>
+      <c r="C24" s="102" t="n"/>
+      <c r="D24" s="102" t="n"/>
       <c r="E24" s="99" t="n">
         <v>156</v>
       </c>
@@ -2088,14 +2060,14 @@
       </c>
     </row>
     <row r="25" ht="27" customHeight="1" s="83">
-      <c r="A25" s="102" t="inlineStr">
+      <c r="A25" s="97" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B25" s="103" t="n"/>
-      <c r="C25" s="103" t="n"/>
-      <c r="D25" s="103" t="n"/>
+      <c r="B25" s="102" t="n"/>
+      <c r="C25" s="102" t="n"/>
+      <c r="D25" s="102" t="n"/>
       <c r="E25" s="99" t="n">
         <v>145</v>
       </c>
@@ -2110,10 +2082,10 @@
       </c>
     </row>
     <row r="26" ht="27" customHeight="1" s="83">
-      <c r="A26" s="102" t="n"/>
-      <c r="B26" s="103" t="n"/>
-      <c r="C26" s="103" t="n"/>
-      <c r="D26" s="103" t="n"/>
+      <c r="A26" s="97" t="n"/>
+      <c r="B26" s="102" t="n"/>
+      <c r="C26" s="102" t="n"/>
+      <c r="D26" s="102" t="n"/>
       <c r="E26" s="99" t="n">
         <v>166</v>
       </c>
@@ -2128,10 +2100,10 @@
       </c>
     </row>
     <row r="27" ht="27" customHeight="1" s="83">
-      <c r="A27" s="102" t="n"/>
-      <c r="B27" s="103" t="n"/>
-      <c r="C27" s="103" t="n"/>
-      <c r="D27" s="103" t="n"/>
+      <c r="A27" s="97" t="n"/>
+      <c r="B27" s="102" t="n"/>
+      <c r="C27" s="102" t="n"/>
+      <c r="D27" s="102" t="n"/>
       <c r="E27" s="99" t="n">
         <v>156</v>
       </c>
@@ -2146,10 +2118,10 @@
       </c>
     </row>
     <row r="28" ht="27" customHeight="1" s="83">
-      <c r="A28" s="102" t="n"/>
-      <c r="B28" s="103" t="n"/>
-      <c r="C28" s="103" t="n"/>
-      <c r="D28" s="103" t="n"/>
+      <c r="A28" s="97" t="n"/>
+      <c r="B28" s="102" t="n"/>
+      <c r="C28" s="102" t="n"/>
+      <c r="D28" s="102" t="n"/>
       <c r="E28" s="99" t="n">
         <v>149</v>
       </c>
@@ -2164,10 +2136,10 @@
       </c>
     </row>
     <row r="29" ht="27" customHeight="1" s="83">
-      <c r="A29" s="102" t="n"/>
-      <c r="B29" s="103" t="n"/>
-      <c r="C29" s="103" t="n"/>
-      <c r="D29" s="103" t="n"/>
+      <c r="A29" s="97" t="n"/>
+      <c r="B29" s="102" t="n"/>
+      <c r="C29" s="102" t="n"/>
+      <c r="D29" s="102" t="n"/>
       <c r="E29" s="99" t="n">
         <v>157</v>
       </c>
@@ -2182,10 +2154,10 @@
       </c>
     </row>
     <row r="30" ht="27" customHeight="1" s="83">
-      <c r="A30" s="102" t="n"/>
-      <c r="B30" s="103" t="n"/>
-      <c r="C30" s="103" t="n"/>
-      <c r="D30" s="103" t="n"/>
+      <c r="A30" s="97" t="n"/>
+      <c r="B30" s="102" t="n"/>
+      <c r="C30" s="102" t="n"/>
+      <c r="D30" s="102" t="n"/>
       <c r="E30" s="99" t="n">
         <v>148</v>
       </c>
@@ -2200,10 +2172,10 @@
       </c>
     </row>
     <row r="31" ht="27" customHeight="1" s="83">
-      <c r="A31" s="102" t="n"/>
-      <c r="B31" s="103" t="n"/>
-      <c r="C31" s="103" t="n"/>
-      <c r="D31" s="103" t="n"/>
+      <c r="A31" s="97" t="n"/>
+      <c r="B31" s="102" t="n"/>
+      <c r="C31" s="102" t="n"/>
+      <c r="D31" s="102" t="n"/>
       <c r="E31" s="99" t="n">
         <v>157</v>
       </c>
@@ -2218,10 +2190,10 @@
       </c>
     </row>
     <row r="32" ht="27" customHeight="1" s="83">
-      <c r="A32" s="102" t="n"/>
-      <c r="B32" s="103" t="n"/>
-      <c r="C32" s="103" t="n"/>
-      <c r="D32" s="103" t="n"/>
+      <c r="A32" s="97" t="n"/>
+      <c r="B32" s="102" t="n"/>
+      <c r="C32" s="102" t="n"/>
+      <c r="D32" s="102" t="n"/>
       <c r="E32" s="99" t="n">
         <v>172</v>
       </c>
@@ -2236,10 +2208,10 @@
       </c>
     </row>
     <row r="33" ht="27" customHeight="1" s="83">
-      <c r="A33" s="102" t="n"/>
-      <c r="B33" s="103" t="n"/>
-      <c r="C33" s="103" t="n"/>
-      <c r="D33" s="103" t="n"/>
+      <c r="A33" s="97" t="n"/>
+      <c r="B33" s="102" t="n"/>
+      <c r="C33" s="102" t="n"/>
+      <c r="D33" s="102" t="n"/>
       <c r="E33" s="99" t="n">
         <v>130</v>
       </c>
@@ -2254,10 +2226,10 @@
       </c>
     </row>
     <row r="34" ht="27" customHeight="1" s="83">
-      <c r="A34" s="104" t="n"/>
-      <c r="B34" s="105" t="n"/>
-      <c r="C34" s="105" t="n"/>
-      <c r="D34" s="105" t="n"/>
+      <c r="A34" s="97" t="n"/>
+      <c r="B34" s="103" t="n"/>
+      <c r="C34" s="103" t="n"/>
+      <c r="D34" s="103" t="n"/>
       <c r="E34" s="99" t="n">
         <v>158</v>
       </c>
@@ -2271,838 +2243,889 @@
         <v>2.64</v>
       </c>
     </row>
-    <row r="35" ht="35" customHeight="1" s="83">
-      <c r="A35" s="106" t="n"/>
-      <c r="B35" s="106" t="inlineStr">
+    <row r="35" ht="27" customHeight="1" s="83">
+      <c r="A35" s="97" t="inlineStr">
+        <is>
+          <t>This is a pre-footer note.</t>
+        </is>
+      </c>
+      <c r="B35" s="98" t="n"/>
+      <c r="C35" s="98" t="n"/>
+      <c r="D35" s="98" t="n"/>
+      <c r="E35" s="99" t="n"/>
+      <c r="F35" s="100" t="n"/>
+      <c r="G35" s="100" t="inlineStr">
+        <is>
+          <t>Another value</t>
+        </is>
+      </c>
+      <c r="H35" s="101" t="n"/>
+    </row>
+    <row r="36" ht="35" customHeight="1" s="83">
+      <c r="A36" s="104" t="n"/>
+      <c r="B36" s="104" t="inlineStr">
         <is>
           <t>SUB TOTAL:</t>
         </is>
       </c>
-      <c r="C35" s="106" t="inlineStr">
+      <c r="C36" s="104" t="inlineStr">
         <is>
           <t>13 PALLETS</t>
         </is>
       </c>
-      <c r="D35" s="106" t="n"/>
-      <c r="E35" s="106">
-        <f>SUM(E22:E34)</f>
+      <c r="D36" s="104" t="n"/>
+      <c r="E36" s="104">
+        <f>SUM(E22:E35)</f>
         <v/>
       </c>
-      <c r="F35" s="106">
-        <f>SUM(F22:F34)</f>
+      <c r="F36" s="104">
+        <f>SUM(F22:F35)</f>
         <v/>
       </c>
-      <c r="G35" s="106">
-        <f>SUM(G22:G34)</f>
+      <c r="G36" s="104">
+        <f>SUM(G22:G35)</f>
         <v/>
       </c>
-      <c r="H35" s="106">
-        <f>SUM(H22:H34)</f>
+      <c r="H36" s="104">
+        <f>SUM(H22:H35)</f>
         <v/>
       </c>
     </row>
-    <row r="37" ht="27" customHeight="1" s="83">
-      <c r="A37" s="96" t="inlineStr">
+    <row r="38" ht="27" customHeight="1" s="83">
+      <c r="A38" s="96" t="inlineStr">
         <is>
           <t>Mark &amp; Nº</t>
         </is>
       </c>
-      <c r="B37" s="96" t="inlineStr">
+      <c r="B38" s="96" t="inlineStr">
         <is>
           <t>P.O Nº</t>
         </is>
       </c>
-      <c r="C37" s="96" t="inlineStr">
+      <c r="C38" s="96" t="inlineStr">
         <is>
           <t>ITEM Nº</t>
         </is>
       </c>
-      <c r="D37" s="96" t="inlineStr">
+      <c r="D38" s="96" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="E37" s="96" t="inlineStr">
+      <c r="E38" s="96" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
       </c>
-      <c r="F37" s="96" t="inlineStr">
+      <c r="F38" s="96" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
         </is>
       </c>
-      <c r="G37" s="96" t="inlineStr">
+      <c r="G38" s="96" t="inlineStr">
         <is>
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="H37" s="96" t="inlineStr">
+      <c r="H38" s="96" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
       </c>
     </row>
-    <row r="38" ht="27" customHeight="1" s="83">
-      <c r="A38" s="97" t="inlineStr">
+    <row r="39" ht="27" customHeight="1" s="83">
+      <c r="A39" s="97" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B38" s="98" t="inlineStr">
+      <c r="B39" s="98" t="inlineStr">
         <is>
           <t>TH25020</t>
         </is>
       </c>
-      <c r="C38" s="98" t="inlineStr">
+      <c r="C39" s="98" t="inlineStr">
         <is>
           <t>split hide</t>
         </is>
       </c>
-      <c r="D38" s="98" t="inlineStr">
+      <c r="D39" s="98" t="inlineStr">
         <is>
           <t>wet blue split</t>
         </is>
       </c>
-      <c r="E38" s="99" t="n">
+      <c r="E39" s="99" t="n">
         <v>132</v>
       </c>
-      <c r="F38" s="100" t="n">
+      <c r="F39" s="100" t="n">
         <v>1697</v>
       </c>
-      <c r="G38" s="100" t="n">
+      <c r="G39" s="100" t="n">
         <v>1737</v>
       </c>
-      <c r="H38" s="101" t="n">
+      <c r="H39" s="101" t="n">
         <v>2.64</v>
       </c>
     </row>
-    <row r="39" ht="27" customHeight="1" s="83">
-      <c r="A39" s="102" t="inlineStr">
+    <row r="40" ht="27" customHeight="1" s="83">
+      <c r="A40" s="97" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B39" s="103" t="n"/>
-      <c r="C39" s="103" t="n"/>
-      <c r="D39" s="103" t="n"/>
-      <c r="E39" s="99" t="n">
+      <c r="B40" s="102" t="n"/>
+      <c r="C40" s="102" t="n"/>
+      <c r="D40" s="102" t="n"/>
+      <c r="E40" s="99" t="n">
         <v>173</v>
       </c>
-      <c r="F39" s="100" t="n">
+      <c r="F40" s="100" t="n">
         <v>2293</v>
       </c>
-      <c r="G39" s="100" t="n">
+      <c r="G40" s="100" t="n">
         <v>2333</v>
-      </c>
-      <c r="H39" s="101" t="n">
-        <v>2.75</v>
-      </c>
-    </row>
-    <row r="40" ht="27" customHeight="1" s="83">
-      <c r="A40" s="102" t="inlineStr">
-        <is>
-          <t>Case Qty:</t>
-        </is>
-      </c>
-      <c r="B40" s="103" t="n"/>
-      <c r="C40" s="103" t="n"/>
-      <c r="D40" s="103" t="n"/>
-      <c r="E40" s="99" t="n">
-        <v>195</v>
-      </c>
-      <c r="F40" s="100" t="n">
-        <v>1899</v>
-      </c>
-      <c r="G40" s="100" t="n">
-        <v>1939</v>
       </c>
       <c r="H40" s="101" t="n">
         <v>2.75</v>
       </c>
     </row>
     <row r="41" ht="27" customHeight="1" s="83">
-      <c r="A41" s="102" t="inlineStr">
+      <c r="A41" s="97" t="inlineStr">
+        <is>
+          <t>Case Qty:</t>
+        </is>
+      </c>
+      <c r="B41" s="102" t="n"/>
+      <c r="C41" s="102" t="n"/>
+      <c r="D41" s="102" t="n"/>
+      <c r="E41" s="99" t="n">
+        <v>195</v>
+      </c>
+      <c r="F41" s="100" t="n">
+        <v>1899</v>
+      </c>
+      <c r="G41" s="100" t="n">
+        <v>1939</v>
+      </c>
+      <c r="H41" s="101" t="n">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="42" ht="27" customHeight="1" s="83">
+      <c r="A42" s="97" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B41" s="103" t="n"/>
-      <c r="C41" s="103" t="n"/>
-      <c r="D41" s="103" t="n"/>
-      <c r="E41" s="99" t="n">
+      <c r="B42" s="102" t="n"/>
+      <c r="C42" s="102" t="n"/>
+      <c r="D42" s="102" t="n"/>
+      <c r="E42" s="99" t="n">
         <v>155</v>
       </c>
-      <c r="F41" s="100" t="n">
+      <c r="F42" s="100" t="n">
         <v>2056</v>
       </c>
-      <c r="G41" s="100" t="n">
+      <c r="G42" s="100" t="n">
         <v>2096</v>
-      </c>
-      <c r="H41" s="101" t="n">
-        <v>2.64</v>
-      </c>
-    </row>
-    <row r="42" ht="27" customHeight="1" s="83">
-      <c r="A42" s="102" t="n"/>
-      <c r="B42" s="103" t="n"/>
-      <c r="C42" s="103" t="n"/>
-      <c r="D42" s="103" t="n"/>
-      <c r="E42" s="99" t="n">
-        <v>152</v>
-      </c>
-      <c r="F42" s="100" t="n">
-        <v>2029</v>
-      </c>
-      <c r="G42" s="100" t="n">
-        <v>2069</v>
       </c>
       <c r="H42" s="101" t="n">
         <v>2.64</v>
       </c>
     </row>
     <row r="43" ht="27" customHeight="1" s="83">
-      <c r="A43" s="102" t="n"/>
-      <c r="B43" s="103" t="n"/>
-      <c r="C43" s="103" t="n"/>
-      <c r="D43" s="103" t="n"/>
+      <c r="A43" s="97" t="n"/>
+      <c r="B43" s="102" t="n"/>
+      <c r="C43" s="102" t="n"/>
+      <c r="D43" s="102" t="n"/>
       <c r="E43" s="99" t="n">
+        <v>152</v>
+      </c>
+      <c r="F43" s="100" t="n">
+        <v>2029</v>
+      </c>
+      <c r="G43" s="100" t="n">
+        <v>2069</v>
+      </c>
+      <c r="H43" s="101" t="n">
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="44" ht="27" customHeight="1" s="83">
+      <c r="A44" s="97" t="n"/>
+      <c r="B44" s="102" t="n"/>
+      <c r="C44" s="102" t="n"/>
+      <c r="D44" s="102" t="n"/>
+      <c r="E44" s="99" t="n">
         <v>154</v>
       </c>
-      <c r="F43" s="100" t="n">
+      <c r="F44" s="100" t="n">
         <v>1844</v>
       </c>
-      <c r="G43" s="100" t="n">
+      <c r="G44" s="100" t="n">
         <v>1884</v>
       </c>
-      <c r="H43" s="101" t="n">
+      <c r="H44" s="101" t="n">
         <v>2.75</v>
       </c>
     </row>
-    <row r="44" ht="27" customHeight="1" s="83">
-      <c r="A44" s="102" t="n"/>
-      <c r="B44" s="103" t="n"/>
-      <c r="C44" s="103" t="n"/>
-      <c r="D44" s="103" t="n"/>
-      <c r="E44" s="99" t="n">
+    <row r="45" ht="27" customHeight="1" s="83">
+      <c r="A45" s="97" t="n"/>
+      <c r="B45" s="102" t="n"/>
+      <c r="C45" s="102" t="n"/>
+      <c r="D45" s="102" t="n"/>
+      <c r="E45" s="99" t="n">
         <v>138</v>
       </c>
-      <c r="F44" s="100" t="n">
+      <c r="F45" s="100" t="n">
         <v>1597</v>
       </c>
-      <c r="G44" s="100" t="n">
+      <c r="G45" s="100" t="n">
         <v>1637</v>
       </c>
-      <c r="H44" s="101" t="n">
+      <c r="H45" s="101" t="n">
         <v>2.53</v>
       </c>
     </row>
-    <row r="45" ht="27" customHeight="1" s="83">
-      <c r="A45" s="102" t="n"/>
-      <c r="B45" s="103" t="n"/>
-      <c r="C45" s="103" t="n"/>
-      <c r="D45" s="103" t="n"/>
-      <c r="E45" s="99" t="n">
+    <row r="46" ht="27" customHeight="1" s="83">
+      <c r="A46" s="97" t="n"/>
+      <c r="B46" s="102" t="n"/>
+      <c r="C46" s="102" t="n"/>
+      <c r="D46" s="102" t="n"/>
+      <c r="E46" s="99" t="n">
         <v>150</v>
       </c>
-      <c r="F45" s="100" t="n">
+      <c r="F46" s="100" t="n">
         <v>1676</v>
       </c>
-      <c r="G45" s="100" t="n">
+      <c r="G46" s="100" t="n">
         <v>1716</v>
-      </c>
-      <c r="H45" s="101" t="n">
-        <v>2.64</v>
-      </c>
-    </row>
-    <row r="46" ht="27" customHeight="1" s="83">
-      <c r="A46" s="102" t="n"/>
-      <c r="B46" s="103" t="n"/>
-      <c r="C46" s="103" t="n"/>
-      <c r="D46" s="103" t="n"/>
-      <c r="E46" s="99" t="n">
-        <v>139</v>
-      </c>
-      <c r="F46" s="100" t="n">
-        <v>1783</v>
-      </c>
-      <c r="G46" s="100" t="n">
-        <v>1823</v>
       </c>
       <c r="H46" s="101" t="n">
         <v>2.64</v>
       </c>
     </row>
     <row r="47" ht="27" customHeight="1" s="83">
-      <c r="A47" s="102" t="n"/>
-      <c r="B47" s="103" t="n"/>
-      <c r="C47" s="103" t="n"/>
-      <c r="D47" s="103" t="n"/>
+      <c r="A47" s="97" t="n"/>
+      <c r="B47" s="102" t="n"/>
+      <c r="C47" s="102" t="n"/>
+      <c r="D47" s="102" t="n"/>
       <c r="E47" s="99" t="n">
+        <v>139</v>
+      </c>
+      <c r="F47" s="100" t="n">
+        <v>1783</v>
+      </c>
+      <c r="G47" s="100" t="n">
+        <v>1823</v>
+      </c>
+      <c r="H47" s="101" t="n">
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="48" ht="27" customHeight="1" s="83">
+      <c r="A48" s="97" t="n"/>
+      <c r="B48" s="102" t="n"/>
+      <c r="C48" s="102" t="n"/>
+      <c r="D48" s="102" t="n"/>
+      <c r="E48" s="99" t="n">
         <v>183</v>
       </c>
-      <c r="F47" s="100" t="n">
+      <c r="F48" s="100" t="n">
         <v>2004</v>
       </c>
-      <c r="G47" s="100" t="n">
+      <c r="G48" s="100" t="n">
         <v>2044</v>
       </c>
-      <c r="H47" s="101" t="n">
+      <c r="H48" s="101" t="n">
         <v>2.75</v>
       </c>
     </row>
-    <row r="48" ht="27" customHeight="1" s="83">
-      <c r="A48" s="102" t="n"/>
-      <c r="B48" s="103" t="n"/>
-      <c r="C48" s="103" t="n"/>
-      <c r="D48" s="103" t="n"/>
-      <c r="E48" s="99" t="n">
+    <row r="49" ht="27" customHeight="1" s="83">
+      <c r="A49" s="97" t="n"/>
+      <c r="B49" s="102" t="n"/>
+      <c r="C49" s="102" t="n"/>
+      <c r="D49" s="102" t="n"/>
+      <c r="E49" s="99" t="n">
         <v>148</v>
       </c>
-      <c r="F48" s="100" t="n">
+      <c r="F49" s="100" t="n">
         <v>1800</v>
       </c>
-      <c r="G48" s="100" t="n">
+      <c r="G49" s="100" t="n">
         <v>1840</v>
-      </c>
-      <c r="H48" s="101" t="n">
-        <v>2.64</v>
-      </c>
-    </row>
-    <row r="49" ht="27" customHeight="1" s="83">
-      <c r="A49" s="102" t="n"/>
-      <c r="B49" s="103" t="n"/>
-      <c r="C49" s="103" t="n"/>
-      <c r="D49" s="103" t="n"/>
-      <c r="E49" s="99" t="n">
-        <v>137</v>
-      </c>
-      <c r="F49" s="100" t="n">
-        <v>1782</v>
-      </c>
-      <c r="G49" s="100" t="n">
-        <v>1822</v>
       </c>
       <c r="H49" s="101" t="n">
         <v>2.64</v>
       </c>
     </row>
     <row r="50" ht="27" customHeight="1" s="83">
-      <c r="A50" s="104" t="n"/>
-      <c r="B50" s="105" t="n"/>
-      <c r="C50" s="105" t="n"/>
-      <c r="D50" s="105" t="n"/>
+      <c r="A50" s="97" t="n"/>
+      <c r="B50" s="102" t="n"/>
+      <c r="C50" s="102" t="n"/>
+      <c r="D50" s="102" t="n"/>
       <c r="E50" s="99" t="n">
-        <v>174</v>
+        <v>137</v>
       </c>
       <c r="F50" s="100" t="n">
-        <v>1784</v>
+        <v>1782</v>
       </c>
       <c r="G50" s="100" t="n">
-        <v>1824</v>
+        <v>1822</v>
       </c>
       <c r="H50" s="101" t="n">
         <v>2.64</v>
       </c>
     </row>
-    <row r="51" ht="35" customHeight="1" s="83">
-      <c r="A51" s="106" t="n"/>
-      <c r="B51" s="106" t="inlineStr">
+    <row r="51" ht="27" customHeight="1" s="83">
+      <c r="A51" s="97" t="n"/>
+      <c r="B51" s="103" t="n"/>
+      <c r="C51" s="103" t="n"/>
+      <c r="D51" s="103" t="n"/>
+      <c r="E51" s="99" t="n">
+        <v>174</v>
+      </c>
+      <c r="F51" s="100" t="n">
+        <v>1784</v>
+      </c>
+      <c r="G51" s="100" t="n">
+        <v>1824</v>
+      </c>
+      <c r="H51" s="101" t="n">
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="52" ht="27" customHeight="1" s="83">
+      <c r="A52" s="97" t="inlineStr">
+        <is>
+          <t>This is a pre-footer note.</t>
+        </is>
+      </c>
+      <c r="B52" s="98" t="n"/>
+      <c r="C52" s="98" t="n"/>
+      <c r="D52" s="98" t="n"/>
+      <c r="E52" s="99" t="n"/>
+      <c r="F52" s="100" t="n"/>
+      <c r="G52" s="100" t="inlineStr">
+        <is>
+          <t>Another value</t>
+        </is>
+      </c>
+      <c r="H52" s="101" t="n"/>
+    </row>
+    <row r="53" ht="35" customHeight="1" s="83">
+      <c r="A53" s="104" t="n"/>
+      <c r="B53" s="104" t="inlineStr">
         <is>
           <t>SUB TOTAL:</t>
         </is>
       </c>
-      <c r="C51" s="106" t="inlineStr">
+      <c r="C53" s="104" t="inlineStr">
         <is>
           <t>13 PALLETS</t>
         </is>
       </c>
-      <c r="D51" s="106" t="n"/>
-      <c r="E51" s="106">
-        <f>SUM(E38:E50)</f>
+      <c r="D53" s="104" t="n"/>
+      <c r="E53" s="104">
+        <f>SUM(E39:E52)</f>
         <v/>
       </c>
-      <c r="F51" s="106">
-        <f>SUM(F38:F50)</f>
+      <c r="F53" s="104">
+        <f>SUM(F39:F52)</f>
         <v/>
       </c>
-      <c r="G51" s="106">
-        <f>SUM(G38:G50)</f>
+      <c r="G53" s="104">
+        <f>SUM(G39:G52)</f>
         <v/>
       </c>
-      <c r="H51" s="106">
-        <f>SUM(H38:H50)</f>
+      <c r="H53" s="104">
+        <f>SUM(H39:H52)</f>
         <v/>
       </c>
     </row>
-    <row r="53" ht="27" customHeight="1" s="83">
-      <c r="A53" s="96" t="inlineStr">
+    <row r="55" ht="27" customHeight="1" s="83">
+      <c r="A55" s="96" t="inlineStr">
         <is>
           <t>Mark &amp; Nº</t>
         </is>
       </c>
-      <c r="B53" s="96" t="inlineStr">
+      <c r="B55" s="96" t="inlineStr">
         <is>
           <t>P.O Nº</t>
         </is>
       </c>
-      <c r="C53" s="96" t="inlineStr">
+      <c r="C55" s="96" t="inlineStr">
         <is>
           <t>ITEM Nº</t>
         </is>
       </c>
-      <c r="D53" s="96" t="inlineStr">
+      <c r="D55" s="96" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="E53" s="96" t="inlineStr">
+      <c r="E55" s="96" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
       </c>
-      <c r="F53" s="96" t="inlineStr">
+      <c r="F55" s="96" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
         </is>
       </c>
-      <c r="G53" s="96" t="inlineStr">
+      <c r="G55" s="96" t="inlineStr">
         <is>
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="H53" s="96" t="inlineStr">
+      <c r="H55" s="96" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
       </c>
     </row>
-    <row r="54" ht="27" customHeight="1" s="83">
-      <c r="A54" s="97" t="inlineStr">
+    <row r="56" ht="27" customHeight="1" s="83">
+      <c r="A56" s="97" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B54" s="98" t="inlineStr">
+      <c r="B56" s="98" t="inlineStr">
         <is>
           <t>TH25020</t>
         </is>
       </c>
-      <c r="C54" s="98" t="inlineStr">
+      <c r="C56" s="98" t="inlineStr">
         <is>
           <t>split hide</t>
         </is>
       </c>
-      <c r="D54" s="98" t="inlineStr">
+      <c r="D56" s="98" t="inlineStr">
         <is>
           <t>wet blue split</t>
         </is>
       </c>
-      <c r="E54" s="99" t="n">
+      <c r="E56" s="99" t="n">
         <v>163</v>
       </c>
-      <c r="F54" s="100" t="n">
+      <c r="F56" s="100" t="n">
         <v>2035</v>
       </c>
-      <c r="G54" s="100" t="n">
+      <c r="G56" s="100" t="n">
         <v>2075</v>
-      </c>
-      <c r="H54" s="101" t="n">
-        <v>2.64</v>
-      </c>
-    </row>
-    <row r="55" ht="27" customHeight="1" s="83">
-      <c r="A55" s="102" t="inlineStr">
-        <is>
-          <t>Des: LEATHER</t>
-        </is>
-      </c>
-      <c r="B55" s="103" t="n"/>
-      <c r="C55" s="103" t="n"/>
-      <c r="D55" s="103" t="n"/>
-      <c r="E55" s="99" t="n">
-        <v>160</v>
-      </c>
-      <c r="F55" s="100" t="n">
-        <v>2095</v>
-      </c>
-      <c r="G55" s="100" t="n">
-        <v>2135</v>
-      </c>
-      <c r="H55" s="101" t="n">
-        <v>2.75</v>
-      </c>
-    </row>
-    <row r="56" ht="27" customHeight="1" s="83">
-      <c r="A56" s="102" t="inlineStr">
-        <is>
-          <t>Case Qty:</t>
-        </is>
-      </c>
-      <c r="B56" s="103" t="n"/>
-      <c r="C56" s="103" t="n"/>
-      <c r="D56" s="103" t="n"/>
-      <c r="E56" s="99" t="n">
-        <v>157</v>
-      </c>
-      <c r="F56" s="100" t="n">
-        <v>2019</v>
-      </c>
-      <c r="G56" s="100" t="n">
-        <v>2059</v>
       </c>
       <c r="H56" s="101" t="n">
         <v>2.64</v>
       </c>
     </row>
     <row r="57" ht="27" customHeight="1" s="83">
-      <c r="A57" s="102" t="inlineStr">
-        <is>
-          <t>MADE IN CAMBODIA</t>
-        </is>
-      </c>
-      <c r="B57" s="103" t="n"/>
-      <c r="C57" s="103" t="n"/>
-      <c r="D57" s="103" t="n"/>
+      <c r="A57" s="97" t="inlineStr">
+        <is>
+          <t>Des: LEATHER</t>
+        </is>
+      </c>
+      <c r="B57" s="102" t="n"/>
+      <c r="C57" s="102" t="n"/>
+      <c r="D57" s="102" t="n"/>
       <c r="E57" s="99" t="n">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F57" s="100" t="n">
-        <v>2270</v>
+        <v>2095</v>
       </c>
       <c r="G57" s="100" t="n">
-        <v>2310</v>
+        <v>2135</v>
       </c>
       <c r="H57" s="101" t="n">
-        <v>2.86</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="58" ht="27" customHeight="1" s="83">
-      <c r="A58" s="102" t="n"/>
-      <c r="B58" s="103" t="n"/>
-      <c r="C58" s="103" t="n"/>
-      <c r="D58" s="103" t="n"/>
+      <c r="A58" s="97" t="inlineStr">
+        <is>
+          <t>Case Qty:</t>
+        </is>
+      </c>
+      <c r="B58" s="102" t="n"/>
+      <c r="C58" s="102" t="n"/>
+      <c r="D58" s="102" t="n"/>
       <c r="E58" s="99" t="n">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F58" s="100" t="n">
-        <v>1784</v>
+        <v>2019</v>
       </c>
       <c r="G58" s="100" t="n">
-        <v>1824</v>
+        <v>2059</v>
       </c>
       <c r="H58" s="101" t="n">
         <v>2.64</v>
       </c>
     </row>
     <row r="59" ht="27" customHeight="1" s="83">
-      <c r="A59" s="102" t="n"/>
-      <c r="B59" s="103" t="n"/>
-      <c r="C59" s="103" t="n"/>
-      <c r="D59" s="103" t="n"/>
+      <c r="A59" s="97" t="inlineStr">
+        <is>
+          <t>MADE IN CAMBODIA</t>
+        </is>
+      </c>
+      <c r="B59" s="102" t="n"/>
+      <c r="C59" s="102" t="n"/>
+      <c r="D59" s="102" t="n"/>
       <c r="E59" s="99" t="n">
+        <v>163</v>
+      </c>
+      <c r="F59" s="100" t="n">
+        <v>2270</v>
+      </c>
+      <c r="G59" s="100" t="n">
+        <v>2310</v>
+      </c>
+      <c r="H59" s="101" t="n">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="60" ht="27" customHeight="1" s="83">
+      <c r="A60" s="97" t="n"/>
+      <c r="B60" s="102" t="n"/>
+      <c r="C60" s="102" t="n"/>
+      <c r="D60" s="102" t="n"/>
+      <c r="E60" s="99" t="n">
+        <v>149</v>
+      </c>
+      <c r="F60" s="100" t="n">
+        <v>1784</v>
+      </c>
+      <c r="G60" s="100" t="n">
+        <v>1824</v>
+      </c>
+      <c r="H60" s="101" t="n">
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="61" ht="27" customHeight="1" s="83">
+      <c r="A61" s="97" t="n"/>
+      <c r="B61" s="102" t="n"/>
+      <c r="C61" s="102" t="n"/>
+      <c r="D61" s="102" t="n"/>
+      <c r="E61" s="99" t="n">
         <v>156</v>
       </c>
-      <c r="F59" s="100" t="n">
+      <c r="F61" s="100" t="n">
         <v>1784</v>
       </c>
-      <c r="G59" s="100" t="n">
+      <c r="G61" s="100" t="n">
         <v>1824</v>
       </c>
-      <c r="H59" s="101" t="n">
+      <c r="H61" s="101" t="n">
         <v>2.75</v>
       </c>
     </row>
-    <row r="60" ht="27" customHeight="1" s="83">
-      <c r="A60" s="102" t="n"/>
-      <c r="B60" s="103" t="n"/>
-      <c r="C60" s="103" t="n"/>
-      <c r="D60" s="103" t="n"/>
-      <c r="E60" s="99" t="n">
+    <row r="62" ht="27" customHeight="1" s="83">
+      <c r="A62" s="97" t="n"/>
+      <c r="B62" s="102" t="n"/>
+      <c r="C62" s="102" t="n"/>
+      <c r="D62" s="102" t="n"/>
+      <c r="E62" s="99" t="n">
         <v>142</v>
       </c>
-      <c r="F60" s="100" t="n">
+      <c r="F62" s="100" t="n">
         <v>2136</v>
       </c>
-      <c r="G60" s="100" t="n">
+      <c r="G62" s="100" t="n">
         <v>2176</v>
       </c>
-      <c r="H60" s="101" t="n">
+      <c r="H62" s="101" t="n">
         <v>2.86</v>
       </c>
     </row>
-    <row r="61" ht="27" customHeight="1" s="83">
-      <c r="A61" s="102" t="n"/>
-      <c r="B61" s="103" t="n"/>
-      <c r="C61" s="103" t="n"/>
-      <c r="D61" s="103" t="n"/>
-      <c r="E61" s="99" t="n">
+    <row r="63" ht="27" customHeight="1" s="83">
+      <c r="A63" s="97" t="n"/>
+      <c r="B63" s="102" t="n"/>
+      <c r="C63" s="102" t="n"/>
+      <c r="D63" s="102" t="n"/>
+      <c r="E63" s="99" t="n">
         <v>151</v>
       </c>
-      <c r="F61" s="100" t="n">
+      <c r="F63" s="100" t="n">
         <v>1827</v>
       </c>
-      <c r="G61" s="100" t="n">
+      <c r="G63" s="100" t="n">
         <v>1867</v>
       </c>
-      <c r="H61" s="101" t="n">
+      <c r="H63" s="101" t="n">
         <v>2.64</v>
       </c>
     </row>
-    <row r="62" ht="27" customHeight="1" s="83">
-      <c r="A62" s="102" t="n"/>
-      <c r="B62" s="103" t="n"/>
-      <c r="C62" s="103" t="n"/>
-      <c r="D62" s="103" t="n"/>
-      <c r="E62" s="99" t="n">
+    <row r="64" ht="27" customHeight="1" s="83">
+      <c r="A64" s="97" t="n"/>
+      <c r="B64" s="102" t="n"/>
+      <c r="C64" s="102" t="n"/>
+      <c r="D64" s="102" t="n"/>
+      <c r="E64" s="99" t="n">
         <v>159</v>
       </c>
-      <c r="F62" s="100" t="n">
+      <c r="F64" s="100" t="n">
         <v>2120</v>
       </c>
-      <c r="G62" s="100" t="n">
+      <c r="G64" s="100" t="n">
         <v>2160</v>
       </c>
-      <c r="H62" s="101" t="n">
+      <c r="H64" s="101" t="n">
         <v>2.64</v>
       </c>
     </row>
-    <row r="63" ht="27" customHeight="1" s="83">
-      <c r="A63" s="102" t="n"/>
-      <c r="B63" s="103" t="n"/>
-      <c r="C63" s="103" t="n"/>
-      <c r="D63" s="103" t="n"/>
-      <c r="E63" s="99" t="n">
+    <row r="65" ht="27" customHeight="1" s="83">
+      <c r="A65" s="97" t="n"/>
+      <c r="B65" s="102" t="n"/>
+      <c r="C65" s="102" t="n"/>
+      <c r="D65" s="102" t="n"/>
+      <c r="E65" s="99" t="n">
         <v>170</v>
       </c>
-      <c r="F63" s="100" t="n">
+      <c r="F65" s="100" t="n">
         <v>2110</v>
       </c>
-      <c r="G63" s="100" t="n">
+      <c r="G65" s="100" t="n">
         <v>2150</v>
       </c>
-      <c r="H63" s="101" t="n">
+      <c r="H65" s="101" t="n">
         <v>2.75</v>
       </c>
     </row>
-    <row r="64" ht="27" customHeight="1" s="83">
-      <c r="A64" s="102" t="n"/>
-      <c r="B64" s="103" t="n"/>
-      <c r="C64" s="103" t="n"/>
-      <c r="D64" s="103" t="n"/>
-      <c r="E64" s="99" t="n">
+    <row r="66" ht="27" customHeight="1" s="83">
+      <c r="A66" s="97" t="n"/>
+      <c r="B66" s="102" t="n"/>
+      <c r="C66" s="102" t="n"/>
+      <c r="D66" s="102" t="n"/>
+      <c r="E66" s="99" t="n">
         <v>156</v>
       </c>
-      <c r="F64" s="100" t="n">
+      <c r="F66" s="100" t="n">
         <v>2180</v>
       </c>
-      <c r="G64" s="100" t="n">
+      <c r="G66" s="100" t="n">
         <v>2220</v>
       </c>
-      <c r="H64" s="101" t="n">
+      <c r="H66" s="101" t="n">
         <v>2.75</v>
       </c>
     </row>
-    <row r="65" ht="27" customHeight="1" s="83">
-      <c r="A65" s="104" t="n"/>
-      <c r="B65" s="105" t="n"/>
-      <c r="C65" s="105" t="n"/>
-      <c r="D65" s="105" t="n"/>
-      <c r="E65" s="99" t="n">
+    <row r="67" ht="27" customHeight="1" s="83">
+      <c r="A67" s="97" t="n"/>
+      <c r="B67" s="103" t="n"/>
+      <c r="C67" s="103" t="n"/>
+      <c r="D67" s="103" t="n"/>
+      <c r="E67" s="99" t="n">
         <v>164</v>
       </c>
-      <c r="F65" s="100" t="n">
+      <c r="F67" s="100" t="n">
         <v>2131</v>
       </c>
-      <c r="G65" s="100" t="n">
+      <c r="G67" s="100" t="n">
         <v>2171</v>
       </c>
-      <c r="H65" s="101" t="n">
+      <c r="H67" s="101" t="n">
         <v>2.64</v>
       </c>
     </row>
-    <row r="66" ht="35" customHeight="1" s="83">
-      <c r="A66" s="106" t="n"/>
-      <c r="B66" s="106" t="inlineStr">
+    <row r="68" ht="27" customHeight="1" s="83">
+      <c r="A68" s="97" t="inlineStr">
+        <is>
+          <t>This is a pre-footer note.</t>
+        </is>
+      </c>
+      <c r="B68" s="98" t="n"/>
+      <c r="C68" s="98" t="n"/>
+      <c r="D68" s="98" t="n"/>
+      <c r="E68" s="99" t="n"/>
+      <c r="F68" s="100" t="n"/>
+      <c r="G68" s="100" t="inlineStr">
+        <is>
+          <t>Another value</t>
+        </is>
+      </c>
+      <c r="H68" s="101" t="n"/>
+    </row>
+    <row r="69" ht="35" customHeight="1" s="83">
+      <c r="A69" s="104" t="n"/>
+      <c r="B69" s="104" t="inlineStr">
         <is>
           <t>SUB TOTAL:</t>
         </is>
       </c>
-      <c r="C66" s="106" t="inlineStr">
+      <c r="C69" s="104" t="inlineStr">
         <is>
           <t>12 PALLETS</t>
         </is>
       </c>
-      <c r="D66" s="106" t="n"/>
-      <c r="E66" s="106">
-        <f>SUM(E54:E65)</f>
+      <c r="D69" s="104" t="n"/>
+      <c r="E69" s="104">
+        <f>SUM(E56:E68)</f>
         <v/>
       </c>
-      <c r="F66" s="106">
-        <f>SUM(F54:F65)</f>
+      <c r="F69" s="104">
+        <f>SUM(F56:F68)</f>
         <v/>
       </c>
-      <c r="G66" s="106">
-        <f>SUM(G54:G65)</f>
+      <c r="G69" s="104">
+        <f>SUM(G56:G68)</f>
         <v/>
       </c>
-      <c r="H66" s="106">
-        <f>SUM(H54:H65)</f>
+      <c r="H69" s="104">
+        <f>SUM(H56:H68)</f>
         <v/>
       </c>
     </row>
-    <row r="67" ht="35" customHeight="1" s="83">
-      <c r="A67" s="106" t="n"/>
-      <c r="B67" s="106" t="inlineStr">
+    <row r="70" ht="35" customHeight="1" s="83">
+      <c r="A70" s="104" t="n"/>
+      <c r="B70" s="104" t="inlineStr">
         <is>
           <t>GRAND TOTAL:</t>
         </is>
       </c>
-      <c r="C67" s="106" t="inlineStr">
+      <c r="C70" s="104" t="inlineStr">
         <is>
           <t>38 PALLETS</t>
         </is>
       </c>
-      <c r="D67" s="106" t="n"/>
-      <c r="E67" s="106">
-        <f>SUM(E22:E34,E38:E50,E54:E65)</f>
+      <c r="D70" s="104" t="n"/>
+      <c r="E70" s="104">
+        <f>SUM(E22:E34,E39:E51,E56:E67)</f>
         <v/>
       </c>
-      <c r="F67" s="106">
-        <f>SUM(F22:F34,F38:F50,F54:F65)</f>
+      <c r="F70" s="104">
+        <f>SUM(F22:F34,F39:F51,F56:F67)</f>
         <v/>
       </c>
-      <c r="G67" s="106">
-        <f>SUM(G22:G34,G38:G50,G54:G65)</f>
+      <c r="G70" s="104">
+        <f>SUM(G22:G34,G39:G51,G56:G67)</f>
         <v/>
       </c>
-      <c r="H67" s="106">
-        <f>SUM(H22:H34,H38:H50,H54:H65)</f>
+      <c r="H70" s="104">
+        <f>SUM(H22:H34,H39:H51,H56:H67)</f>
         <v/>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" s="29" t="n"/>
-      <c r="B71" s="29" t="n"/>
-      <c r="C71" s="30" t="n"/>
-      <c r="D71" s="30" t="n"/>
-      <c r="E71" s="30" t="n"/>
-      <c r="F71" s="30" t="n"/>
-      <c r="G71" s="30" t="n"/>
-      <c r="H71" s="30" t="n"/>
-      <c r="I71" s="39" t="n"/>
-      <c r="L71" s="82" t="n"/>
-    </row>
-    <row r="72" ht="27" customHeight="1" s="83">
-      <c r="A72" s="85" t="inlineStr">
+    <row r="74">
+      <c r="A74" s="29" t="n"/>
+      <c r="B74" s="29" t="n"/>
+      <c r="C74" s="30" t="n"/>
+      <c r="D74" s="30" t="n"/>
+      <c r="E74" s="30" t="n"/>
+      <c r="F74" s="30" t="n"/>
+      <c r="G74" s="30" t="n"/>
+      <c r="H74" s="30" t="n"/>
+      <c r="I74" s="39" t="n"/>
+      <c r="L74" s="82" t="n"/>
+    </row>
+    <row r="75" ht="27" customHeight="1" s="83">
+      <c r="A75" s="85" t="inlineStr">
         <is>
           <t>Country of Original Cambodia</t>
         </is>
       </c>
-      <c r="D72" s="85" t="n"/>
-      <c r="E72" s="85" t="n"/>
-      <c r="F72" s="31" t="n"/>
-      <c r="G72" s="31" t="n"/>
-      <c r="H72" s="31" t="n"/>
-      <c r="I72" s="80" t="n"/>
-      <c r="J72" s="18" t="n"/>
-      <c r="K72" s="18" t="n"/>
-    </row>
-    <row r="73" ht="27" customHeight="1" s="83">
-      <c r="A73" s="32" t="inlineStr">
+      <c r="D75" s="85" t="n"/>
+      <c r="E75" s="85" t="n"/>
+      <c r="F75" s="31" t="n"/>
+      <c r="G75" s="31" t="n"/>
+      <c r="H75" s="31" t="n"/>
+      <c r="I75" s="80" t="n"/>
+      <c r="J75" s="18" t="n"/>
+      <c r="K75" s="18" t="n"/>
+    </row>
+    <row r="76" ht="27" customHeight="1" s="83">
+      <c r="A76" s="32" t="inlineStr">
         <is>
           <t>Manufacture:</t>
         </is>
       </c>
-      <c r="B73" s="86" t="inlineStr">
+      <c r="B76" s="86" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="J73" s="18" t="n"/>
-      <c r="K73" s="18" t="n"/>
-      <c r="L73" s="82" t="n"/>
-    </row>
-    <row r="74" ht="27" customHeight="1" s="83">
-      <c r="A74" s="87" t="inlineStr">
+      <c r="J76" s="18" t="n"/>
+      <c r="K76" s="18" t="n"/>
+      <c r="L76" s="82" t="n"/>
+    </row>
+    <row r="77" ht="27" customHeight="1" s="83">
+      <c r="A77" s="87" t="inlineStr">
         <is>
           <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
                                           /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
-      <c r="J74" s="33" t="n"/>
-      <c r="K74" s="33" t="n"/>
-      <c r="L74" s="82" t="n"/>
-    </row>
-    <row r="75">
-      <c r="A75" s="33" t="inlineStr">
+      <c r="J77" s="33" t="n"/>
+      <c r="K77" s="33" t="n"/>
+      <c r="L77" s="82" t="n"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="33" t="inlineStr">
         <is>
           <t>A/C NO:100001100764430</t>
         </is>
       </c>
-      <c r="B75" s="33" t="n"/>
-      <c r="C75" s="33" t="n"/>
-      <c r="D75" s="33" t="n"/>
-      <c r="E75" s="33" t="n"/>
-      <c r="F75" s="33" t="n"/>
-      <c r="G75" s="33" t="n"/>
-      <c r="H75" s="33" t="n"/>
-      <c r="I75" s="33" t="n"/>
-      <c r="J75" s="33" t="n"/>
-      <c r="K75" s="33" t="n"/>
-    </row>
-    <row r="76">
-      <c r="A76" s="33" t="inlineStr">
+      <c r="B78" s="33" t="n"/>
+      <c r="C78" s="33" t="n"/>
+      <c r="D78" s="33" t="n"/>
+      <c r="E78" s="33" t="n"/>
+      <c r="F78" s="33" t="n"/>
+      <c r="G78" s="33" t="n"/>
+      <c r="H78" s="33" t="n"/>
+      <c r="I78" s="33" t="n"/>
+      <c r="J78" s="33" t="n"/>
+      <c r="K78" s="33" t="n"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="33" t="inlineStr">
         <is>
           <t>SWIFT CODE  ：BKCHKHPPXXX</t>
         </is>
       </c>
-      <c r="B76" s="33" t="n"/>
-      <c r="C76" s="33" t="n"/>
-      <c r="D76" s="33" t="n"/>
-      <c r="E76" s="33" t="n"/>
-      <c r="F76" s="5" t="inlineStr">
+      <c r="B79" s="33" t="n"/>
+      <c r="C79" s="33" t="n"/>
+      <c r="D79" s="33" t="n"/>
+      <c r="E79" s="33" t="n"/>
+      <c r="F79" s="5" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
-      <c r="G76" s="33" t="n"/>
-      <c r="H76" s="33" t="n"/>
-      <c r="I76" s="33" t="n"/>
-      <c r="J76" s="33" t="n"/>
-      <c r="K76" s="33" t="n"/>
-    </row>
-    <row r="77">
-      <c r="F77" s="18" t="n"/>
-      <c r="G77" s="18" t="n"/>
-      <c r="I77" s="3" t="n"/>
-    </row>
-    <row r="78">
-      <c r="F78" s="18" t="n"/>
-      <c r="G78" s="18" t="n"/>
-      <c r="H78" s="34" t="n"/>
-    </row>
-    <row r="79">
-      <c r="F79" s="18" t="n"/>
-      <c r="G79" s="18" t="n"/>
-      <c r="H79" s="18" t="n"/>
+      <c r="G79" s="33" t="n"/>
+      <c r="H79" s="33" t="n"/>
+      <c r="I79" s="33" t="n"/>
+      <c r="J79" s="33" t="n"/>
+      <c r="K79" s="33" t="n"/>
     </row>
     <row r="80">
       <c r="F80" s="18" t="n"/>
       <c r="G80" s="18" t="n"/>
-      <c r="H80" s="18" t="n"/>
+      <c r="I80" s="3" t="n"/>
     </row>
     <row r="81">
       <c r="F81" s="18" t="n"/>
       <c r="G81" s="18" t="n"/>
-      <c r="H81" s="19" t="n"/>
-      <c r="I81" s="19" t="n"/>
-      <c r="J81" s="19" t="n"/>
-    </row>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
+      <c r="H81" s="34" t="n"/>
+    </row>
+    <row r="82">
+      <c r="F82" s="18" t="n"/>
+      <c r="G82" s="18" t="n"/>
+      <c r="H82" s="18" t="n"/>
+    </row>
+    <row r="83">
+      <c r="F83" s="18" t="n"/>
+      <c r="G83" s="18" t="n"/>
+      <c r="H83" s="18" t="n"/>
+    </row>
+    <row r="84">
+      <c r="F84" s="18" t="n"/>
+      <c r="G84" s="18" t="n"/>
+      <c r="H84" s="19" t="n"/>
+      <c r="I84" s="19" t="n"/>
+      <c r="J84" s="19" t="n"/>
+    </row>
     <row r="85"/>
     <row r="86"/>
     <row r="87"/>
@@ -3221,23 +3244,23 @@
     <row r="200" ht="27" customHeight="1" s="83"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C39:C51"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="D39:D51"/>
+    <mergeCell ref="C56:C67"/>
     <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A74:I74"/>
-    <mergeCell ref="B54:B65"/>
-    <mergeCell ref="D54:D65"/>
+    <mergeCell ref="A77:I77"/>
     <mergeCell ref="C22:C34"/>
+    <mergeCell ref="A200:B200"/>
+    <mergeCell ref="B39:B51"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A5:I5"/>
-    <mergeCell ref="B38:B50"/>
+    <mergeCell ref="D56:D67"/>
+    <mergeCell ref="B56:B67"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B76:I76"/>
+    <mergeCell ref="A6:I6"/>
     <mergeCell ref="A4:I4"/>
-    <mergeCell ref="C54:C65"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="B73:I73"/>
-    <mergeCell ref="C38:C50"/>
-    <mergeCell ref="A200:B200"/>
-    <mergeCell ref="D38:D50"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A6:I6"/>
     <mergeCell ref="B22:B34"/>
     <mergeCell ref="D22:D34"/>
   </mergeCells>
@@ -3381,7 +3404,7 @@
           <t>Date:</t>
         </is>
       </c>
-      <c r="G9" s="107">
+      <c r="G9" s="105">
         <f>'Packing list'!I9</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
adding merge to the footer row, pre footer, and grand total footer
</commit_message>
<xml_diff>
--- a/invoice_gen/result.xlsx
+++ b/invoice_gen/result.xlsx
@@ -280,7 +280,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -370,6 +370,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
@@ -378,7 +411,7 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -650,7 +683,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="39" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -663,6 +696,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2250,8 +2287,8 @@
         </is>
       </c>
       <c r="B35" s="98" t="n"/>
-      <c r="C35" s="98" t="n"/>
-      <c r="D35" s="98" t="n"/>
+      <c r="C35" s="104" t="n"/>
+      <c r="D35" s="105" t="n"/>
       <c r="E35" s="99" t="n"/>
       <c r="F35" s="100" t="n"/>
       <c r="G35" s="100" t="inlineStr">
@@ -2262,31 +2299,31 @@
       <c r="H35" s="101" t="n"/>
     </row>
     <row r="36" ht="35" customHeight="1" s="83">
-      <c r="A36" s="104" t="n"/>
-      <c r="B36" s="104" t="inlineStr">
-        <is>
-          <t>SUB TOTAL:</t>
-        </is>
-      </c>
-      <c r="C36" s="104" t="inlineStr">
+      <c r="A36" s="106" t="n"/>
+      <c r="B36" s="106" t="inlineStr">
+        <is>
+          <t>TOTAL OF:</t>
+        </is>
+      </c>
+      <c r="C36" s="106" t="inlineStr">
         <is>
           <t>13 PALLETS</t>
         </is>
       </c>
-      <c r="D36" s="104" t="n"/>
-      <c r="E36" s="104">
+      <c r="D36" s="106" t="n"/>
+      <c r="E36" s="106">
         <f>SUM(E22:E35)</f>
         <v/>
       </c>
-      <c r="F36" s="104">
+      <c r="F36" s="106">
         <f>SUM(F22:F35)</f>
         <v/>
       </c>
-      <c r="G36" s="104">
+      <c r="G36" s="106">
         <f>SUM(G22:G35)</f>
         <v/>
       </c>
-      <c r="H36" s="104">
+      <c r="H36" s="106">
         <f>SUM(H22:H35)</f>
         <v/>
       </c>
@@ -2602,8 +2639,8 @@
         </is>
       </c>
       <c r="B52" s="98" t="n"/>
-      <c r="C52" s="98" t="n"/>
-      <c r="D52" s="98" t="n"/>
+      <c r="C52" s="104" t="n"/>
+      <c r="D52" s="105" t="n"/>
       <c r="E52" s="99" t="n"/>
       <c r="F52" s="100" t="n"/>
       <c r="G52" s="100" t="inlineStr">
@@ -2614,31 +2651,31 @@
       <c r="H52" s="101" t="n"/>
     </row>
     <row r="53" ht="35" customHeight="1" s="83">
-      <c r="A53" s="104" t="n"/>
-      <c r="B53" s="104" t="inlineStr">
-        <is>
-          <t>SUB TOTAL:</t>
-        </is>
-      </c>
-      <c r="C53" s="104" t="inlineStr">
+      <c r="A53" s="106" t="n"/>
+      <c r="B53" s="106" t="inlineStr">
+        <is>
+          <t>TOTAL OF:</t>
+        </is>
+      </c>
+      <c r="C53" s="106" t="inlineStr">
         <is>
           <t>13 PALLETS</t>
         </is>
       </c>
-      <c r="D53" s="104" t="n"/>
-      <c r="E53" s="104">
+      <c r="D53" s="106" t="n"/>
+      <c r="E53" s="106">
         <f>SUM(E39:E52)</f>
         <v/>
       </c>
-      <c r="F53" s="104">
+      <c r="F53" s="106">
         <f>SUM(F39:F52)</f>
         <v/>
       </c>
-      <c r="G53" s="104">
+      <c r="G53" s="106">
         <f>SUM(G39:G52)</f>
         <v/>
       </c>
-      <c r="H53" s="104">
+      <c r="H53" s="106">
         <f>SUM(H39:H52)</f>
         <v/>
       </c>
@@ -2936,8 +2973,8 @@
         </is>
       </c>
       <c r="B68" s="98" t="n"/>
-      <c r="C68" s="98" t="n"/>
-      <c r="D68" s="98" t="n"/>
+      <c r="C68" s="104" t="n"/>
+      <c r="D68" s="105" t="n"/>
       <c r="E68" s="99" t="n"/>
       <c r="F68" s="100" t="n"/>
       <c r="G68" s="100" t="inlineStr">
@@ -2948,61 +2985,61 @@
       <c r="H68" s="101" t="n"/>
     </row>
     <row r="69" ht="35" customHeight="1" s="83">
-      <c r="A69" s="104" t="n"/>
-      <c r="B69" s="104" t="inlineStr">
-        <is>
-          <t>SUB TOTAL:</t>
-        </is>
-      </c>
-      <c r="C69" s="104" t="inlineStr">
+      <c r="A69" s="106" t="n"/>
+      <c r="B69" s="106" t="inlineStr">
+        <is>
+          <t>TOTAL OF:</t>
+        </is>
+      </c>
+      <c r="C69" s="106" t="inlineStr">
         <is>
           <t>12 PALLETS</t>
         </is>
       </c>
-      <c r="D69" s="104" t="n"/>
-      <c r="E69" s="104">
+      <c r="D69" s="106" t="n"/>
+      <c r="E69" s="106">
         <f>SUM(E56:E68)</f>
         <v/>
       </c>
-      <c r="F69" s="104">
+      <c r="F69" s="106">
         <f>SUM(F56:F68)</f>
         <v/>
       </c>
-      <c r="G69" s="104">
+      <c r="G69" s="106">
         <f>SUM(G56:G68)</f>
         <v/>
       </c>
-      <c r="H69" s="104">
+      <c r="H69" s="106">
         <f>SUM(H56:H68)</f>
         <v/>
       </c>
     </row>
     <row r="70" ht="35" customHeight="1" s="83">
-      <c r="A70" s="104" t="n"/>
-      <c r="B70" s="104" t="inlineStr">
-        <is>
-          <t>GRAND TOTAL:</t>
-        </is>
-      </c>
-      <c r="C70" s="104" t="inlineStr">
+      <c r="A70" s="106" t="n"/>
+      <c r="B70" s="106" t="inlineStr">
+        <is>
+          <t>TOTAL OF:</t>
+        </is>
+      </c>
+      <c r="C70" s="106" t="inlineStr">
         <is>
           <t>38 PALLETS</t>
         </is>
       </c>
-      <c r="D70" s="104" t="n"/>
-      <c r="E70" s="104">
+      <c r="D70" s="106" t="n"/>
+      <c r="E70" s="106">
         <f>SUM(E22:E34,E39:E51,E56:E67)</f>
         <v/>
       </c>
-      <c r="F70" s="104">
+      <c r="F70" s="106">
         <f>SUM(F22:F34,F39:F51,F56:F67)</f>
         <v/>
       </c>
-      <c r="G70" s="104">
+      <c r="G70" s="106">
         <f>SUM(G22:G34,G39:G51,G56:G67)</f>
         <v/>
       </c>
-      <c r="H70" s="104">
+      <c r="H70" s="106">
         <f>SUM(H22:H34,H39:H51,H56:H67)</f>
         <v/>
       </c>
@@ -3243,7 +3280,7 @@
     <row r="199"/>
     <row r="200" ht="27" customHeight="1" s="83"/>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="22">
     <mergeCell ref="C39:C51"/>
     <mergeCell ref="A75:C75"/>
     <mergeCell ref="D39:D51"/>
@@ -3252,7 +3289,9 @@
     <mergeCell ref="A77:I77"/>
     <mergeCell ref="C22:C34"/>
     <mergeCell ref="A200:B200"/>
+    <mergeCell ref="B52:C52"/>
     <mergeCell ref="B39:B51"/>
+    <mergeCell ref="B68:C68"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A5:I5"/>
     <mergeCell ref="D56:D67"/>
@@ -3261,6 +3300,7 @@
     <mergeCell ref="B76:I76"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="A4:I4"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B22:B34"/>
     <mergeCell ref="D22:D34"/>
   </mergeCells>
@@ -3404,7 +3444,7 @@
           <t>Date:</t>
         </is>
       </c>
-      <c r="G9" s="105">
+      <c r="G9" s="107">
         <f>'Packing list'!I9</f>
         <v/>
       </c>

</xml_diff>